<commit_message>
Actualización automática: 2025-05-20 13:27
</commit_message>
<xml_diff>
--- a/seguridad/Informe_Diario_Unidades.xlsx
+++ b/seguridad/Informe_Diario_Unidades.xlsx
@@ -1225,8 +1225,8 @@
   <dimension ref="A1:AF39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1373,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-05-20 13:30
</commit_message>
<xml_diff>
--- a/seguridad/Informe_Diario_Unidades.xlsx
+++ b/seguridad/Informe_Diario_Unidades.xlsx
@@ -1226,7 +1226,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D3" sqref="D3"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1373,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-05-20 13:45
</commit_message>
<xml_diff>
--- a/seguridad/Informe_Diario_Unidades.xlsx
+++ b/seguridad/Informe_Diario_Unidades.xlsx
@@ -1226,7 +1226,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <selection pane="topRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1373,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Actualización automática: 2025-06-06 10:11
</commit_message>
<xml_diff>
--- a/seguridad/Informe_Diario_Unidades.xlsx
+++ b/seguridad/Informe_Diario_Unidades.xlsx
@@ -758,17 +758,17 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Luis Ibarra</t>
+          <t>Adrian Caro</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>120</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
+          <t>FORD RANGER 2011</t>
         </is>
       </c>
       <c r="D2" s="7" t="n">
@@ -776,14 +776,14 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>04:50:18</t>
+          <t>04:37:32</t>
         </is>
       </c>
       <c r="F2" s="1" t="n">
-        <v>100</v>
+        <v>82.59999999999999</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>14.31</v>
+        <v>11.37</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
@@ -795,7 +795,7 @@
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:00:09</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -821,11 +821,11 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>72.01000000000001</v>
+        <v>69.01000000000001</v>
       </c>
       <c r="R2" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 12:53PM CST</t>
+          <t>Jun 5 5:07PM CST</t>
         </is>
       </c>
       <c r="S2" s="1" t="n">
@@ -878,17 +878,17 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Miguel Zamora</t>
+          <t>Moises Martinez</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>149</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>TOYOTA HILUX 2024</t>
         </is>
       </c>
       <c r="D3" s="7" t="n">
@@ -896,28 +896,28 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>03:38:59</t>
+          <t>03:10:33</t>
         </is>
       </c>
       <c r="F3" s="1" t="n">
-        <v>80.3</v>
+        <v>65.7</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>0</v>
+        <v>10.83</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
+          <t>00:00:29</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
           <t>00:00:26</t>
         </is>
       </c>
-      <c r="J3" s="1" t="inlineStr">
-        <is>
-          <t>00:00:15</t>
-        </is>
-      </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
           <t>00:00:00</t>
@@ -941,11 +941,11 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1" t="n">
-        <v>74.44</v>
+        <v>76.01000000000001</v>
       </c>
       <c r="R3" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 2:29PM CST</t>
+          <t>Jun 5 1:01PM CST</t>
         </is>
       </c>
       <c r="S3" s="1" t="n">
@@ -998,17 +998,17 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Adrian Caro</t>
+          <t>Miguel Guizar</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>150</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>FORD RANGER 2011</t>
+          <t>Hino 300 2024</t>
         </is>
       </c>
       <c r="D4" s="7" t="n">
@@ -1016,14 +1016,14 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>03:24:18</t>
+          <t>03:53:45</t>
         </is>
       </c>
       <c r="F4" s="1" t="n">
-        <v>61.3</v>
+        <v>59.6</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>8.289999999999999</v>
+        <v>5.59</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
@@ -1061,11 +1061,11 @@
         <v>0</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>65.01000000000001</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="R4" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 3:36PM CST</t>
+          <t>Jun 5 9:14AM CST</t>
         </is>
       </c>
       <c r="S4" s="1" t="n">
@@ -1118,17 +1118,17 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Miguel Guizar</t>
+          <t>Gerardo Aguillón</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>142</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>Hino 300 2024</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D5" s="7" t="n">
@@ -1136,26 +1136,26 @@
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>03:37:11</t>
+          <t>03:34:59</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>57.5</v>
+        <v>44.1</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>5.43</v>
+        <v>6.96</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr">
@@ -1181,11 +1181,11 @@
         <v>0</v>
       </c>
       <c r="Q5" s="1" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="R5" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 4:35PM CST</t>
+          <t>Jun 5 2:11PM CST</t>
         </is>
       </c>
       <c r="S5" s="1" t="n">
@@ -1238,17 +1238,17 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Hugo López</t>
+          <t>Alejandro Lara</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>110</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX</t>
+          <t>WORKEN</t>
         </is>
       </c>
       <c r="D6" s="7" t="n">
@@ -1256,14 +1256,14 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>02:44:06</t>
+          <t>02:06:32</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>39.5</v>
+        <v>43</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>7.13</v>
+        <v>13</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>0</v>
@@ -1301,11 +1301,11 @@
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="n">
-        <v>58</v>
+        <v>65.01000000000001</v>
       </c>
       <c r="R6" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 1:15PM CST</t>
+          <t>Jun 5 10:08AM CST</t>
         </is>
       </c>
       <c r="S6" s="1" t="n">
@@ -1358,17 +1358,17 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Gerardo Aguillón</t>
+          <t>Hugo López</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>153</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX</t>
         </is>
       </c>
       <c r="D7" s="7" t="n">
@@ -1376,26 +1376,26 @@
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>02:51:12</t>
+          <t>02:48:13</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>35.4</v>
+        <v>41.4</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>5.91</v>
+        <v>6.94</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:21</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr">
@@ -1421,11 +1421,11 @@
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="R7" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 2:25PM CST</t>
+          <t>Jun 5 11:56AM CST</t>
         </is>
       </c>
       <c r="S7" s="1" t="n">
@@ -1496,21 +1496,21 @@
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>02:42:19</t>
+          <t>02:40:23</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>35.1</v>
+        <v>34.1</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>6.14</v>
+        <v>6.27</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="J8" s="1" t="inlineStr">
@@ -1541,11 +1541,11 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="R8" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 9:25AM CST</t>
+          <t>Jun 5 9:58AM CST</t>
         </is>
       </c>
       <c r="S8" s="1" t="n">
@@ -1616,21 +1616,21 @@
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>01:50:11</t>
+          <t>01:30:01</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>28.4</v>
+        <v>21.2</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>2.8</v>
+        <v>2.16</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J9" s="1" t="inlineStr">
@@ -1661,11 +1661,11 @@
         <v>0</v>
       </c>
       <c r="Q9" s="1" t="n">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="R9" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 5:22PM CST</t>
+          <t>Jun 5 7:24AM CST</t>
         </is>
       </c>
       <c r="S9" s="1" t="n">
@@ -1736,21 +1736,21 @@
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>02:01:17</t>
+          <t>01:50:31</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>22.8</v>
+        <v>20.5</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>10.8</v>
+        <v>8.98</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J10" s="1" t="inlineStr">
@@ -1781,11 +1781,11 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="R10" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 2:19PM CST</t>
+          <t>Jun 5 2:44PM CST</t>
         </is>
       </c>
       <c r="S10" s="1" t="n">
@@ -1838,17 +1838,17 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Marcos Barbosa</t>
+          <t>Álvaro Zapata</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>124</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2023</t>
+          <t>KENWORTH</t>
         </is>
       </c>
       <c r="D11" s="7" t="n">
@@ -1856,26 +1856,26 @@
       </c>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>02:10:58</t>
+          <t>00:19:24</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>21.9</v>
+        <v>4.1</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>3.84</v>
+        <v>2.24</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J11" s="1" t="inlineStr">
         <is>
-          <t>00:00:04</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K11" s="1" t="inlineStr">
@@ -1901,11 +1901,11 @@
         <v>0</v>
       </c>
       <c r="Q11" s="1" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="R11" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 3:00PM CST</t>
+          <t>Jun 5 4:27PM CST</t>
         </is>
       </c>
       <c r="S11" s="1" t="n">
@@ -1958,17 +1958,17 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Luis Galindo</t>
+          <t>Martin Quezada</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>122</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH 2009</t>
+          <t>INTERNACIONAL</t>
         </is>
       </c>
       <c r="D12" s="7" t="n">
@@ -1976,14 +1976,14 @@
       </c>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>00:17:34</t>
+          <t>00:02:33</t>
         </is>
       </c>
       <c r="F12" s="1" t="n">
-        <v>4</v>
+        <v>0.7</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>2.81</v>
+        <v>2.83</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>0</v>
@@ -2021,11 +2021,11 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="R12" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 2:42PM CST</t>
+          <t>Jun 5 11:48AM CST</t>
         </is>
       </c>
       <c r="S12" s="1" t="n">
@@ -2096,14 +2096,14 @@
       </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>00:00:56</t>
+          <t>00:03:10</t>
         </is>
       </c>
       <c r="F13" s="1" t="n">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.29</v>
+        <v>0.74</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>0</v>
@@ -2141,11 +2141,11 @@
         <v>0</v>
       </c>
       <c r="Q13" s="1" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="R13" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 7:15PM CST</t>
+          <t>Jun 5 7:35AM CST</t>
         </is>
       </c>
       <c r="S13" s="1" t="n">
@@ -2198,44 +2198,44 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Emmanuel Salcedo</t>
+          <t>Alexis Alvarado</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>145</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>HINO 500</t>
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>03:40:34</t>
+          <t>00:01:16</t>
         </is>
       </c>
       <c r="F14" s="1" t="n">
-        <v>58.5</v>
+        <v>0.1</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>9.77</v>
+        <v>0.46</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="inlineStr">
         <is>
-          <t>00:00:54</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J14" s="1" t="inlineStr">
         <is>
-          <t>00:00:55</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K14" s="1" t="inlineStr">
@@ -2261,11 +2261,11 @@
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>67.01000000000001</v>
+        <v>23</v>
       </c>
       <c r="R14" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 1:49PM CST</t>
+          <t>Jun 5 7:41PM CST</t>
         </is>
       </c>
       <c r="S14" s="1" t="n">
@@ -2318,17 +2318,17 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Eduardo Hernandez</t>
+          <t>Mario Ballinas</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>144</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D15" s="7" t="n">
@@ -2336,26 +2336,26 @@
       </c>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>02:51:57</t>
+          <t>04:00:54</t>
         </is>
       </c>
       <c r="F15" s="1" t="n">
-        <v>51.4</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>8.130000000000001</v>
+        <v>12.58</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="inlineStr">
         <is>
-          <t>00:00:42</t>
+          <t>00:01:06</t>
         </is>
       </c>
       <c r="J15" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:27</t>
         </is>
       </c>
       <c r="K15" s="1" t="inlineStr">
@@ -2381,11 +2381,11 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>76.01000000000001</v>
+        <v>89.01000000000001</v>
       </c>
       <c r="R15" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 1:22PM CST</t>
+          <t>Jun 5 3:16PM CST</t>
         </is>
       </c>
       <c r="S15" s="1" t="n">
@@ -2438,44 +2438,44 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Angel Cortez</t>
+          <t>José Morales</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>141</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2018</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D16" s="7" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>02:55:38</t>
+          <t>03:13:47</t>
         </is>
       </c>
       <c r="F16" s="1" t="n">
-        <v>74.09999999999999</v>
+        <v>56.4</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>10.23</v>
+        <v>8.66</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="inlineStr">
         <is>
-          <t>00:02:05</t>
+          <t>00:00:32</t>
         </is>
       </c>
       <c r="J16" s="1" t="inlineStr">
         <is>
-          <t>00:02:10</t>
+          <t>00:00:59</t>
         </is>
       </c>
       <c r="K16" s="1" t="inlineStr">
@@ -2501,11 +2501,11 @@
         <v>0</v>
       </c>
       <c r="Q16" s="1" t="n">
-        <v>80.01000000000001</v>
+        <v>67.01000000000001</v>
       </c>
       <c r="R16" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 1:40PM CST</t>
+          <t>Jun 5 1:41PM CST</t>
         </is>
       </c>
       <c r="S16" s="1" t="n">
@@ -2558,17 +2558,17 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>David Serrano</t>
+          <t>Fernando Ornelas</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>138</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>TOYOTA HILUX 2020</t>
         </is>
       </c>
       <c r="D17" s="7" t="n">
@@ -2576,26 +2576,26 @@
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>02:24:37</t>
+          <t>02:39:41</t>
         </is>
       </c>
       <c r="F17" s="1" t="n">
-        <v>38.8</v>
+        <v>46.9</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>3.91</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>00:00:30</t>
+          <t>00:00:53</t>
         </is>
       </c>
       <c r="J17" s="1" t="inlineStr">
         <is>
-          <t>00:00:47</t>
+          <t>00:00:40</t>
         </is>
       </c>
       <c r="K17" s="1" t="inlineStr">
@@ -2621,11 +2621,11 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="n">
-        <v>68.01000000000001</v>
+        <v>75.01000000000001</v>
       </c>
       <c r="R17" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 9:00AM CST</t>
+          <t>Jun 5 2:57PM CST</t>
         </is>
       </c>
       <c r="S17" s="1" t="n">
@@ -2678,17 +2678,17 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Fernando Ornelas</t>
+          <t>Daniel Iñiguez</t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>131</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2020</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D18" s="7" t="n">
@@ -2696,31 +2696,31 @@
       </c>
       <c r="E18" s="1" t="inlineStr">
         <is>
-          <t>02:05:52</t>
+          <t>01:45:19</t>
         </is>
       </c>
       <c r="F18" s="1" t="n">
-        <v>31.2</v>
+        <v>37.3</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>5.53</v>
+        <v>5.36</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="inlineStr">
         <is>
-          <t>00:00:32</t>
+          <t>00:01:17</t>
         </is>
       </c>
       <c r="J18" s="1" t="inlineStr">
         <is>
-          <t>00:00:32</t>
+          <t>00:00:42</t>
         </is>
       </c>
       <c r="K18" s="1" t="inlineStr">
         <is>
-          <t>00:00:06</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L18" s="1" t="inlineStr">
@@ -2741,11 +2741,11 @@
         <v>0</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>67.01000000000001</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="R18" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 1:28PM CST</t>
+          <t>Jun 5 3:57PM CST</t>
         </is>
       </c>
       <c r="S18" s="1" t="n">
@@ -2798,17 +2798,17 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Kevin De La O</t>
+          <t>Miguel Zamora</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="D19" s="7" t="n">
@@ -2816,11 +2816,11 @@
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>05:32:28</t>
+          <t>05:25:42</t>
         </is>
       </c>
       <c r="F19" s="1" t="n">
-        <v>122</v>
+        <v>165.8</v>
       </c>
       <c r="G19" s="1" t="n">
         <v>0</v>
@@ -2830,17 +2830,17 @@
       </c>
       <c r="I19" s="1" t="inlineStr">
         <is>
-          <t>00:02:09</t>
+          <t>00:03:23</t>
         </is>
       </c>
       <c r="J19" s="1" t="inlineStr">
         <is>
-          <t>00:01:17</t>
+          <t>00:04:09</t>
         </is>
       </c>
       <c r="K19" s="1" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="L19" s="1" t="inlineStr">
@@ -2852,7 +2852,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="1" t="n">
         <v>0</v>
@@ -2861,11 +2861,11 @@
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>87.73</v>
+        <v>95.51000000000001</v>
       </c>
       <c r="R19" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 1:47PM CST</t>
+          <t>Jun 5 7:20PM CST</t>
         </is>
       </c>
       <c r="S19" s="1" t="n">
@@ -2918,17 +2918,17 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Eduardo Lopez</t>
+          <t>Diego Cardenas</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>134</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2020</t>
+          <t>TOYOTA HILUX 2018</t>
         </is>
       </c>
       <c r="D20" s="7" t="n">
@@ -2936,31 +2936,31 @@
       </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>03:18:53</t>
+          <t>05:30:04</t>
         </is>
       </c>
       <c r="F20" s="1" t="n">
-        <v>77.7</v>
+        <v>120.9</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>10.67</v>
+        <v>16.29</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="inlineStr">
         <is>
-          <t>00:02:44</t>
+          <t>00:03:17</t>
         </is>
       </c>
       <c r="J20" s="1" t="inlineStr">
         <is>
-          <t>00:02:07</t>
+          <t>00:01:43</t>
         </is>
       </c>
       <c r="K20" s="1" t="inlineStr">
         <is>
-          <t>00:00:06</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="L20" s="1" t="inlineStr">
@@ -2981,11 +2981,11 @@
         <v>0</v>
       </c>
       <c r="Q20" s="1" t="n">
-        <v>79.01000000000001</v>
+        <v>83.01000000000001</v>
       </c>
       <c r="R20" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 2:44PM CST</t>
+          <t>Jun 5 1:35PM CST</t>
         </is>
       </c>
       <c r="S20" s="1" t="n">
@@ -3038,17 +3038,17 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Mario Ballinas</t>
+          <t>Daniel Mercado</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>130</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D21" s="7" t="n">
@@ -3056,26 +3056,26 @@
       </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>03:06:49</t>
+          <t>04:50:29</t>
         </is>
       </c>
       <c r="F21" s="1" t="n">
-        <v>59.7</v>
+        <v>116.6</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>9.710000000000001</v>
+        <v>16.86</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="inlineStr">
         <is>
-          <t>00:01:19</t>
+          <t>00:02:30</t>
         </is>
       </c>
       <c r="J21" s="1" t="inlineStr">
         <is>
-          <t>00:01:13</t>
+          <t>00:01:33</t>
         </is>
       </c>
       <c r="K21" s="1" t="inlineStr">
@@ -3101,11 +3101,11 @@
         <v>0</v>
       </c>
       <c r="Q21" s="1" t="n">
-        <v>92.01000000000001</v>
+        <v>87.01000000000001</v>
       </c>
       <c r="R21" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 1:12PM CST</t>
+          <t>Jun 5 10:09AM CST</t>
         </is>
       </c>
       <c r="S21" s="1" t="n">
@@ -3158,12 +3158,12 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Daniel Iñiguez</t>
+          <t>Emmanuel Salcedo</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>132</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
@@ -3176,31 +3176,31 @@
       </c>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>00:37:42</t>
+          <t>03:36:43</t>
         </is>
       </c>
       <c r="F22" s="1" t="n">
-        <v>10.9</v>
+        <v>67.09999999999999</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>2.83</v>
+        <v>9.84</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="inlineStr">
         <is>
-          <t>00:00:23</t>
+          <t>00:01:55</t>
         </is>
       </c>
       <c r="J22" s="1" t="inlineStr">
         <is>
-          <t>00:00:33</t>
+          <t>00:01:47</t>
         </is>
       </c>
       <c r="K22" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="L22" s="1" t="inlineStr">
@@ -3221,11 +3221,11 @@
         <v>0</v>
       </c>
       <c r="Q22" s="1" t="n">
-        <v>63</v>
+        <v>69.01000000000001</v>
       </c>
       <c r="R22" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 2:45PM CST</t>
+          <t>Jun 5 3:14PM CST</t>
         </is>
       </c>
       <c r="S22" s="1" t="n">
@@ -3278,49 +3278,49 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Diego Cardenas</t>
+          <t>Eduardo Lopez</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>136</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2018</t>
+          <t>TOYOTA HILUX 2020</t>
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>04:54:06</t>
+          <t>02:16:53</t>
         </is>
       </c>
       <c r="F23" s="1" t="n">
-        <v>111.6</v>
+        <v>46.9</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>15.02</v>
+        <v>7.4</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I23" s="1" t="inlineStr">
         <is>
-          <t>00:03:04</t>
+          <t>00:00:41</t>
         </is>
       </c>
       <c r="J23" s="1" t="inlineStr">
         <is>
-          <t>00:02:37</t>
+          <t>00:01:07</t>
         </is>
       </c>
       <c r="K23" s="1" t="inlineStr">
         <is>
-          <t>00:00:44</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="L23" s="1" t="inlineStr">
@@ -3341,11 +3341,11 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>81.01000000000001</v>
+        <v>64</v>
       </c>
       <c r="R23" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 12:22PM CST</t>
+          <t>Jun 5 4:05PM CST</t>
         </is>
       </c>
       <c r="S23" s="1" t="n">
@@ -3398,17 +3398,17 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Jorge Tornero</t>
+          <t>Marcos Barbosa</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>147</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>HINO 300</t>
+          <t>TOYOTA HILUX 2023</t>
         </is>
       </c>
       <c r="D24" s="7" t="n">
@@ -3416,43 +3416,43 @@
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>02:57:34</t>
+          <t>04:34:36</t>
         </is>
       </c>
       <c r="F24" s="1" t="n">
-        <v>72.5</v>
+        <v>149.4</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>6.72</v>
+        <v>16.46</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I24" s="1" t="inlineStr">
         <is>
-          <t>00:00:33</t>
+          <t>00:05:21</t>
         </is>
       </c>
       <c r="J24" s="1" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:03:59</t>
         </is>
       </c>
       <c r="K24" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:00:45</t>
         </is>
       </c>
       <c r="L24" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N24" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" s="1" t="n">
         <v>0</v>
@@ -3461,11 +3461,11 @@
         <v>0</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>84.01000000000001</v>
+        <v>92.01000000000001</v>
       </c>
       <c r="R24" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 10:04AM CST</t>
+          <t>Jun 5 3:14PM CST</t>
         </is>
       </c>
       <c r="S24" s="1" t="n">
@@ -3518,17 +3518,17 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>José Morales</t>
+          <t>Kevin De La O</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>116</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>VAN HYUNDAI</t>
         </is>
       </c>
       <c r="D25" s="7" t="n">
@@ -3536,36 +3536,36 @@
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>02:46:40</t>
+          <t>05:00:01</t>
         </is>
       </c>
       <c r="F25" s="1" t="n">
-        <v>54.5</v>
+        <v>132.7</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>8.220000000000001</v>
+        <v>0</v>
       </c>
       <c r="H25" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I25" s="1" t="inlineStr">
         <is>
-          <t>00:00:54</t>
+          <t>00:03:12</t>
         </is>
       </c>
       <c r="J25" s="1" t="inlineStr">
         <is>
-          <t>00:01:17</t>
+          <t>00:01:19</t>
         </is>
       </c>
       <c r="K25" s="1" t="inlineStr">
         <is>
-          <t>00:00:44</t>
+          <t>00:00:43</t>
         </is>
       </c>
       <c r="L25" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:06</t>
         </is>
       </c>
       <c r="M25" s="1" t="n">
@@ -3581,11 +3581,11 @@
         <v>0</v>
       </c>
       <c r="Q25" s="1" t="n">
-        <v>68.01000000000001</v>
+        <v>94.31999999999999</v>
       </c>
       <c r="R25" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 2:19PM CST</t>
+          <t>Jun 5 12:44PM CST</t>
         </is>
       </c>
       <c r="S25" s="1" t="n">
@@ -3638,61 +3638,61 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>Luis Galindo</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>118</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>KENWORTH 2009</t>
         </is>
       </c>
       <c r="D26" s="8" t="n">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E26" s="1" t="inlineStr">
         <is>
-          <t>02:25:21</t>
+          <t>06:47:38</t>
         </is>
       </c>
       <c r="F26" s="1" t="n">
-        <v>41.2</v>
+        <v>363.7</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>4.5</v>
+        <v>88.81</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="1" t="inlineStr">
         <is>
-          <t>00:01:12</t>
+          <t>00:04:48</t>
         </is>
       </c>
       <c r="J26" s="1" t="inlineStr">
         <is>
-          <t>00:01:36</t>
+          <t>00:13:43</t>
         </is>
       </c>
       <c r="K26" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:02:44</t>
         </is>
       </c>
       <c r="L26" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="M26" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O26" s="1" t="n">
         <v>0</v>
@@ -3701,11 +3701,11 @@
         <v>0</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <v>80.01000000000001</v>
+        <v>95.01000000000001</v>
       </c>
       <c r="R26" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 12:19PM CST</t>
+          <t>Jun 5 10:07AM CST</t>
         </is>
       </c>
       <c r="S26" s="1" t="n">
@@ -3758,54 +3758,54 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Alberto Sanchez</t>
+          <t>Angel Cortez</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>133</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>VW DELIVERY 10.6</t>
+          <t>TOYOTA HILUX 2018</t>
         </is>
       </c>
       <c r="D27" s="8" t="n">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
-          <t>09:12:44</t>
+          <t>03:54:10</t>
         </is>
       </c>
       <c r="F27" s="1" t="n">
-        <v>427.7</v>
+        <v>120.5</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>0</v>
+        <v>16.39</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I27" s="1" t="inlineStr">
         <is>
-          <t>00:12:39</t>
+          <t>00:03:39</t>
         </is>
       </c>
       <c r="J27" s="1" t="inlineStr">
         <is>
-          <t>00:08:01</t>
+          <t>00:02:55</t>
         </is>
       </c>
       <c r="K27" s="1" t="inlineStr">
         <is>
-          <t>00:01:43</t>
+          <t>00:00:50</t>
         </is>
       </c>
       <c r="L27" s="1" t="inlineStr">
         <is>
-          <t>00:00:15</t>
+          <t>00:00:22</t>
         </is>
       </c>
       <c r="M27" s="1" t="n">
@@ -3821,11 +3821,11 @@
         <v>0</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <v>99.61</v>
+        <v>82.01000000000001</v>
       </c>
       <c r="R27" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 6:17AM CST</t>
+          <t>Jun 5 1:45PM CST</t>
         </is>
       </c>
       <c r="S27" s="1" t="n">
@@ -3878,54 +3878,54 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Daniel Mercado</t>
+          <t>Eduardo Hernandez</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>152</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
-        </is>
-      </c>
-      <c r="D28" s="8" t="n">
-        <v>82</v>
+          <t>TOYOTA HILUX</t>
+        </is>
+      </c>
+      <c r="D28" s="9" t="n">
+        <v>63</v>
       </c>
       <c r="E28" s="1" t="inlineStr">
         <is>
-          <t>03:11:12</t>
+          <t>03:46:27</t>
         </is>
       </c>
       <c r="F28" s="1" t="n">
-        <v>61.4</v>
+        <v>101.4</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>8.890000000000001</v>
+        <v>14.14</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I28" s="1" t="inlineStr">
         <is>
-          <t>00:01:02</t>
+          <t>00:04:03</t>
         </is>
       </c>
       <c r="J28" s="1" t="inlineStr">
         <is>
-          <t>00:01:26</t>
+          <t>00:07:11</t>
         </is>
       </c>
       <c r="K28" s="1" t="inlineStr">
         <is>
-          <t>00:00:09</t>
+          <t>00:01:56</t>
         </is>
       </c>
       <c r="L28" s="1" t="inlineStr">
         <is>
-          <t>00:00:17</t>
+          <t>00:00:23</t>
         </is>
       </c>
       <c r="M28" s="1" t="n">
@@ -3941,11 +3941,11 @@
         <v>0</v>
       </c>
       <c r="Q28" s="1" t="n">
-        <v>74.01000000000001</v>
+        <v>113.01</v>
       </c>
       <c r="R28" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 1:02PM CST</t>
+          <t>Jun 5 3:01PM CST</t>
         </is>
       </c>
       <c r="S28" s="1" t="n">
@@ -3998,54 +3998,54 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Alejandro Lara</t>
+          <t>Alberto Sanchez</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>154</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>WORKEN</t>
-        </is>
-      </c>
-      <c r="D29" s="8" t="n">
-        <v>81</v>
+          <t>VW DELIVERY 10.6</t>
+        </is>
+      </c>
+      <c r="D29" s="9" t="n">
+        <v>58</v>
       </c>
       <c r="E29" s="1" t="inlineStr">
         <is>
-          <t>05:27:42</t>
+          <t>04:46:26</t>
         </is>
       </c>
       <c r="F29" s="1" t="n">
-        <v>350</v>
+        <v>296.5</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>85.5</v>
+        <v>0</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I29" s="1" t="inlineStr">
         <is>
-          <t>00:01:14</t>
+          <t>00:03:58</t>
         </is>
       </c>
       <c r="J29" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:04:45</t>
         </is>
       </c>
       <c r="K29" s="1" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:01:47</t>
         </is>
       </c>
       <c r="L29" s="1" t="inlineStr">
         <is>
-          <t>00:00:32</t>
+          <t>00:00:47</t>
         </is>
       </c>
       <c r="M29" s="1" t="n">
@@ -4061,11 +4061,11 @@
         <v>0</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>69.01000000000001</v>
+        <v>100.5</v>
       </c>
       <c r="R29" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 1:26PM CST</t>
+          <t>Jun 5 12:25PM CST</t>
         </is>
       </c>
       <c r="S29" s="1" t="n">
@@ -4118,61 +4118,61 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Moises Martinez</t>
+          <t>Armando Muñoz</t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>102</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
-        </is>
-      </c>
-      <c r="D30" s="8" t="n">
-        <v>79</v>
+          <t>HINO 300</t>
+        </is>
+      </c>
+      <c r="D30" s="9" t="n">
+        <v>55</v>
       </c>
       <c r="E30" s="1" t="inlineStr">
         <is>
-          <t>03:23:03</t>
+          <t>05:25:12</t>
         </is>
       </c>
       <c r="F30" s="1" t="n">
-        <v>71.40000000000001</v>
+        <v>253.8</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>12.84</v>
+        <v>29.62</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I30" s="1" t="inlineStr">
         <is>
-          <t>00:01:02</t>
+          <t>00:06:44</t>
         </is>
       </c>
       <c r="J30" s="1" t="inlineStr">
         <is>
-          <t>00:00:49</t>
+          <t>00:06:26</t>
         </is>
       </c>
       <c r="K30" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:01:51</t>
         </is>
       </c>
       <c r="L30" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:59</t>
         </is>
       </c>
       <c r="M30" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" s="1" t="n">
         <v>0</v>
@@ -4185,7 +4185,7 @@
       </c>
       <c r="R30" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 12:52PM CST</t>
+          <t>Jun 5 8:57AM CST</t>
         </is>
       </c>
       <c r="S30" s="1" t="n">
@@ -4238,12 +4238,12 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Armando Muñoz</t>
+          <t>Jorge Tornero</t>
         </is>
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>117</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
@@ -4252,73 +4252,73 @@
         </is>
       </c>
       <c r="D31" s="9" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E31" s="1" t="inlineStr">
         <is>
-          <t>12:13:32</t>
+          <t>04:08:00</t>
         </is>
       </c>
       <c r="F31" s="1" t="n">
-        <v>574.2</v>
+        <v>85.3</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>75.45999999999999</v>
+        <v>9.65</v>
       </c>
       <c r="H31" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="1" t="inlineStr">
         <is>
-          <t>00:13:40</t>
+          <t>00:01:24</t>
         </is>
       </c>
       <c r="J31" s="1" t="inlineStr">
         <is>
-          <t>00:13:19</t>
+          <t>00:00:28</t>
         </is>
       </c>
       <c r="K31" s="1" t="inlineStr">
         <is>
-          <t>00:07:49</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L31" s="1" t="inlineStr">
         <is>
-          <t>00:02:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M31" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1" t="n">
+        <v>74.01000000000001</v>
+      </c>
+      <c r="R31" s="1" t="inlineStr">
+        <is>
+          <t>Jun 5 9:45AM CST</t>
+        </is>
+      </c>
+      <c r="S31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="O31" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="1" t="n">
-        <v>90.01000000000001</v>
-      </c>
-      <c r="R31" s="1" t="inlineStr">
-        <is>
-          <t>Jun 4 5:08PM CST</t>
-        </is>
-      </c>
-      <c r="S31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V31" s="1" t="n">
-        <v>0</v>
       </c>
       <c r="W31" s="1" t="n">
         <v>0</v>
@@ -4372,15 +4372,15 @@
         </is>
       </c>
       <c r="D32" s="9" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E32" s="1" t="inlineStr">
         <is>
-          <t>10:37:43</t>
+          <t>07:54:21</t>
         </is>
       </c>
       <c r="F32" s="1" t="n">
-        <v>571.4</v>
+        <v>367.3</v>
       </c>
       <c r="G32" s="1" t="n">
         <v>0</v>
@@ -4390,42 +4390,42 @@
       </c>
       <c r="I32" s="1" t="inlineStr">
         <is>
+          <t>00:05:14</t>
+        </is>
+      </c>
+      <c r="J32" s="1" t="inlineStr">
+        <is>
           <t>00:11:05</t>
         </is>
       </c>
-      <c r="J32" s="1" t="inlineStr">
-        <is>
-          <t>00:13:18</t>
-        </is>
-      </c>
       <c r="K32" s="1" t="inlineStr">
         <is>
-          <t>00:05:40</t>
+          <t>00:04:34</t>
         </is>
       </c>
       <c r="L32" s="1" t="inlineStr">
         <is>
-          <t>00:02:56</t>
+          <t>00:02:01</t>
         </is>
       </c>
       <c r="M32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N32" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O32" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q32" s="1" t="n">
-        <v>99.34</v>
+        <v>98.73999999999999</v>
       </c>
       <c r="R32" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 2:02PM CST</t>
+          <t>Jun 5 6:47AM CST</t>
         </is>
       </c>
       <c r="S32" s="1" t="n">
@@ -4478,58 +4478,58 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Alexis Alvarado</t>
+          <t>Luis Ibarra</t>
         </is>
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>148</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr">
         <is>
-          <t>HINO 500</t>
+          <t>TOYOTA HILUX 2024</t>
         </is>
       </c>
       <c r="D33" s="9" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E33" s="1" t="inlineStr">
         <is>
-          <t>06:10:55</t>
+          <t>03:52:33</t>
         </is>
       </c>
       <c r="F33" s="1" t="n">
-        <v>346</v>
+        <v>73.8</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>83.7</v>
+        <v>10.32</v>
       </c>
       <c r="H33" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="1" t="inlineStr">
         <is>
-          <t>00:10:54</t>
+          <t>00:00:21</t>
         </is>
       </c>
       <c r="J33" s="1" t="inlineStr">
         <is>
-          <t>00:05:17</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="K33" s="1" t="inlineStr">
         <is>
-          <t>00:04:32</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L33" s="1" t="inlineStr">
         <is>
-          <t>00:01:29</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M33" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N33" s="1" t="n">
         <v>0</v>
@@ -4541,11 +4541,11 @@
         <v>0</v>
       </c>
       <c r="Q33" s="1" t="n">
-        <v>103.01</v>
+        <v>66.01000000000001</v>
       </c>
       <c r="R33" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 1:15PM CST</t>
+          <t>Jun 5 1:35PM CST</t>
         </is>
       </c>
       <c r="S33" s="1" t="n">
@@ -4558,7 +4558,7 @@
         <v>0</v>
       </c>
       <c r="V33" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W33" s="1" t="n">
         <v>0</v>
@@ -4598,17 +4598,17 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Álvaro Zapata</t>
+          <t>/</t>
         </is>
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>126</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D34" s="9" t="n">
@@ -4616,36 +4616,36 @@
       </c>
       <c r="E34" s="1" t="inlineStr">
         <is>
-          <t>05:58:21</t>
+          <t>04:12:54</t>
         </is>
       </c>
       <c r="F34" s="1" t="n">
-        <v>317.3</v>
+        <v>68.09999999999999</v>
       </c>
       <c r="G34" s="1" t="n">
-        <v>77.04000000000001</v>
+        <v>8.31</v>
       </c>
       <c r="H34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I34" s="1" t="inlineStr">
         <is>
-          <t>00:03:40</t>
+          <t>00:02:08</t>
         </is>
       </c>
       <c r="J34" s="1" t="inlineStr">
         <is>
-          <t>00:03:52</t>
+          <t>00:03:02</t>
         </is>
       </c>
       <c r="K34" s="1" t="inlineStr">
         <is>
-          <t>00:01:16</t>
+          <t>00:00:46</t>
         </is>
       </c>
       <c r="L34" s="1" t="inlineStr">
         <is>
-          <t>00:01:04</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="M34" s="1" t="n">
@@ -4661,21 +4661,21 @@
         <v>0</v>
       </c>
       <c r="Q34" s="1" t="n">
-        <v>120.01</v>
+        <v>82.01000000000001</v>
       </c>
       <c r="R34" s="1" t="inlineStr">
         <is>
-          <t>Jun 4 11:02AM CST</t>
+          <t>Jun 5 11:00AM CST</t>
         </is>
       </c>
       <c r="S34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T34" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U34" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V34" s="1" t="n">
         <v>0</v>
@@ -4718,179 +4718,137 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Alberto Jimenez</t>
+          <t>David Serrano</t>
         </is>
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>125</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
-        </is>
-      </c>
-      <c r="D35" s="10" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="E35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="F35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="G35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="H35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="I35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="J35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="K35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="L35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="M35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="N35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="O35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="P35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Q35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="R35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="S35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="T35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="U35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="V35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="W35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="X35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Y35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Z35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AA35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AB35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AC35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AD35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AE35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AF35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
+          <t>TOYOTA HILUX 2017</t>
+        </is>
+      </c>
+      <c r="D35" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="inlineStr">
+        <is>
+          <t>02:25:29</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>50.3</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>4.44</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1" t="inlineStr">
+        <is>
+          <t>00:02:28</t>
+        </is>
+      </c>
+      <c r="J35" s="1" t="inlineStr">
+        <is>
+          <t>00:02:35</t>
+        </is>
+      </c>
+      <c r="K35" s="1" t="inlineStr">
+        <is>
+          <t>00:00:52</t>
+        </is>
+      </c>
+      <c r="L35" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="M35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1" t="n">
+        <v>92.01000000000001</v>
+      </c>
+      <c r="R35" s="1" t="inlineStr">
+        <is>
+          <t>Jun 5 10:30AM CST</t>
+        </is>
+      </c>
+      <c r="S35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="1" t="inlineStr">
+        <is>
+          <t>Sin ruta.</t>
+        </is>
+      </c>
+      <c r="Z35" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="AA35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Alberto Compras</t>
+          <t>Alberto Jimenez</t>
         </is>
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>103</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr">
         <is>
-          <t>NISSAN 1993</t>
+          <t>VAN HYUNDAI</t>
         </is>
       </c>
       <c r="D36" s="10" t="inlineStr">
@@ -5042,17 +5000,17 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Martin Quezada</t>
+          <t>Alberto Compras</t>
         </is>
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>115</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr">
         <is>
-          <t>INTERNACIONAL</t>
+          <t>NISSAN 1993</t>
         </is>
       </c>
       <c r="D37" s="10" t="inlineStr">

</xml_diff>

<commit_message>
Actualización automática: 2025-06-17 10:39
</commit_message>
<xml_diff>
--- a/seguridad/Informe_Diario_Unidades.xlsx
+++ b/seguridad/Informe_Diario_Unidades.xlsx
@@ -758,17 +758,17 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Luis Ibarra</t>
+          <t>Miguel Guizar</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>150</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
+          <t>Hino 300 2024</t>
         </is>
       </c>
       <c r="D2" s="7" t="n">
@@ -776,26 +776,26 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>07:04:02</t>
+          <t>05:38:51</t>
         </is>
       </c>
       <c r="F2" s="1" t="n">
-        <v>168.9</v>
+        <v>186</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>21.73</v>
+        <v>16.49</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>00:00:39</t>
+          <t>00:00:44</t>
         </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>00:00:23</t>
+          <t>00:00:27</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -821,11 +821,11 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>89.01000000000001</v>
+        <v>93.01000000000001</v>
       </c>
       <c r="R2" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 10:24AM CST</t>
+          <t>Jun 16 1:31PM CST</t>
         </is>
       </c>
       <c r="S2" s="1" t="n">
@@ -878,17 +878,17 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Alberto Sesmas</t>
+          <t>Diego Cardenas</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>134</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH</t>
+          <t>TOYOTA HILUX 2018</t>
         </is>
       </c>
       <c r="D3" s="7" t="n">
@@ -896,26 +896,26 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>03:09:40</t>
+          <t>03:13:20</t>
         </is>
       </c>
       <c r="F3" s="1" t="n">
-        <v>85.90000000000001</v>
+        <v>66.40000000000001</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>24.86</v>
+        <v>9.26</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:00:25</t>
         </is>
       </c>
       <c r="K3" s="1" t="inlineStr">
@@ -941,11 +941,11 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1" t="n">
-        <v>81.01000000000001</v>
+        <v>74.01000000000001</v>
       </c>
       <c r="R3" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 12:16PM CST</t>
+          <t>Jun 16 4:58PM CST</t>
         </is>
       </c>
       <c r="S3" s="1" t="n">
@@ -998,17 +998,17 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Hugo López</t>
+          <t>Daniel Iñiguez</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>131</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D4" s="7" t="n">
@@ -1016,26 +1016,26 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>04:33:19</t>
+          <t>02:29:24</t>
         </is>
       </c>
       <c r="F4" s="1" t="n">
-        <v>68.40000000000001</v>
+        <v>41.9</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>12.05</v>
+        <v>5.33</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="1" t="inlineStr">
         <is>
-          <t>00:00:42</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
@@ -1061,11 +1061,11 @@
         <v>0</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>67.01000000000001</v>
+        <v>65.01000000000001</v>
       </c>
       <c r="R4" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 2:13PM CST</t>
+          <t>Jun 16 2:34PM CST</t>
         </is>
       </c>
       <c r="S4" s="1" t="n">
@@ -1118,17 +1118,17 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Gerardo Aguillón</t>
+          <t>Marcos Barbosa</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>147</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX 2023</t>
         </is>
       </c>
       <c r="D5" s="7" t="n">
@@ -1136,14 +1136,14 @@
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>05:09:27</t>
+          <t>02:50:04</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>65.3</v>
+        <v>38.4</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>10.3</v>
+        <v>5.86</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="R5" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 1:31PM CST</t>
+          <t>Jun 16 12:00PM CST</t>
         </is>
       </c>
       <c r="S5" s="1" t="n">
@@ -1256,26 +1256,26 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>05:08:35</t>
+          <t>02:26:09</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>64.3</v>
+        <v>32.6</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>12.33</v>
+        <v>5.81</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>00:00:55</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:21</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr">
@@ -1301,11 +1301,11 @@
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="n">
-        <v>59</v>
+        <v>76.01000000000001</v>
       </c>
       <c r="R6" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 1:19PM CST</t>
+          <t>Jun 16 1:14PM CST</t>
         </is>
       </c>
       <c r="S6" s="1" t="n">
@@ -1358,17 +1358,17 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Marcos Barbosa</t>
+          <t>Hugo López</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>153</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2023</t>
+          <t>TOYOTA HILUX</t>
         </is>
       </c>
       <c r="D7" s="7" t="n">
@@ -1376,26 +1376,26 @@
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>03:37:08</t>
+          <t>02:10:17</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>47.4</v>
+        <v>32.3</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>7.43</v>
+        <v>6.52</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>00:00:55</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="R7" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 11:42AM CST</t>
+          <t>Jun 16 12:40PM CST</t>
         </is>
       </c>
       <c r="S7" s="1" t="n">
@@ -1478,17 +1478,17 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Alejandro Lara</t>
+          <t>Gerardo Aguillón</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>142</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>WORKEN</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D8" s="7" t="n">
@@ -1496,21 +1496,21 @@
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>01:36:41</t>
+          <t>02:25:46</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>44.7</v>
+        <v>31.5</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>11.5</v>
+        <v>4.97</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:04</t>
         </is>
       </c>
       <c r="J8" s="1" t="inlineStr">
@@ -1541,11 +1541,11 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="R8" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 7:47AM CST</t>
+          <t>Jun 16 3:52PM CST</t>
         </is>
       </c>
       <c r="S8" s="1" t="n">
@@ -1598,17 +1598,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Luis Ramirez</t>
+          <t>Daniel Magallanes</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>127</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>FORD F350 3MTS 2006</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D9" s="7" t="n">
@@ -1616,21 +1616,21 @@
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>03:46:09</t>
+          <t>01:12:17</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>40.5</v>
+        <v>25.3</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>17.85</v>
+        <v>2.2</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="J9" s="1" t="inlineStr">
@@ -1661,11 +1661,11 @@
         <v>0</v>
       </c>
       <c r="Q9" s="1" t="n">
-        <v>59</v>
+        <v>78.01000000000001</v>
       </c>
       <c r="R9" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 12:50PM CST</t>
+          <t>Jun 16 6:28PM CST</t>
         </is>
       </c>
       <c r="S9" s="1" t="n">
@@ -1718,17 +1718,17 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Martin Quezada</t>
+          <t>Kevin De La O</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>116</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>INTERNACIONAL</t>
+          <t>VAN HYUNDAI</t>
         </is>
       </c>
       <c r="D10" s="7" t="n">
@@ -1736,21 +1736,21 @@
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>01:28:18</t>
+          <t>00:17:44</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>24.4</v>
+        <v>5.8</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>14.72</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J10" s="1" t="inlineStr">
@@ -1781,11 +1781,11 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="n">
-        <v>56</v>
+        <v>51.54</v>
       </c>
       <c r="R10" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 10:28AM CST</t>
+          <t>Jun 16 2:07PM CST</t>
         </is>
       </c>
       <c r="S10" s="1" t="n">
@@ -1838,44 +1838,44 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Daniel Mercado</t>
+          <t>Alejandro Suarez</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>146</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>HINO 500</t>
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>06:28:29</t>
+          <t>00:18:35</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>145.9</v>
+        <v>4.5</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>19.16</v>
+        <v>1.37</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="inlineStr">
         <is>
-          <t>00:02:33</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J11" s="1" t="inlineStr">
         <is>
-          <t>00:00:49</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K11" s="1" t="inlineStr">
@@ -1901,11 +1901,11 @@
         <v>0</v>
       </c>
       <c r="Q11" s="1" t="n">
-        <v>85.01000000000001</v>
+        <v>50</v>
       </c>
       <c r="R11" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 10:33AM CST</t>
+          <t>Jun 16 4:46PM CST</t>
         </is>
       </c>
       <c r="S11" s="1" t="n">
@@ -1958,49 +1958,49 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Daniel Iñiguez</t>
+          <t>Martin Quezada</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>122</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>INTERNACIONAL</t>
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>07:31:28</t>
+          <t>00:17:39</t>
         </is>
       </c>
       <c r="F12" s="1" t="n">
-        <v>136.4</v>
+        <v>4</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>18.66</v>
+        <v>2.7</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I12" s="1" t="inlineStr">
         <is>
-          <t>00:01:37</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J12" s="1" t="inlineStr">
         <is>
-          <t>00:00:42</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K12" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L12" s="1" t="inlineStr">
@@ -2021,11 +2021,11 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="n">
-        <v>75.01000000000001</v>
+        <v>54</v>
       </c>
       <c r="R12" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 8:30AM CST</t>
+          <t>Jun 16 3:05PM CST</t>
         </is>
       </c>
       <c r="S12" s="1" t="n">
@@ -2078,44 +2078,44 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Angel Cortez</t>
+          <t>Jorge Tornero</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>117</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2018</t>
+          <t>HINO 300</t>
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>03:39:52</t>
+          <t>00:02:30</t>
         </is>
       </c>
       <c r="F13" s="1" t="n">
-        <v>101.4</v>
+        <v>0.5</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>14.53</v>
+        <v>0.35</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="inlineStr">
         <is>
-          <t>00:01:09</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J13" s="1" t="inlineStr">
         <is>
-          <t>00:00:48</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K13" s="1" t="inlineStr">
@@ -2141,11 +2141,11 @@
         <v>0</v>
       </c>
       <c r="Q13" s="1" t="n">
-        <v>83.01000000000001</v>
+        <v>51</v>
       </c>
       <c r="R13" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 10:50AM CST</t>
+          <t>Jun 16 4:31PM CST</t>
         </is>
       </c>
       <c r="S13" s="1" t="n">
@@ -2198,44 +2198,44 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Fernando Ornelas</t>
+          <t>Francisco Marquez</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>135</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2020</t>
+          <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>04:25:46</t>
+          <t>00:01:18</t>
         </is>
       </c>
       <c r="F14" s="1" t="n">
-        <v>72.09999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>12.38</v>
+        <v>0.5</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="inlineStr">
         <is>
-          <t>00:01:29</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J14" s="1" t="inlineStr">
         <is>
-          <t>00:01:44</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K14" s="1" t="inlineStr">
@@ -2261,11 +2261,11 @@
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>79.01000000000001</v>
+        <v>18</v>
       </c>
       <c r="R14" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 10:07AM CST</t>
+          <t>Jun 16 7:05PM CST</t>
         </is>
       </c>
       <c r="S14" s="1" t="n">
@@ -2318,17 +2318,17 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Daniel Magallanes</t>
+          <t>Luis Galindo</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>118</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>KENWORTH 2009</t>
         </is>
       </c>
       <c r="D15" s="7" t="n">
@@ -2336,26 +2336,26 @@
       </c>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>03:42:11</t>
+          <t>03:10:40</t>
         </is>
       </c>
       <c r="F15" s="1" t="n">
-        <v>60.1</v>
+        <v>81.90000000000001</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>5.61</v>
+        <v>27.58</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="inlineStr">
         <is>
-          <t>00:00:37</t>
+          <t>00:01:05</t>
         </is>
       </c>
       <c r="J15" s="1" t="inlineStr">
         <is>
-          <t>00:00:50</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="K15" s="1" t="inlineStr">
@@ -2381,11 +2381,11 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>74.01000000000001</v>
+        <v>79.01000000000001</v>
       </c>
       <c r="R15" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 7:52AM CST</t>
+          <t>Jun 16 9:20AM CST</t>
         </is>
       </c>
       <c r="S15" s="1" t="n">
@@ -2438,12 +2438,12 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Miguel Zamora</t>
+          <t>Fernando Garcia</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
@@ -2456,11 +2456,11 @@
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>03:16:53</t>
+          <t>02:11:13</t>
         </is>
       </c>
       <c r="F16" s="1" t="n">
-        <v>58.7</v>
+        <v>68.09999999999999</v>
       </c>
       <c r="G16" s="1" t="n">
         <v>0</v>
@@ -2470,12 +2470,12 @@
       </c>
       <c r="I16" s="1" t="inlineStr">
         <is>
-          <t>00:01:37</t>
+          <t>00:00:32</t>
         </is>
       </c>
       <c r="J16" s="1" t="inlineStr">
         <is>
-          <t>00:00:57</t>
+          <t>00:00:56</t>
         </is>
       </c>
       <c r="K16" s="1" t="inlineStr">
@@ -2501,11 +2501,11 @@
         <v>0</v>
       </c>
       <c r="Q16" s="1" t="n">
-        <v>91.04000000000001</v>
+        <v>84.5</v>
       </c>
       <c r="R16" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 2:51PM CST</t>
+          <t>Jun 16 2:35PM CST</t>
         </is>
       </c>
       <c r="S16" s="1" t="n">
@@ -2558,44 +2558,44 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>José Morales</t>
+          <t>Daniel Rocha</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>136</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX 2020</t>
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>05:39:20</t>
+          <t>02:56:16</t>
         </is>
       </c>
       <c r="F17" s="1" t="n">
-        <v>101.2</v>
+        <v>49</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>13.59</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>00:03:48</t>
+          <t>00:00:43</t>
         </is>
       </c>
       <c r="J17" s="1" t="inlineStr">
         <is>
-          <t>00:02:50</t>
+          <t>00:00:39</t>
         </is>
       </c>
       <c r="K17" s="1" t="inlineStr">
@@ -2621,11 +2621,11 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="n">
-        <v>78.01000000000001</v>
+        <v>66.01000000000001</v>
       </c>
       <c r="R17" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 11:27AM CST</t>
+          <t>Jun 16 1:42PM CST</t>
         </is>
       </c>
       <c r="S17" s="1" t="n">
@@ -2678,49 +2678,49 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Kevin De La O</t>
+          <t xml:space="preserve">David Herrera </t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>120</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
+          <t>FORD RANGER 2011</t>
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E18" s="1" t="inlineStr">
         <is>
-          <t>05:10:21</t>
+          <t>01:44:53</t>
         </is>
       </c>
       <c r="F18" s="1" t="n">
-        <v>96.3</v>
+        <v>30.2</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>0</v>
+        <v>4.82</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="inlineStr">
         <is>
-          <t>00:01:28</t>
+          <t>00:00:32</t>
         </is>
       </c>
       <c r="J18" s="1" t="inlineStr">
         <is>
-          <t>00:01:58</t>
+          <t>00:00:28</t>
         </is>
       </c>
       <c r="K18" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L18" s="1" t="inlineStr">
@@ -2741,11 +2741,11 @@
         <v>0</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>95.91</v>
+        <v>66.01000000000001</v>
       </c>
       <c r="R18" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 7:49AM CST</t>
+          <t>Jun 16 12:39PM CST</t>
         </is>
       </c>
       <c r="S18" s="1" t="n">
@@ -2798,49 +2798,49 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>Moises Martinez</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>149</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>TOYOTA HILUX 2024</t>
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>04:21:59</t>
+          <t>00:56:47</t>
         </is>
       </c>
       <c r="F19" s="1" t="n">
-        <v>78.09999999999999</v>
+        <v>29.3</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>9.15</v>
+        <v>3.83</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="inlineStr">
         <is>
-          <t>00:01:49</t>
+          <t>00:00:17</t>
         </is>
       </c>
       <c r="J19" s="1" t="inlineStr">
         <is>
-          <t>00:01:25</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="K19" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L19" s="1" t="inlineStr">
@@ -2861,11 +2861,11 @@
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>84.01000000000001</v>
+        <v>66.01000000000001</v>
       </c>
       <c r="R19" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 11:50AM CST</t>
+          <t>Jun 16 12:05PM CST</t>
         </is>
       </c>
       <c r="S19" s="1" t="n">
@@ -2918,49 +2918,49 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Diego Cardenas</t>
+          <t>Eduardo Hernandez</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>152</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2018</t>
+          <t>TOYOTA HILUX</t>
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>08:09:01</t>
+          <t>01:19:49</t>
         </is>
       </c>
       <c r="F20" s="1" t="n">
-        <v>171.6</v>
+        <v>25.4</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>24.08</v>
+        <v>3.87</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="inlineStr">
         <is>
-          <t>00:03:50</t>
+          <t>00:00:37</t>
         </is>
       </c>
       <c r="J20" s="1" t="inlineStr">
         <is>
-          <t>00:02:42</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="K20" s="1" t="inlineStr">
         <is>
-          <t>00:00:55</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L20" s="1" t="inlineStr">
@@ -2981,11 +2981,11 @@
         <v>0</v>
       </c>
       <c r="Q20" s="1" t="n">
-        <v>90.01000000000001</v>
+        <v>69.01000000000001</v>
       </c>
       <c r="R20" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 8:20AM CST</t>
+          <t>Jun 16 3:15PM CST</t>
         </is>
       </c>
       <c r="S20" s="1" t="n">
@@ -3038,49 +3038,49 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Moises Martinez</t>
+          <t xml:space="preserve">Cristian Estrada </t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>132</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>04:31:59</t>
+          <t>04:01:30</t>
         </is>
       </c>
       <c r="F21" s="1" t="n">
-        <v>101</v>
+        <v>92.90000000000001</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>16.32</v>
+        <v>12.4</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="inlineStr">
         <is>
-          <t>00:01:37</t>
+          <t>00:03:39</t>
         </is>
       </c>
       <c r="J21" s="1" t="inlineStr">
         <is>
-          <t>00:03:15</t>
+          <t>00:02:01</t>
         </is>
       </c>
       <c r="K21" s="1" t="inlineStr">
         <is>
-          <t>00:00:37</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L21" s="1" t="inlineStr">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="R21" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 12:03PM CST</t>
+          <t>Jun 16 2:07PM CST</t>
         </is>
       </c>
       <c r="S21" s="1" t="n">
@@ -3158,49 +3158,49 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">David Herrera </t>
+          <t>José Morales</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>141</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t>FORD RANGER 2011</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>05:32:03</t>
+          <t>01:19:15</t>
         </is>
       </c>
       <c r="F22" s="1" t="n">
-        <v>177.1</v>
+        <v>27.2</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>21.3</v>
+        <v>4.18</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="inlineStr">
         <is>
-          <t>00:05:25</t>
+          <t>00:00:49</t>
         </is>
       </c>
       <c r="J22" s="1" t="inlineStr">
         <is>
-          <t>00:05:38</t>
+          <t>00:00:27</t>
         </is>
       </c>
       <c r="K22" s="1" t="inlineStr">
         <is>
-          <t>00:00:43</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L22" s="1" t="inlineStr">
@@ -3221,11 +3221,11 @@
         <v>0</v>
       </c>
       <c r="Q22" s="1" t="n">
-        <v>102.01</v>
+        <v>71.01000000000001</v>
       </c>
       <c r="R22" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 3:14PM CST</t>
+          <t>Jun 16 11:01AM CST</t>
         </is>
       </c>
       <c r="S22" s="1" t="n">
@@ -3278,61 +3278,61 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cristian Estrada </t>
+          <t>Fernando Ornelas</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>138</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>TOYOTA HILUX 2020</t>
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>06:33:33</t>
+          <t>01:48:24</t>
         </is>
       </c>
       <c r="F23" s="1" t="n">
-        <v>103.3</v>
+        <v>33.6</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>16.91</v>
+        <v>5.75</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I23" s="1" t="inlineStr">
         <is>
-          <t>00:02:08</t>
+          <t>00:00:49</t>
         </is>
       </c>
       <c r="J23" s="1" t="inlineStr">
         <is>
-          <t>00:02:08</t>
+          <t>00:06:10</t>
         </is>
       </c>
       <c r="K23" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L23" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N23" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23" s="1" t="n">
         <v>0</v>
@@ -3341,11 +3341,11 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>85.01000000000001</v>
+        <v>76.01000000000001</v>
       </c>
       <c r="R23" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 1:24PM CST</t>
+          <t>Jun 16 1:19PM CST</t>
         </is>
       </c>
       <c r="S23" s="1" t="n">
@@ -3398,54 +3398,54 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Daniel Rocha</t>
+          <t>Daniel Mercado</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>130</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2020</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D24" s="8" t="n">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>06:42:40</t>
+          <t>02:30:48</t>
         </is>
       </c>
       <c r="F24" s="1" t="n">
-        <v>125.8</v>
+        <v>46.6</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>20.35</v>
+        <v>6.92</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I24" s="1" t="inlineStr">
         <is>
-          <t>00:00:55</t>
+          <t>00:00:49</t>
         </is>
       </c>
       <c r="J24" s="1" t="inlineStr">
         <is>
-          <t>00:00:50</t>
+          <t>00:02:04</t>
         </is>
       </c>
       <c r="K24" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:43</t>
         </is>
       </c>
       <c r="L24" s="1" t="inlineStr">
         <is>
-          <t>00:00:36</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M24" s="1" t="n">
@@ -3461,11 +3461,11 @@
         <v>0</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>81.01000000000001</v>
+        <v>84.01000000000001</v>
       </c>
       <c r="R24" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 2:34PM CST</t>
+          <t>Jun 16 2:22PM CST</t>
         </is>
       </c>
       <c r="S24" s="1" t="n">
@@ -3518,74 +3518,74 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Alexis Alvarado</t>
+          <t>Angel Cortez</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>133</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr">
         <is>
-          <t>HINO 500</t>
-        </is>
-      </c>
-      <c r="D25" s="9" t="n">
-        <v>68</v>
+          <t>TOYOTA HILUX 2018</t>
+        </is>
+      </c>
+      <c r="D25" s="8" t="n">
+        <v>86</v>
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>08:28:28</t>
+          <t>04:03:33</t>
         </is>
       </c>
       <c r="F25" s="1" t="n">
-        <v>616.5</v>
+        <v>90.8</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>129.79</v>
+        <v>14.64</v>
       </c>
       <c r="H25" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I25" s="1" t="inlineStr">
         <is>
-          <t>00:13:55</t>
+          <t>00:03:30</t>
         </is>
       </c>
       <c r="J25" s="1" t="inlineStr">
         <is>
-          <t>00:16:30</t>
+          <t>00:01:29</t>
         </is>
       </c>
       <c r="K25" s="1" t="inlineStr">
         <is>
-          <t>00:04:40</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="L25" s="1" t="inlineStr">
         <is>
-          <t>00:00:27</t>
+          <t>00:00:17</t>
         </is>
       </c>
       <c r="M25" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N25" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O25" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q25" s="1" t="n">
-        <v>107.01</v>
+        <v>80.01000000000001</v>
       </c>
       <c r="R25" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 4:26AM CST</t>
+          <t>Jun 16 5:10PM CST</t>
         </is>
       </c>
       <c r="S25" s="1" t="n">
@@ -3638,61 +3638,61 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Armando Muñoz</t>
+          <t>Alberto Sanchez</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>154</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>HINO 300</t>
-        </is>
-      </c>
-      <c r="D26" s="9" t="n">
-        <v>68</v>
+          <t>VW DELIVERY 10.6</t>
+        </is>
+      </c>
+      <c r="D26" s="8" t="n">
+        <v>79</v>
       </c>
       <c r="E26" s="1" t="inlineStr">
         <is>
-          <t>07:18:08</t>
+          <t>05:54:13</t>
         </is>
       </c>
       <c r="F26" s="1" t="n">
-        <v>185.2</v>
+        <v>285.4</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>23.61</v>
+        <v>0</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="1" t="inlineStr">
         <is>
-          <t>00:07:29</t>
+          <t>00:11:23</t>
         </is>
       </c>
       <c r="J26" s="1" t="inlineStr">
         <is>
-          <t>00:06:06</t>
+          <t>00:08:23</t>
         </is>
       </c>
       <c r="K26" s="1" t="inlineStr">
         <is>
-          <t>00:00:33</t>
+          <t>00:00:59</t>
         </is>
       </c>
       <c r="L26" s="1" t="inlineStr">
         <is>
-          <t>00:01:11</t>
+          <t>00:00:22</t>
         </is>
       </c>
       <c r="M26" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O26" s="1" t="n">
         <v>0</v>
@@ -3701,11 +3701,11 @@
         <v>0</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <v>89.01000000000001</v>
+        <v>112.63</v>
       </c>
       <c r="R26" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 1:03PM CST</t>
+          <t>Jun 16 12:34PM CST</t>
         </is>
       </c>
       <c r="S26" s="1" t="n">
@@ -3758,12 +3758,12 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Fernando Garcia</t>
+          <t>Miguel Zamora</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
@@ -3771,16 +3771,16 @@
           <t>Volkswagen</t>
         </is>
       </c>
-      <c r="D27" s="9" t="n">
-        <v>67</v>
+      <c r="D27" s="8" t="n">
+        <v>77</v>
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
-          <t>05:39:20</t>
+          <t>09:48:13</t>
         </is>
       </c>
       <c r="F27" s="1" t="n">
-        <v>319.9</v>
+        <v>484</v>
       </c>
       <c r="G27" s="1" t="n">
         <v>0</v>
@@ -3790,42 +3790,42 @@
       </c>
       <c r="I27" s="1" t="inlineStr">
         <is>
-          <t>00:08:02</t>
+          <t>00:05:26</t>
         </is>
       </c>
       <c r="J27" s="1" t="inlineStr">
         <is>
-          <t>00:10:09</t>
+          <t>00:06:47</t>
         </is>
       </c>
       <c r="K27" s="1" t="inlineStr">
         <is>
-          <t>00:04:05</t>
+          <t>00:04:55</t>
         </is>
       </c>
       <c r="L27" s="1" t="inlineStr">
         <is>
-          <t>00:00:12</t>
+          <t>00:00:22</t>
         </is>
       </c>
       <c r="M27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="O27" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="P27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <v>100.19</v>
+        <v>103.9</v>
       </c>
       <c r="R27" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 10:05AM CST</t>
+          <t>Jun 16 9:28AM CST</t>
         </is>
       </c>
       <c r="S27" s="1" t="n">
@@ -3878,62 +3878,62 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Jorge Tornero</t>
+          <t>Mario Ballinas</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>144</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>HINO 300</t>
-        </is>
-      </c>
-      <c r="D28" s="9" t="n">
-        <v>64</v>
+          <t>TOYOTA HILUX 2021</t>
+        </is>
+      </c>
+      <c r="D28" s="8" t="n">
+        <v>74</v>
       </c>
       <c r="E28" s="1" t="inlineStr">
         <is>
-          <t>07:41:56</t>
+          <t>03:19:11</t>
         </is>
       </c>
       <c r="F28" s="1" t="n">
-        <v>153.4</v>
+        <v>76.7</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>14.37</v>
+        <v>9.26</v>
       </c>
       <c r="H28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1" t="inlineStr">
+        <is>
+          <t>00:04:21</t>
+        </is>
+      </c>
+      <c r="J28" s="1" t="inlineStr">
+        <is>
+          <t>00:03:20</t>
+        </is>
+      </c>
+      <c r="K28" s="1" t="inlineStr">
+        <is>
+          <t>00:01:01</t>
+        </is>
+      </c>
+      <c r="L28" s="1" t="inlineStr">
+        <is>
+          <t>00:00:16</t>
+        </is>
+      </c>
+      <c r="M28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I28" s="1" t="inlineStr">
-        <is>
-          <t>00:04:18</t>
-        </is>
-      </c>
-      <c r="J28" s="1" t="inlineStr">
-        <is>
-          <t>00:01:56</t>
-        </is>
-      </c>
-      <c r="K28" s="1" t="inlineStr">
-        <is>
-          <t>00:00:11</t>
-        </is>
-      </c>
-      <c r="L28" s="1" t="inlineStr">
-        <is>
-          <t>00:00:06</t>
-        </is>
-      </c>
-      <c r="M28" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="O28" s="1" t="n">
         <v>0</v>
       </c>
@@ -3941,11 +3941,11 @@
         <v>0</v>
       </c>
       <c r="Q28" s="1" t="n">
-        <v>75.01000000000001</v>
+        <v>90.01000000000001</v>
       </c>
       <c r="R28" s="1" t="inlineStr">
         <is>
-          <t>Jun 14 8:20AM CST</t>
+          <t>Jun 16 2:00PM CST</t>
         </is>
       </c>
       <c r="S28" s="1" t="n">
@@ -3958,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="V28" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W28" s="1" t="n">
         <v>0</v>
@@ -3998,54 +3998,54 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>David Serrano</t>
+          <t>Luis Ibarra</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>148</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>TOYOTA HILUX 2024</t>
         </is>
       </c>
       <c r="D29" s="9" t="n">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E29" s="1" t="inlineStr">
         <is>
-          <t>04:57:54</t>
+          <t>04:09:49</t>
         </is>
       </c>
       <c r="F29" s="1" t="n">
-        <v>112.1</v>
+        <v>95.8</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>10.77</v>
+        <v>12.82</v>
       </c>
       <c r="H29" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="1" t="inlineStr">
         <is>
-          <t>00:02:10</t>
+          <t>00:00:39</t>
         </is>
       </c>
       <c r="J29" s="1" t="inlineStr">
         <is>
-          <t>00:05:10</t>
+          <t>00:00:25</t>
         </is>
       </c>
       <c r="K29" s="1" t="inlineStr">
         <is>
-          <t>00:01:51</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="L29" s="1" t="inlineStr">
         <is>
-          <t>00:00:48</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M29" s="1" t="n">
@@ -4061,11 +4061,11 @@
         <v>0</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>102.01</v>
+        <v>74.01000000000001</v>
       </c>
       <c r="R29" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 8:29AM CST</t>
+          <t>Jun 16 1:21PM CST</t>
         </is>
       </c>
       <c r="S29" s="1" t="n">
@@ -4078,7 +4078,7 @@
         <v>0</v>
       </c>
       <c r="V29" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W29" s="1" t="n">
         <v>0</v>
@@ -4118,81 +4118,81 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Francisco Marquez</t>
+          <t>David Serrano</t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>125</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D30" s="9" t="n">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1" t="inlineStr">
         <is>
-          <t>14:06:21</t>
+          <t>03:30:40</t>
         </is>
       </c>
       <c r="F30" s="1" t="n">
-        <v>747.2</v>
+        <v>71.8</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>230.99</v>
+        <v>6.45</v>
       </c>
       <c r="H30" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I30" s="1" t="inlineStr">
         <is>
-          <t>00:15:48</t>
+          <t>00:01:11</t>
         </is>
       </c>
       <c r="J30" s="1" t="inlineStr">
         <is>
-          <t>00:12:50</t>
+          <t>00:03:00</t>
         </is>
       </c>
       <c r="K30" s="1" t="inlineStr">
         <is>
-          <t>00:07:30</t>
+          <t>00:01:39</t>
         </is>
       </c>
       <c r="L30" s="1" t="inlineStr">
         <is>
-          <t>00:01:59</t>
+          <t>00:00:17</t>
         </is>
       </c>
       <c r="M30" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O30" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P30" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q30" s="1" t="n">
-        <v>100.01</v>
+        <v>84.01000000000001</v>
       </c>
       <c r="R30" s="1" t="inlineStr">
         <is>
-          <t>Jun 13 4:21AM CST</t>
+          <t>Jun 16 9:34AM CST</t>
         </is>
       </c>
       <c r="S30" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T30" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U30" s="1" t="n">
         <v>0</v>
@@ -4238,737 +4238,989 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Alejandro Suarez</t>
+          <t>Luis Ramirez</t>
         </is>
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>101</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>HINO 500</t>
-        </is>
-      </c>
-      <c r="D31" s="9" t="n">
-        <v>52</v>
-      </c>
-      <c r="E31" s="1" t="inlineStr">
-        <is>
-          <t>14:09:07</t>
-        </is>
-      </c>
-      <c r="F31" s="1" t="n">
-        <v>726.3</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>176.47</v>
-      </c>
-      <c r="H31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" s="1" t="inlineStr">
-        <is>
-          <t>00:12:40</t>
-        </is>
-      </c>
-      <c r="J31" s="1" t="inlineStr">
-        <is>
-          <t>00:13:14</t>
-        </is>
-      </c>
-      <c r="K31" s="1" t="inlineStr">
-        <is>
-          <t>00:07:20</t>
-        </is>
-      </c>
-      <c r="L31" s="1" t="inlineStr">
-        <is>
-          <t>00:02:29</t>
-        </is>
-      </c>
-      <c r="M31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O31" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="P31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="1" t="n">
-        <v>109.01</v>
-      </c>
-      <c r="R31" s="1" t="inlineStr">
-        <is>
-          <t>Jun 14 3:38PM CST</t>
-        </is>
-      </c>
-      <c r="S31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z31" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE31" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF31" s="1" t="n">
-        <v>0</v>
+          <t>FORD F350 3MTS 2006</t>
+        </is>
+      </c>
+      <c r="D31" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF31" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Luis Galindo</t>
+          <t>Armando Muñoz</t>
         </is>
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>102</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH 2009</t>
-        </is>
-      </c>
-      <c r="D32" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1" t="inlineStr">
-        <is>
-          <t>08:22:27</t>
-        </is>
-      </c>
-      <c r="F32" s="1" t="n">
-        <v>416</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <v>115.1</v>
-      </c>
-      <c r="H32" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I32" s="1" t="inlineStr">
-        <is>
-          <t>00:07:11</t>
-        </is>
-      </c>
-      <c r="J32" s="1" t="inlineStr">
-        <is>
-          <t>00:17:53</t>
-        </is>
-      </c>
-      <c r="K32" s="1" t="inlineStr">
-        <is>
-          <t>00:12:52</t>
-        </is>
-      </c>
-      <c r="L32" s="1" t="inlineStr">
-        <is>
-          <t>00:02:59</t>
-        </is>
-      </c>
-      <c r="M32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="N32" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="O32" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="P32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="1" t="n">
-        <v>97.01000000000001</v>
-      </c>
-      <c r="R32" s="1" t="inlineStr">
-        <is>
-          <t>Jun 13 12:11PM CST</t>
-        </is>
-      </c>
-      <c r="S32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V32" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="W32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y32" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z32" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE32" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF32" s="1" t="n">
-        <v>0</v>
+          <t>HINO 300</t>
+        </is>
+      </c>
+      <c r="D32" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF32" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Miguel Guizar</t>
+          <t>Alberto Jimenez</t>
         </is>
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>103</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr">
         <is>
-          <t>Hino 300 2024</t>
-        </is>
-      </c>
-      <c r="D33" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" s="1" t="inlineStr">
-        <is>
-          <t>10:34:35</t>
-        </is>
-      </c>
-      <c r="F33" s="1" t="n">
-        <v>345.7</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>36.09</v>
-      </c>
-      <c r="H33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" s="1" t="inlineStr">
-        <is>
-          <t>00:09:26</t>
-        </is>
-      </c>
-      <c r="J33" s="1" t="inlineStr">
-        <is>
-          <t>00:11:15</t>
-        </is>
-      </c>
-      <c r="K33" s="1" t="inlineStr">
-        <is>
-          <t>00:06:23</t>
-        </is>
-      </c>
-      <c r="L33" s="1" t="inlineStr">
-        <is>
-          <t>00:05:22</t>
-        </is>
-      </c>
-      <c r="M33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="O33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P33" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q33" s="1" t="n">
-        <v>96.01000000000001</v>
-      </c>
-      <c r="R33" s="1" t="inlineStr">
-        <is>
-          <t>Jun 13 6:13PM CST</t>
-        </is>
-      </c>
-      <c r="S33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y33" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z33" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF33" s="1" t="n">
-        <v>0</v>
+          <t>VAN HYUNDAI</t>
+        </is>
+      </c>
+      <c r="D33" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF33" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Alberto Sanchez</t>
+          <t>Alejandro Lara</t>
         </is>
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>110</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>VW DELIVERY 10.6</t>
-        </is>
-      </c>
-      <c r="D34" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="1" t="inlineStr">
-        <is>
-          <t>06:27:38</t>
-        </is>
-      </c>
-      <c r="F34" s="1" t="n">
-        <v>244.4</v>
-      </c>
-      <c r="G34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" s="1" t="inlineStr">
-        <is>
-          <t>00:03:41</t>
-        </is>
-      </c>
-      <c r="J34" s="1" t="inlineStr">
-        <is>
-          <t>00:04:41</t>
-        </is>
-      </c>
-      <c r="K34" s="1" t="inlineStr">
-        <is>
-          <t>00:04:59</t>
-        </is>
-      </c>
-      <c r="L34" s="1" t="inlineStr">
-        <is>
-          <t>00:05:30</t>
-        </is>
-      </c>
-      <c r="M34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O34" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="P34" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q34" s="1" t="n">
-        <v>105.44</v>
-      </c>
-      <c r="R34" s="1" t="inlineStr">
-        <is>
-          <t>Jun 13 1:46PM CST</t>
-        </is>
-      </c>
-      <c r="S34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z34" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE34" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF34" s="1" t="n">
-        <v>0</v>
+          <t>WORKEN</t>
+        </is>
+      </c>
+      <c r="D34" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF34" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Mario Ballinas</t>
+          <t>Alberto Compras</t>
         </is>
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>115</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
-        </is>
-      </c>
-      <c r="D35" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" s="1" t="inlineStr">
-        <is>
-          <t>05:19:22</t>
-        </is>
-      </c>
-      <c r="F35" s="1" t="n">
-        <v>94.5</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>14.97</v>
-      </c>
-      <c r="H35" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I35" s="1" t="inlineStr">
-        <is>
-          <t>00:03:26</t>
-        </is>
-      </c>
-      <c r="J35" s="1" t="inlineStr">
-        <is>
-          <t>00:01:49</t>
-        </is>
-      </c>
-      <c r="K35" s="1" t="inlineStr">
-        <is>
-          <t>00:00:05</t>
-        </is>
-      </c>
-      <c r="L35" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="M35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="1" t="n">
-        <v>77.01000000000001</v>
-      </c>
-      <c r="R35" s="1" t="inlineStr">
-        <is>
-          <t>Jun 13 5:58PM CST</t>
-        </is>
-      </c>
-      <c r="S35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T35" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="U35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y35" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z35" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF35" s="1" t="n">
-        <v>0</v>
+          <t>NISSAN 1993</t>
+        </is>
+      </c>
+      <c r="D35" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Eduardo Hernandez</t>
+          <t>Alberto Sesmas</t>
         </is>
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>124</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX</t>
-        </is>
-      </c>
-      <c r="D36" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="1" t="inlineStr">
-        <is>
-          <t>04:56:55</t>
-        </is>
-      </c>
-      <c r="F36" s="1" t="n">
-        <v>87.5</v>
-      </c>
-      <c r="G36" s="1" t="n">
-        <v>13.9</v>
-      </c>
-      <c r="H36" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I36" s="1" t="inlineStr">
-        <is>
-          <t>00:01:51</t>
-        </is>
-      </c>
-      <c r="J36" s="1" t="inlineStr">
-        <is>
-          <t>00:01:09</t>
-        </is>
-      </c>
-      <c r="K36" s="1" t="inlineStr">
-        <is>
-          <t>00:00:05</t>
-        </is>
-      </c>
-      <c r="L36" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="M36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="1" t="n">
-        <v>73.01000000000001</v>
-      </c>
-      <c r="R36" s="1" t="inlineStr">
-        <is>
-          <t>Jun 14 12:47PM CST</t>
-        </is>
-      </c>
-      <c r="S36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U36" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="V36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z36" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF36" s="1" t="n">
-        <v>0</v>
+          <t>KENWORTH</t>
+        </is>
+      </c>
+      <c r="D36" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Alberto Jimenez</t>
+          <t>/</t>
         </is>
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>126</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D37" s="10" t="inlineStr">
@@ -5120,17 +5372,17 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Alberto Compras</t>
+          <t>Abraham Arana</t>
         </is>
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr">
         <is>
-          <t>NISSAN 1993</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D38" s="10" t="inlineStr">
@@ -5282,17 +5534,17 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Abraham Arana</t>
+          <t>Alexis Alvarado</t>
         </is>
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>145</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>HINO 500</t>
         </is>
       </c>
       <c r="D39" s="10" t="inlineStr">

</xml_diff>

<commit_message>
Actualización automática: 2025-06-19 10:22
</commit_message>
<xml_diff>
--- a/seguridad/Informe_Diario_Unidades.xlsx
+++ b/seguridad/Informe_Diario_Unidades.xlsx
@@ -221,8 +221,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="InformeTable" displayName="InformeTable" ref="A1:AF39" headerRowCount="1">
-  <autoFilter ref="A1:AF39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="InformeTable" displayName="InformeTable" ref="A1:AF41" headerRowCount="1">
+  <autoFilter ref="A1:AF41"/>
   <tableColumns count="32">
     <tableColumn id="1" name="Operador"/>
     <tableColumn id="2" name="Número de unidad"/>
@@ -550,7 +550,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF39"/>
+  <dimension ref="A1:AF41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
@@ -758,7 +758,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Diego Cardenas</t>
+          <t xml:space="preserve">David Herrera </t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -776,26 +776,26 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>05:08:14</t>
+          <t>02:58:47</t>
         </is>
       </c>
       <c r="F2" s="1" t="n">
-        <v>91.90000000000001</v>
+        <v>51</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>16.22</v>
+        <v>7.78</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>00:01:05</t>
+          <t>00:00:06</t>
         </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -821,11 +821,11 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="R2" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 4:33PM CST</t>
+          <t>Jun 18 4:07PM CST</t>
         </is>
       </c>
       <c r="S2" s="1" t="n">
@@ -878,17 +878,17 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Luis Ibarra</t>
+          <t>Eduardo Hernandez</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>152</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
+          <t>TOYOTA HILUX</t>
         </is>
       </c>
       <c r="D3" s="7" t="n">
@@ -896,21 +896,21 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>03:26:59</t>
+          <t>02:09:22</t>
         </is>
       </c>
       <c r="F3" s="1" t="n">
-        <v>75.40000000000001</v>
+        <v>43.8</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>11.37</v>
+        <v>7.12</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:21</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
@@ -941,11 +941,11 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1" t="n">
-        <v>73.01000000000001</v>
+        <v>60</v>
       </c>
       <c r="R3" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 1:15PM CST</t>
+          <t>Jun 18 1:11PM CST</t>
         </is>
       </c>
       <c r="S3" s="1" t="n">
@@ -998,17 +998,17 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Jorge Tornero</t>
+          <t>Daniel Rocha</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>136</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>HINO 300</t>
+          <t>TOYOTA HILUX 2020</t>
         </is>
       </c>
       <c r="D4" s="7" t="n">
@@ -1016,26 +1016,26 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>02:44:34</t>
+          <t>02:27:43</t>
         </is>
       </c>
       <c r="F4" s="1" t="n">
-        <v>58.7</v>
+        <v>40.6</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>6.17</v>
+        <v>6.04</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="1" t="inlineStr">
         <is>
-          <t>00:00:34</t>
+          <t>00:00:37</t>
         </is>
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
@@ -1061,11 +1061,11 @@
         <v>0</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>75.01000000000001</v>
+        <v>60</v>
       </c>
       <c r="R4" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 9:11AM CST</t>
+          <t>Jun 18 1:45PM CST</t>
         </is>
       </c>
       <c r="S4" s="1" t="n">
@@ -1118,17 +1118,17 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cristian Estrada </t>
+          <t>Gerardo Aguillón</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>156</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t xml:space="preserve">TOYOTA HILUX </t>
         </is>
       </c>
       <c r="D5" s="7" t="n">
@@ -1136,21 +1136,21 @@
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>02:33:40</t>
+          <t>02:55:27</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>44.7</v>
+        <v>36.3</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>7.1</v>
+        <v>5.78</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J5" s="1" t="inlineStr">
@@ -1181,11 +1181,11 @@
         <v>0</v>
       </c>
       <c r="Q5" s="1" t="n">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="R5" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 12:36PM CST</t>
+          <t>Jun 18 2:27PM CST</t>
         </is>
       </c>
       <c r="S5" s="1" t="n">
@@ -1238,17 +1238,17 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Luis Galindo</t>
+          <t>Christian Aguilar</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>143</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH 2009</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D6" s="7" t="n">
@@ -1256,21 +1256,21 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>01:26:27</t>
+          <t>02:51:50</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>35.6</v>
+        <v>33.4</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>10.56</v>
+        <v>5.87</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J6" s="1" t="inlineStr">
@@ -1301,11 +1301,11 @@
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="R6" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 11:06AM CST</t>
+          <t>Jun 18 1:14PM CST</t>
         </is>
       </c>
       <c r="S6" s="1" t="n">
@@ -1358,17 +1358,17 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Hugo López</t>
+          <t xml:space="preserve">Cristian Estrada </t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>132</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D7" s="7" t="n">
@@ -1376,26 +1376,26 @@
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>02:37:19</t>
+          <t>01:52:08</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>33.7</v>
+        <v>33.4</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>6.86</v>
+        <v>4.63</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:31</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K7" s="1" t="inlineStr">
@@ -1421,11 +1421,11 @@
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>66.01000000000001</v>
+        <v>69.01000000000001</v>
       </c>
       <c r="R7" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 2:34PM CST</t>
+          <t>Jun 18 9:16AM CST</t>
         </is>
       </c>
       <c r="S7" s="1" t="n">
@@ -1478,17 +1478,17 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Armando Muñoz</t>
+          <t>Hugo López</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>153</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>HINO 300</t>
+          <t>TOYOTA HILUX</t>
         </is>
       </c>
       <c r="D8" s="7" t="n">
@@ -1496,26 +1496,26 @@
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>02:06:14</t>
+          <t>01:59:31</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>32.9</v>
+        <v>30.5</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>3.69</v>
+        <v>5.48</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J8" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K8" s="1" t="inlineStr">
@@ -1541,11 +1541,11 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="R8" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 3:03PM CST</t>
+          <t>Jun 18 8:03AM CST</t>
         </is>
       </c>
       <c r="S8" s="1" t="n">
@@ -1598,17 +1598,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Kevin De La O</t>
+          <t>Marcos Barbosa</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>147</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
+          <t>TOYOTA HILUX 2023</t>
         </is>
       </c>
       <c r="D9" s="7" t="n">
@@ -1616,26 +1616,26 @@
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>01:42:48</t>
+          <t>02:28:45</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>28.1</v>
+        <v>28.5</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>0</v>
+        <v>4.45</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K9" s="1" t="inlineStr">
@@ -1661,11 +1661,11 @@
         <v>0</v>
       </c>
       <c r="Q9" s="1" t="n">
-        <v>60.96</v>
+        <v>46</v>
       </c>
       <c r="R9" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 1:13PM CST</t>
+          <t>Jun 18 2:27PM CST</t>
         </is>
       </c>
       <c r="S9" s="1" t="n">
@@ -1718,17 +1718,17 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Christian Aguilar</t>
+          <t>Luis Ramirez</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>101</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>FORD F350 3MTS 2006</t>
         </is>
       </c>
       <c r="D10" s="7" t="n">
@@ -1736,26 +1736,26 @@
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>02:10:03</t>
+          <t>01:54:43</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>26.3</v>
+        <v>22.1</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>4.84</v>
+        <v>9.42</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J10" s="1" t="inlineStr">
         <is>
-          <t>00:00:27</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K10" s="1" t="inlineStr">
@@ -1781,11 +1781,11 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="n">
-        <v>66.01000000000001</v>
+        <v>54</v>
       </c>
       <c r="R10" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 1:54PM CST</t>
+          <t>Jun 18 3:05PM CST</t>
         </is>
       </c>
       <c r="S10" s="1" t="n">
@@ -1838,17 +1838,17 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Fernando Garcia</t>
+          <t>Luis Galindo</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>118</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>KENWORTH 2009</t>
         </is>
       </c>
       <c r="D11" s="7" t="n">
@@ -1856,14 +1856,14 @@
       </c>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>01:07:41</t>
+          <t>00:21:31</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>17.1</v>
+        <v>4.5</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0</v>
+        <v>3.85</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>0</v>
@@ -1901,11 +1901,11 @@
         <v>0</v>
       </c>
       <c r="Q11" s="1" t="n">
-        <v>50.92</v>
+        <v>40</v>
       </c>
       <c r="R11" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 11:30AM CST</t>
+          <t>Jun 18 2:54PM CST</t>
         </is>
       </c>
       <c r="S11" s="1" t="n">
@@ -1958,17 +1958,17 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Alberto Sesmas</t>
+          <t>Abraham Arana</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D12" s="7" t="n">
@@ -1976,14 +1976,14 @@
       </c>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>00:31:32</t>
+          <t>00:14:39</t>
         </is>
       </c>
       <c r="F12" s="1" t="n">
-        <v>5.7</v>
+        <v>4.3</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>2.65</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>0</v>
@@ -2021,11 +2021,11 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="n">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="R12" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 1:15PM CST</t>
+          <t>Jun 18 6:15PM CST</t>
         </is>
       </c>
       <c r="S12" s="1" t="n">
@@ -2078,17 +2078,17 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Martin Quezada</t>
+          <t>Alexis Alvarado</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>145</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>INTERNACIONAL</t>
+          <t>HINO 500</t>
         </is>
       </c>
       <c r="D13" s="7" t="n">
@@ -2096,21 +2096,21 @@
       </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>00:01:20</t>
+          <t>00:18:44</t>
         </is>
       </c>
       <c r="F13" s="1" t="n">
-        <v>0.1</v>
+        <v>4.1</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.79</v>
+        <v>1.43</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="J13" s="1" t="inlineStr">
@@ -2141,11 +2141,11 @@
         <v>0</v>
       </c>
       <c r="Q13" s="1" t="n">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="R13" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 6:14PM CST</t>
+          <t>Jun 18 2:14PM CST</t>
         </is>
       </c>
       <c r="S13" s="1" t="n">
@@ -2198,44 +2198,44 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Angel Cortez</t>
+          <t>Alejandro Lara</t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>110</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2018</t>
+          <t>WORKEN</t>
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>03:09:03</t>
+          <t>00:13:15</t>
         </is>
       </c>
       <c r="F14" s="1" t="n">
-        <v>103.2</v>
+        <v>4</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>13.58</v>
+        <v>2</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="inlineStr">
         <is>
-          <t>00:01:00</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J14" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K14" s="1" t="inlineStr">
@@ -2261,11 +2261,11 @@
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>80.01000000000001</v>
+        <v>47</v>
       </c>
       <c r="R14" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 10:30AM CST</t>
+          <t>Jun 18 12:59PM CST</t>
         </is>
       </c>
       <c r="S14" s="1" t="n">
@@ -2318,44 +2318,44 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Eduardo Hernandez</t>
+          <t xml:space="preserve">Compras </t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>120</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX</t>
+          <t>FORD RANGER 2011</t>
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>02:55:32</t>
+          <t>00:14:06</t>
         </is>
       </c>
       <c r="F15" s="1" t="n">
-        <v>54.6</v>
+        <v>1.4</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>8.59</v>
+        <v>0.38</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="inlineStr">
         <is>
-          <t>00:01:29</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J15" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K15" s="1" t="inlineStr">
@@ -2381,11 +2381,11 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>70.01000000000001</v>
+        <v>44</v>
       </c>
       <c r="R15" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 2:34PM CST</t>
+          <t>Jun 18 6:35PM CST</t>
         </is>
       </c>
       <c r="S15" s="1" t="n">
@@ -2438,17 +2438,17 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">David Herrera </t>
+          <t>Angel Cortez</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>133</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>FORD RANGER 2011</t>
+          <t>TOYOTA HILUX 2018</t>
         </is>
       </c>
       <c r="D16" s="7" t="n">
@@ -2456,26 +2456,26 @@
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>01:57:51</t>
+          <t>04:21:32</t>
         </is>
       </c>
       <c r="F16" s="1" t="n">
-        <v>37.2</v>
+        <v>108.3</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>5.18</v>
+        <v>15.77</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="inlineStr">
         <is>
-          <t>00:00:50</t>
+          <t>00:01:56</t>
         </is>
       </c>
       <c r="J16" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:00:45</t>
         </is>
       </c>
       <c r="K16" s="1" t="inlineStr">
@@ -2501,11 +2501,11 @@
         <v>0</v>
       </c>
       <c r="Q16" s="1" t="n">
-        <v>62</v>
+        <v>81.01000000000001</v>
       </c>
       <c r="R16" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 2:49PM CST</t>
+          <t>Jun 18 1:45PM CST</t>
         </is>
       </c>
       <c r="S16" s="1" t="n">
@@ -2558,17 +2558,17 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Daniel Rocha</t>
+          <t xml:space="preserve">Diego Cardenas </t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>142</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2020</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D17" s="7" t="n">
@@ -2576,26 +2576,26 @@
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>01:53:40</t>
+          <t>04:53:59</t>
         </is>
       </c>
       <c r="F17" s="1" t="n">
-        <v>35.5</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>6.44</v>
+        <v>15.87</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:02:35</t>
         </is>
       </c>
       <c r="J17" s="1" t="inlineStr">
         <is>
-          <t>00:00:49</t>
+          <t>00:01:15</t>
         </is>
       </c>
       <c r="K17" s="1" t="inlineStr">
@@ -2621,11 +2621,11 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="n">
-        <v>71.01000000000001</v>
+        <v>78.01000000000001</v>
       </c>
       <c r="R17" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 2:46PM CST</t>
+          <t>Jun 18 11:58AM CST</t>
         </is>
       </c>
       <c r="S17" s="1" t="n">
@@ -2678,17 +2678,17 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Miguel Zamora</t>
+          <t xml:space="preserve">Daniel Iñiguez </t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>141</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D18" s="7" t="n">
@@ -2696,26 +2696,26 @@
       </c>
       <c r="E18" s="1" t="inlineStr">
         <is>
-          <t>01:52:07</t>
+          <t>04:35:17</t>
         </is>
       </c>
       <c r="F18" s="1" t="n">
-        <v>32.5</v>
+        <v>89.8</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>0</v>
+        <v>12.09</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="inlineStr">
         <is>
-          <t>00:00:36</t>
+          <t>00:02:11</t>
         </is>
       </c>
       <c r="J18" s="1" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:00:51</t>
         </is>
       </c>
       <c r="K18" s="1" t="inlineStr">
@@ -2741,11 +2741,11 @@
         <v>0</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>68.06</v>
+        <v>70.01000000000001</v>
       </c>
       <c r="R18" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 3:45PM CST</t>
+          <t>Jun 18 2:33PM CST</t>
         </is>
       </c>
       <c r="S18" s="1" t="n">
@@ -2798,17 +2798,17 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Luis Ramirez</t>
+          <t>Alberto Sesmas</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>124</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>FORD F350 3MTS 2006</t>
+          <t>KENWORTH</t>
         </is>
       </c>
       <c r="D19" s="7" t="n">
@@ -2816,26 +2816,26 @@
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>01:18:11</t>
+          <t>02:32:08</t>
         </is>
       </c>
       <c r="F19" s="1" t="n">
-        <v>13.8</v>
+        <v>52.4</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>5.9</v>
+        <v>16.44</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="inlineStr">
         <is>
-          <t>00:00:12</t>
+          <t>00:01:25</t>
         </is>
       </c>
       <c r="J19" s="1" t="inlineStr">
         <is>
-          <t>00:00:26</t>
+          <t>00:00:48</t>
         </is>
       </c>
       <c r="K19" s="1" t="inlineStr">
@@ -2861,11 +2861,11 @@
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>67.01000000000001</v>
+        <v>79.01000000000001</v>
       </c>
       <c r="R19" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 11:11AM CST</t>
+          <t>Jun 18 9:05AM CST</t>
         </is>
       </c>
       <c r="S19" s="1" t="n">
@@ -2918,44 +2918,44 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Mario Ballinas</t>
+          <t>Alberto Sanchez</t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>154</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>VW DELIVERY 10.6</t>
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>01:45:25</t>
+          <t>00:44:39</t>
         </is>
       </c>
       <c r="F20" s="1" t="n">
-        <v>33.5</v>
+        <v>14.9</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>5.46</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="inlineStr">
         <is>
-          <t>00:00:59</t>
+          <t>00:00:29</t>
         </is>
       </c>
       <c r="J20" s="1" t="inlineStr">
         <is>
-          <t>00:00:39</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K20" s="1" t="inlineStr">
@@ -2981,11 +2981,11 @@
         <v>0</v>
       </c>
       <c r="Q20" s="1" t="n">
-        <v>78.01000000000001</v>
+        <v>71.86</v>
       </c>
       <c r="R20" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 1:32PM CST</t>
+          <t>Jun 18 4:30PM CST</t>
         </is>
       </c>
       <c r="S20" s="1" t="n">
@@ -3038,17 +3038,17 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Daniel Iñiguez</t>
+          <t>Miguel Guizar</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>150</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>Hino 300 2024</t>
         </is>
       </c>
       <c r="D21" s="7" t="n">
@@ -3056,26 +3056,26 @@
       </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>01:07:56</t>
+          <t>02:52:45</t>
         </is>
       </c>
       <c r="F21" s="1" t="n">
-        <v>27.6</v>
+        <v>73.8</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>3.42</v>
+        <v>7.86</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="inlineStr">
         <is>
-          <t>00:00:59</t>
+          <t>00:02:34</t>
         </is>
       </c>
       <c r="J21" s="1" t="inlineStr">
         <is>
-          <t>00:00:36</t>
+          <t>00:00:52</t>
         </is>
       </c>
       <c r="K21" s="1" t="inlineStr">
@@ -3101,11 +3101,11 @@
         <v>0</v>
       </c>
       <c r="Q21" s="1" t="n">
-        <v>77.01000000000001</v>
+        <v>73.01000000000001</v>
       </c>
       <c r="R21" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 2:39PM CST</t>
+          <t>Jun 18 5:00PM CST</t>
         </is>
       </c>
       <c r="S21" s="1" t="n">
@@ -3158,49 +3158,49 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Gerardo Aguillón</t>
+          <t xml:space="preserve">José Morales </t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>155</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t xml:space="preserve">TOYOTA HILUX </t>
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>04:25:48</t>
+          <t>02:21:22</t>
         </is>
       </c>
       <c r="F22" s="1" t="n">
-        <v>105.4</v>
+        <v>43.2</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>14.13</v>
+        <v>6.8</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="inlineStr">
         <is>
-          <t>00:04:33</t>
+          <t>00:00:38</t>
         </is>
       </c>
       <c r="J22" s="1" t="inlineStr">
         <is>
-          <t>00:02:19</t>
+          <t>00:00:43</t>
         </is>
       </c>
       <c r="K22" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:06</t>
         </is>
       </c>
       <c r="L22" s="1" t="inlineStr">
@@ -3221,11 +3221,11 @@
         <v>0</v>
       </c>
       <c r="Q22" s="1" t="n">
-        <v>84.01000000000001</v>
+        <v>71.01000000000001</v>
       </c>
       <c r="R22" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 12:25PM CST</t>
+          <t>Jun 18 2:14PM CST</t>
         </is>
       </c>
       <c r="S22" s="1" t="n">
@@ -3278,39 +3278,39 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>José Morales</t>
+          <t>Moises Martinez</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>149</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX 2024</t>
         </is>
       </c>
       <c r="D23" s="7" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>03:49:56</t>
+          <t>02:07:01</t>
         </is>
       </c>
       <c r="F23" s="1" t="n">
-        <v>75.90000000000001</v>
+        <v>41.4</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>9.66</v>
+        <v>7.27</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I23" s="1" t="inlineStr">
         <is>
-          <t>00:01:39</t>
+          <t>00:01:14</t>
         </is>
       </c>
       <c r="J23" s="1" t="inlineStr">
@@ -3320,7 +3320,7 @@
       </c>
       <c r="K23" s="1" t="inlineStr">
         <is>
-          <t>00:00:17</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L23" s="1" t="inlineStr">
@@ -3341,11 +3341,11 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>74.01000000000001</v>
+        <v>77.01000000000001</v>
       </c>
       <c r="R23" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 9:45AM CST</t>
+          <t>Jun 18 2:13PM CST</t>
         </is>
       </c>
       <c r="S23" s="1" t="n">
@@ -3398,49 +3398,49 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Moises Martinez</t>
+          <t>Mario Ballinas</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>144</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D24" s="7" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>02:14:46</t>
+          <t>02:27:01</t>
         </is>
       </c>
       <c r="F24" s="1" t="n">
-        <v>45.9</v>
+        <v>40</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>8.529999999999999</v>
+        <v>7.25</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I24" s="1" t="inlineStr">
         <is>
-          <t>00:00:51</t>
+          <t>00:00:22</t>
         </is>
       </c>
       <c r="J24" s="1" t="inlineStr">
         <is>
-          <t>00:00:52</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="K24" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:00:06</t>
         </is>
       </c>
       <c r="L24" s="1" t="inlineStr">
@@ -3461,11 +3461,11 @@
         <v>0</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>82.01000000000001</v>
+        <v>63</v>
       </c>
       <c r="R24" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 4:10PM CST</t>
+          <t>Jun 18 11:38AM CST</t>
         </is>
       </c>
       <c r="S24" s="1" t="n">
@@ -3518,12 +3518,12 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Daniel Mercado</t>
+          <t>Jonathan Alvarez</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>131</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr">
@@ -3532,35 +3532,35 @@
         </is>
       </c>
       <c r="D25" s="7" t="n">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>02:55:39</t>
+          <t>01:50:05</t>
         </is>
       </c>
       <c r="F25" s="1" t="n">
-        <v>62.3</v>
+        <v>29.3</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>9.76</v>
+        <v>4.73</v>
       </c>
       <c r="H25" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I25" s="1" t="inlineStr">
         <is>
-          <t>00:01:40</t>
+          <t>00:01:10</t>
         </is>
       </c>
       <c r="J25" s="1" t="inlineStr">
         <is>
-          <t>00:02:47</t>
+          <t>00:00:38</t>
         </is>
       </c>
       <c r="K25" s="1" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L25" s="1" t="inlineStr">
@@ -3581,11 +3581,11 @@
         <v>0</v>
       </c>
       <c r="Q25" s="1" t="n">
-        <v>81.01000000000001</v>
+        <v>67.01000000000001</v>
       </c>
       <c r="R25" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 10:45AM CST</t>
+          <t>Jun 18 2:29PM CST</t>
         </is>
       </c>
       <c r="S25" s="1" t="n">
@@ -3638,17 +3638,17 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Daniel Magallanes</t>
+          <t>Jorge Tornero</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>117</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>HINO 300</t>
         </is>
       </c>
       <c r="D26" s="7" t="n">
@@ -3656,36 +3656,36 @@
       </c>
       <c r="E26" s="1" t="inlineStr">
         <is>
-          <t>01:25:27</t>
+          <t>03:51:44</t>
         </is>
       </c>
       <c r="F26" s="1" t="n">
-        <v>29.7</v>
+        <v>78</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>2.67</v>
+        <v>8.15</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:01:31</t>
         </is>
       </c>
       <c r="J26" s="1" t="inlineStr">
         <is>
-          <t>00:00:29</t>
+          <t>00:01:03</t>
         </is>
       </c>
       <c r="K26" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:00:04</t>
         </is>
       </c>
       <c r="L26" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="M26" s="1" t="n">
@@ -3701,11 +3701,11 @@
         <v>0</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <v>74.01000000000001</v>
+        <v>76.01000000000001</v>
       </c>
       <c r="R26" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 11:29AM CST</t>
+          <t>Jun 18 10:22AM CST</t>
         </is>
       </c>
       <c r="S26" s="1" t="n">
@@ -3758,54 +3758,54 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>David Serrano</t>
+          <t>Fernando Ornelas</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>138</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
-        </is>
-      </c>
-      <c r="D27" s="8" t="n">
-        <v>89</v>
+          <t>TOYOTA HILUX 2020</t>
+        </is>
+      </c>
+      <c r="D27" s="7" t="n">
+        <v>95</v>
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
-          <t>04:25:02</t>
+          <t>03:15:49</t>
         </is>
       </c>
       <c r="F27" s="1" t="n">
-        <v>81.3</v>
+        <v>44.5</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>7.2</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I27" s="1" t="inlineStr">
         <is>
-          <t>00:01:16</t>
+          <t>00:00:39</t>
         </is>
       </c>
       <c r="J27" s="1" t="inlineStr">
         <is>
-          <t>00:01:48</t>
+          <t>00:00:28</t>
         </is>
       </c>
       <c r="K27" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:28</t>
         </is>
       </c>
       <c r="L27" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M27" s="1" t="n">
@@ -3821,11 +3821,11 @@
         <v>0</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <v>82.01000000000001</v>
+        <v>76.01000000000001</v>
       </c>
       <c r="R27" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 10:57AM CST</t>
+          <t>Jun 18 3:41PM CST</t>
         </is>
       </c>
       <c r="S27" s="1" t="n">
@@ -3878,12 +3878,12 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>Daniel Magallanes</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>127</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr">
@@ -3891,41 +3891,41 @@
           <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
-      <c r="D28" s="8" t="n">
-        <v>89</v>
+      <c r="D28" s="7" t="n">
+        <v>94</v>
       </c>
       <c r="E28" s="1" t="inlineStr">
         <is>
-          <t>03:00:17</t>
+          <t>01:21:24</t>
         </is>
       </c>
       <c r="F28" s="1" t="n">
-        <v>72.3</v>
+        <v>22.4</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>6.84</v>
+        <v>2.12</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I28" s="1" t="inlineStr">
         <is>
-          <t>00:03:16</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="J28" s="1" t="inlineStr">
         <is>
-          <t>00:03:27</t>
+          <t>00:01:02</t>
         </is>
       </c>
       <c r="K28" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="L28" s="1" t="inlineStr">
         <is>
-          <t>00:00:06</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M28" s="1" t="n">
@@ -3941,11 +3941,11 @@
         <v>0</v>
       </c>
       <c r="Q28" s="1" t="n">
-        <v>90.01000000000001</v>
+        <v>74.01000000000001</v>
       </c>
       <c r="R28" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 1:25PM CST</t>
+          <t>Jun 18 11:47AM CST</t>
         </is>
       </c>
       <c r="S28" s="1" t="n">
@@ -3998,49 +3998,49 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Alberto Sanchez</t>
+          <t>Daniel Mercado</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>130</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>VW DELIVERY 10.6</t>
-        </is>
-      </c>
-      <c r="D29" s="8" t="n">
-        <v>83</v>
+          <t>TOYOTA HILUX 2017</t>
+        </is>
+      </c>
+      <c r="D29" s="7" t="n">
+        <v>93</v>
       </c>
       <c r="E29" s="1" t="inlineStr">
         <is>
-          <t>00:44:48</t>
+          <t>04:12:39</t>
         </is>
       </c>
       <c r="F29" s="1" t="n">
-        <v>15.1</v>
+        <v>118.8</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>0</v>
+        <v>14.08</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I29" s="1" t="inlineStr">
         <is>
-          <t>00:00:33</t>
+          <t>00:03:18</t>
         </is>
       </c>
       <c r="J29" s="1" t="inlineStr">
         <is>
-          <t>00:00:32</t>
+          <t>00:02:51</t>
         </is>
       </c>
       <c r="K29" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:00:36</t>
         </is>
       </c>
       <c r="L29" s="1" t="inlineStr">
@@ -4061,11 +4061,11 @@
         <v>0</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>72.54000000000001</v>
+        <v>84.01000000000001</v>
       </c>
       <c r="R29" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 12:46PM CST</t>
+          <t>Jun 18 2:02PM CST</t>
         </is>
       </c>
       <c r="S29" s="1" t="n">
@@ -4118,54 +4118,54 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Francisco Marquez</t>
+          <t>Fernando Garcia</t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
-        </is>
-      </c>
-      <c r="D30" s="8" t="n">
-        <v>70</v>
+          <t>Volkswagen</t>
+        </is>
+      </c>
+      <c r="D30" s="7" t="n">
+        <v>91</v>
       </c>
       <c r="E30" s="1" t="inlineStr">
         <is>
-          <t>08:01:57</t>
+          <t>10:09:15</t>
         </is>
       </c>
       <c r="F30" s="1" t="n">
-        <v>380.1</v>
+        <v>407.2</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>117.49</v>
+        <v>0</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I30" s="1" t="inlineStr">
         <is>
-          <t>00:06:57</t>
+          <t>00:06:13</t>
         </is>
       </c>
       <c r="J30" s="1" t="inlineStr">
         <is>
-          <t>00:03:38</t>
+          <t>00:04:28</t>
         </is>
       </c>
       <c r="K30" s="1" t="inlineStr">
         <is>
-          <t>00:04:16</t>
+          <t>00:01:54</t>
         </is>
       </c>
       <c r="L30" s="1" t="inlineStr">
         <is>
-          <t>00:00:33</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="M30" s="1" t="n">
@@ -4175,17 +4175,17 @@
         <v>0</v>
       </c>
       <c r="O30" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P30" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q30" s="1" t="n">
-        <v>100.01</v>
+        <v>97.64</v>
       </c>
       <c r="R30" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 4:52AM CST</t>
+          <t>Jun 18 7:06AM CST</t>
         </is>
       </c>
       <c r="S30" s="1" t="n">
@@ -4238,74 +4238,74 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Alejandro Suarez</t>
+          <t>Armando Muñoz</t>
         </is>
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>102</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>HINO 500</t>
-        </is>
-      </c>
-      <c r="D31" s="9" t="n">
-        <v>69</v>
+          <t>HINO 300</t>
+        </is>
+      </c>
+      <c r="D31" s="8" t="n">
+        <v>79</v>
       </c>
       <c r="E31" s="1" t="inlineStr">
         <is>
-          <t>08:03:25</t>
+          <t>08:35:08</t>
         </is>
       </c>
       <c r="F31" s="1" t="n">
-        <v>374.1</v>
+        <v>359.9</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>89.20999999999999</v>
+        <v>47.57</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I31" s="1" t="inlineStr">
         <is>
-          <t>00:06:17</t>
+          <t>00:12:25</t>
         </is>
       </c>
       <c r="J31" s="1" t="inlineStr">
         <is>
-          <t>00:08:29</t>
+          <t>00:08:34</t>
         </is>
       </c>
       <c r="K31" s="1" t="inlineStr">
         <is>
-          <t>00:01:54</t>
+          <t>00:01:18</t>
         </is>
       </c>
       <c r="L31" s="1" t="inlineStr">
         <is>
-          <t>00:00:59</t>
+          <t>00:00:38</t>
         </is>
       </c>
       <c r="M31" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O31" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P31" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q31" s="1" t="n">
-        <v>108.01</v>
+        <v>91.01000000000001</v>
       </c>
       <c r="R31" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 6:12AM CST</t>
+          <t>Jun 18 6:02AM CST</t>
         </is>
       </c>
       <c r="S31" s="1" t="n">
@@ -4358,74 +4358,74 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Miguel Guizar</t>
+          <t>Francisco Marquez</t>
         </is>
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>135</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr">
         <is>
-          <t>Hino 300 2024</t>
-        </is>
-      </c>
-      <c r="D32" s="9" t="n">
-        <v>0</v>
+          <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
+        </is>
+      </c>
+      <c r="D32" s="8" t="n">
+        <v>79</v>
       </c>
       <c r="E32" s="1" t="inlineStr">
         <is>
-          <t>06:29:56</t>
+          <t>06:07:50</t>
         </is>
       </c>
       <c r="F32" s="1" t="n">
-        <v>345</v>
+        <v>323.1</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>37.88</v>
+        <v>85.5</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I32" s="1" t="inlineStr">
         <is>
-          <t>00:02:54</t>
+          <t>00:09:37</t>
         </is>
       </c>
       <c r="J32" s="1" t="inlineStr">
         <is>
-          <t>00:06:14</t>
+          <t>00:02:25</t>
         </is>
       </c>
       <c r="K32" s="1" t="inlineStr">
         <is>
-          <t>00:07:57</t>
+          <t>00:01:18</t>
         </is>
       </c>
       <c r="L32" s="1" t="inlineStr">
         <is>
-          <t>00:05:17</t>
+          <t>00:00:26</t>
         </is>
       </c>
       <c r="M32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N32" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P32" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="1" t="n">
-        <v>111.01</v>
+        <v>99.01000000000001</v>
       </c>
       <c r="R32" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 9:22AM CST</t>
+          <t>Jun 18 11:22AM CST</t>
         </is>
       </c>
       <c r="S32" s="1" t="n">
@@ -4478,62 +4478,62 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Marcos Barbosa</t>
+          <t>Alejandro Suarez</t>
         </is>
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>146</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2023</t>
+          <t>HINO 500</t>
         </is>
       </c>
       <c r="D33" s="9" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E33" s="1" t="inlineStr">
         <is>
-          <t>02:08:58</t>
+          <t>05:22:06</t>
         </is>
       </c>
       <c r="F33" s="1" t="n">
-        <v>24.7</v>
+        <v>331</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>4.2</v>
+        <v>74.56999999999999</v>
       </c>
       <c r="H33" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I33" s="1" t="inlineStr">
+        <is>
+          <t>00:04:02</t>
+        </is>
+      </c>
+      <c r="J33" s="1" t="inlineStr">
+        <is>
+          <t>00:07:58</t>
+        </is>
+      </c>
+      <c r="K33" s="1" t="inlineStr">
+        <is>
+          <t>00:04:01</t>
+        </is>
+      </c>
+      <c r="L33" s="1" t="inlineStr">
+        <is>
+          <t>00:01:03</t>
+        </is>
+      </c>
+      <c r="M33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I33" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="J33" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="K33" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="L33" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="M33" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="O33" s="1" t="n">
         <v>0</v>
       </c>
@@ -4541,11 +4541,11 @@
         <v>0</v>
       </c>
       <c r="Q33" s="1" t="n">
-        <v>48</v>
+        <v>107.01</v>
       </c>
       <c r="R33" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 1:29PM CST</t>
+          <t>Jun 18 12:41PM CST</t>
         </is>
       </c>
       <c r="S33" s="1" t="n">
@@ -4558,7 +4558,7 @@
         <v>0</v>
       </c>
       <c r="V33" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W33" s="1" t="n">
         <v>0</v>
@@ -4589,7 +4589,7 @@
         <v>0</v>
       </c>
       <c r="AE33" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AF33" s="1" t="n">
         <v>0</v>
@@ -4598,44 +4598,44 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Fernando Ornelas</t>
+          <t>Adrian Caro</t>
         </is>
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>116</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2020</t>
+          <t>VAN HYUNDAI</t>
         </is>
       </c>
       <c r="D34" s="9" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E34" s="1" t="inlineStr">
         <is>
-          <t>01:12:10</t>
+          <t>03:13:45</t>
         </is>
       </c>
       <c r="F34" s="1" t="n">
-        <v>22.1</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="G34" s="1" t="n">
-        <v>4.45</v>
+        <v>0</v>
       </c>
       <c r="H34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I34" s="1" t="inlineStr">
         <is>
-          <t>00:00:27</t>
+          <t>00:01:48</t>
         </is>
       </c>
       <c r="J34" s="1" t="inlineStr">
         <is>
-          <t>00:00:32</t>
+          <t>00:00:36</t>
         </is>
       </c>
       <c r="K34" s="1" t="inlineStr">
@@ -4661,11 +4661,11 @@
         <v>0</v>
       </c>
       <c r="Q34" s="1" t="n">
-        <v>66.01000000000001</v>
+        <v>85.77</v>
       </c>
       <c r="R34" s="1" t="inlineStr">
         <is>
-          <t>Jun 17 8:51AM CST</t>
+          <t>Jun 18 4:35PM CST</t>
         </is>
       </c>
       <c r="S34" s="1" t="n">
@@ -4718,808 +4718,922 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Alberto Jimenez</t>
+          <t>Martin Quezada</t>
         </is>
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>122</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
-        </is>
-      </c>
-      <c r="D35" s="10" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="E35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="F35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="G35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="H35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="I35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="J35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="K35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="L35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="M35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="N35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="O35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="P35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Q35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="R35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="S35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="T35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="U35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="V35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="W35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="X35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Y35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Z35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AA35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AB35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AC35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AD35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AE35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AF35" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
+          <t>INTERNACIONAL</t>
+        </is>
+      </c>
+      <c r="D35" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="inlineStr">
+        <is>
+          <t>07:23:03</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>469.4</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>132.51</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I35" s="1" t="inlineStr">
+        <is>
+          <t>00:02:04</t>
+        </is>
+      </c>
+      <c r="J35" s="1" t="inlineStr">
+        <is>
+          <t>00:05:45</t>
+        </is>
+      </c>
+      <c r="K35" s="1" t="inlineStr">
+        <is>
+          <t>00:00:28</t>
+        </is>
+      </c>
+      <c r="L35" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="M35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1" t="n">
+        <v>101.01</v>
+      </c>
+      <c r="R35" s="1" t="inlineStr">
+        <is>
+          <t>Jun 18 6:05AM CST</t>
+        </is>
+      </c>
+      <c r="S35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="1" t="inlineStr">
+        <is>
+          <t>Sin ruta.</t>
+        </is>
+      </c>
+      <c r="Z35" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="AA35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Alejandro Lara</t>
+          <t>Luis Ibarra</t>
         </is>
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>148</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr">
         <is>
-          <t>WORKEN</t>
-        </is>
-      </c>
-      <c r="D36" s="10" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="E36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="F36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="G36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="H36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="I36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="J36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="K36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="L36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="M36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="N36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="O36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="P36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Q36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="R36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="S36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="T36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="U36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="V36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="W36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="X36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Y36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Z36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AA36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AB36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AC36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AD36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AE36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AF36" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
+          <t>TOYOTA HILUX 2024</t>
+        </is>
+      </c>
+      <c r="D36" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="inlineStr">
+        <is>
+          <t>04:52:13</t>
+        </is>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>102.1</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="H36" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I36" s="1" t="inlineStr">
+        <is>
+          <t>00:00:33</t>
+        </is>
+      </c>
+      <c r="J36" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="K36" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="L36" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="M36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1" t="n">
+        <v>80.01000000000001</v>
+      </c>
+      <c r="R36" s="1" t="inlineStr">
+        <is>
+          <t>Jun 18 2:09PM CST</t>
+        </is>
+      </c>
+      <c r="S36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="1" t="inlineStr">
+        <is>
+          <t>Sin ruta.</t>
+        </is>
+      </c>
+      <c r="Z36" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="AA36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF36" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Alberto Compras</t>
+          <t>David Serrano</t>
         </is>
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>125</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr">
         <is>
-          <t>NISSAN 1993</t>
-        </is>
-      </c>
-      <c r="D37" s="10" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="E37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="F37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="G37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="H37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="I37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="J37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="K37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="L37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="M37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="N37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="O37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="P37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Q37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="R37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="S37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="T37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="U37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="V37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="W37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="X37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Y37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Z37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AA37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AB37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AC37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AD37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AE37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AF37" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
+          <t>TOYOTA HILUX 2017</t>
+        </is>
+      </c>
+      <c r="D37" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="inlineStr">
+        <is>
+          <t>01:59:26</t>
+        </is>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="G37" s="1" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1" t="inlineStr">
+        <is>
+          <t>00:01:34</t>
+        </is>
+      </c>
+      <c r="J37" s="1" t="inlineStr">
+        <is>
+          <t>00:01:28</t>
+        </is>
+      </c>
+      <c r="K37" s="1" t="inlineStr">
+        <is>
+          <t>00:00:11</t>
+        </is>
+      </c>
+      <c r="L37" s="1" t="inlineStr">
+        <is>
+          <t>00:00:10</t>
+        </is>
+      </c>
+      <c r="M37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="1" t="n">
+        <v>88.01000000000001</v>
+      </c>
+      <c r="R37" s="1" t="inlineStr">
+        <is>
+          <t>Jun 18 8:53AM CST</t>
+        </is>
+      </c>
+      <c r="S37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="1" t="inlineStr">
+        <is>
+          <t>Sin ruta.</t>
+        </is>
+      </c>
+      <c r="Z37" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="AA37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF37" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Abraham Arana</t>
+          <t>/</t>
         </is>
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>126</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
-        </is>
-      </c>
-      <c r="D38" s="10" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="E38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="F38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="G38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="H38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="I38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="J38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="K38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="L38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="M38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="N38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="O38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="P38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Q38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="R38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="S38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="T38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="U38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="V38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="W38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="X38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Y38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Z38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AA38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AB38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AC38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AD38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AE38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AF38" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
+          <t>TOYOTA HILUX 2017</t>
+        </is>
+      </c>
+      <c r="D38" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1" t="inlineStr">
+        <is>
+          <t>02:26:38</t>
+        </is>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="G38" s="1" t="n">
+        <v>4.87</v>
+      </c>
+      <c r="H38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" s="1" t="inlineStr">
+        <is>
+          <t>00:01:11</t>
+        </is>
+      </c>
+      <c r="J38" s="1" t="inlineStr">
+        <is>
+          <t>00:00:55</t>
+        </is>
+      </c>
+      <c r="K38" s="1" t="inlineStr">
+        <is>
+          <t>00:00:10</t>
+        </is>
+      </c>
+      <c r="L38" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="M38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="1" t="n">
+        <v>74.01000000000001</v>
+      </c>
+      <c r="R38" s="1" t="inlineStr">
+        <is>
+          <t>Jun 18 9:32AM CST</t>
+        </is>
+      </c>
+      <c r="S38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="U38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="1" t="inlineStr">
+        <is>
+          <t>Sin ruta.</t>
+        </is>
+      </c>
+      <c r="Z38" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="AA38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF38" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Alexis Alvarado</t>
+          <t>Miguel Zamora</t>
         </is>
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr">
         <is>
-          <t>HINO 500</t>
-        </is>
-      </c>
-      <c r="D39" s="10" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="E39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="F39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="G39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="H39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="I39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="J39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="K39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="L39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="M39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="N39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="O39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="P39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Q39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="R39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="S39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="T39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="U39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="V39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="W39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="X39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Y39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="Z39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AA39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AB39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AC39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AD39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AE39" s="11" t="inlineStr">
-        <is>
-          <t>Sin ruta</t>
-        </is>
-      </c>
-      <c r="AF39" s="11" t="inlineStr">
+          <t>Volkswagen</t>
+        </is>
+      </c>
+      <c r="D39" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1" t="inlineStr">
+        <is>
+          <t>01:18:07</t>
+        </is>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="G39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="1" t="inlineStr">
+        <is>
+          <t>00:01:30</t>
+        </is>
+      </c>
+      <c r="J39" s="1" t="inlineStr">
+        <is>
+          <t>00:04:24</t>
+        </is>
+      </c>
+      <c r="K39" s="1" t="inlineStr">
+        <is>
+          <t>00:02:29</t>
+        </is>
+      </c>
+      <c r="L39" s="1" t="inlineStr">
+        <is>
+          <t>00:00:22</t>
+        </is>
+      </c>
+      <c r="M39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="1" t="n">
+        <v>83.39</v>
+      </c>
+      <c r="R39" s="1" t="inlineStr">
+        <is>
+          <t>Jun 18 1:01PM CST</t>
+        </is>
+      </c>
+      <c r="S39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="U39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="V39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="1" t="inlineStr">
+        <is>
+          <t>Sin ruta.</t>
+        </is>
+      </c>
+      <c r="Z39" s="1" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="AA39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF39" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>Alberto Jimenez</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="inlineStr">
+        <is>
+          <t>VAN HYUNDAI</t>
+        </is>
+      </c>
+      <c r="D40" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF40" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>Alberto Compras</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="inlineStr">
+        <is>
+          <t>NISSAN 1993</t>
+        </is>
+      </c>
+      <c r="D41" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE41" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF41" s="11" t="inlineStr">
         <is>
           <t>Sin ruta</t>
         </is>

</xml_diff>

<commit_message>
Actualización automática: 2025-06-20 10:33
</commit_message>
<xml_diff>
--- a/seguridad/Informe_Diario_Unidades.xlsx
+++ b/seguridad/Informe_Diario_Unidades.xlsx
@@ -758,17 +758,17 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">David Herrera </t>
+          <t>Luis Ibarra</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>148</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2018</t>
+          <t>TOYOTA HILUX 2024</t>
         </is>
       </c>
       <c r="D2" s="7" t="n">
@@ -776,26 +776,26 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>02:58:47</t>
+          <t>04:49:46</t>
         </is>
       </c>
       <c r="F2" s="1" t="n">
-        <v>51</v>
+        <v>94.7</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>7.78</v>
+        <v>14.15</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>00:00:06</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:18</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -821,11 +821,11 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <v>56</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="R2" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 4:07PM CST</t>
+          <t>Jun 19 11:36AM CST</t>
         </is>
       </c>
       <c r="S2" s="1" t="n">
@@ -878,17 +878,17 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Eduardo Hernandez</t>
+          <t>Gerardo Aguillón</t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>156</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX</t>
+          <t xml:space="preserve">TOYOTA HILUX </t>
         </is>
       </c>
       <c r="D3" s="7" t="n">
@@ -896,21 +896,21 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>02:09:22</t>
+          <t>03:24:34</t>
         </is>
       </c>
       <c r="F3" s="1" t="n">
-        <v>43.8</v>
+        <v>38.3</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>7.12</v>
+        <v>6.46</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
@@ -941,11 +941,11 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="R3" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 1:11PM CST</t>
+          <t>Jun 19 2:18PM CST</t>
         </is>
       </c>
       <c r="S3" s="1" t="n">
@@ -998,17 +998,17 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Daniel Rocha</t>
+          <t>Eduardo Hernandez</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>152</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2020</t>
+          <t>TOYOTA HILUX</t>
         </is>
       </c>
       <c r="D4" s="7" t="n">
@@ -1016,26 +1016,26 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>02:27:43</t>
+          <t>02:05:32</t>
         </is>
       </c>
       <c r="F4" s="1" t="n">
-        <v>40.6</v>
+        <v>36.9</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>6.04</v>
+        <v>5.81</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="1" t="inlineStr">
         <is>
-          <t>00:00:37</t>
+          <t>00:00:21</t>
         </is>
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
@@ -1061,11 +1061,11 @@
         <v>0</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R4" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 1:45PM CST</t>
+          <t>Jun 19 1:05PM CST</t>
         </is>
       </c>
       <c r="S4" s="1" t="n">
@@ -1118,17 +1118,17 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Gerardo Aguillón</t>
+          <t>Christian Aguilar</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>143</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">TOYOTA HILUX </t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D5" s="7" t="n">
@@ -1136,26 +1136,26 @@
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>02:55:27</t>
+          <t>02:36:53</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>36.3</v>
+        <v>34.9</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>5.78</v>
+        <v>6.28</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:31</t>
         </is>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr">
@@ -1181,11 +1181,11 @@
         <v>0</v>
       </c>
       <c r="Q5" s="1" t="n">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="R5" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 2:27PM CST</t>
+          <t>Jun 19 2:24PM CST</t>
         </is>
       </c>
       <c r="S5" s="1" t="n">
@@ -1238,17 +1238,17 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Christian Aguilar</t>
+          <t>Marcos Barbosa</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>147</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX 2023</t>
         </is>
       </c>
       <c r="D6" s="7" t="n">
@@ -1256,14 +1256,14 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>02:51:50</t>
+          <t>01:56:30</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>33.4</v>
+        <v>22.1</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>5.87</v>
+        <v>3.96</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>0</v>
@@ -1301,11 +1301,11 @@
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="n">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="R6" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 1:14PM CST</t>
+          <t>Jun 19 3:00PM CST</t>
         </is>
       </c>
       <c r="S6" s="1" t="n">
@@ -1358,17 +1358,17 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cristian Estrada </t>
+          <t>Luis Ramirez</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>101</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>FORD F350 3MTS 2006</t>
         </is>
       </c>
       <c r="D7" s="7" t="n">
@@ -1376,21 +1376,21 @@
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>01:52:08</t>
+          <t>01:43:54</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>33.4</v>
+        <v>16.6</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>4.63</v>
+        <v>7.59</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>00:00:31</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
@@ -1421,11 +1421,11 @@
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>69.01000000000001</v>
+        <v>58</v>
       </c>
       <c r="R7" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 9:16AM CST</t>
+          <t>Jun 19 2:38PM CST</t>
         </is>
       </c>
       <c r="S7" s="1" t="n">
@@ -1478,17 +1478,17 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Hugo López</t>
+          <t xml:space="preserve">Compras </t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>120</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX</t>
+          <t>FORD RANGER 2011</t>
         </is>
       </c>
       <c r="D8" s="7" t="n">
@@ -1496,21 +1496,21 @@
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>01:59:31</t>
+          <t>00:39:10</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>30.5</v>
+        <v>5.8</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>5.48</v>
+        <v>1.51</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:06</t>
         </is>
       </c>
       <c r="J8" s="1" t="inlineStr">
@@ -1541,11 +1541,11 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="R8" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 8:03AM CST</t>
+          <t>Jun 19 1:28PM CST</t>
         </is>
       </c>
       <c r="S8" s="1" t="n">
@@ -1598,17 +1598,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Marcos Barbosa</t>
+          <t>Alberto Sesmas</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>124</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2023</t>
+          <t>KENWORTH</t>
         </is>
       </c>
       <c r="D9" s="7" t="n">
@@ -1616,21 +1616,21 @@
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>02:28:45</t>
+          <t>00:17:50</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>28.5</v>
+        <v>4.2</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>4.45</v>
+        <v>2.34</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J9" s="1" t="inlineStr">
@@ -1661,11 +1661,11 @@
         <v>0</v>
       </c>
       <c r="Q9" s="1" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="R9" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 2:27PM CST</t>
+          <t>Jun 19 4:20PM CST</t>
         </is>
       </c>
       <c r="S9" s="1" t="n">
@@ -1718,17 +1718,17 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Luis Ramirez</t>
+          <t>Alejandro Lara</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>110</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>FORD F350 3MTS 2006</t>
+          <t>WORKEN</t>
         </is>
       </c>
       <c r="D10" s="7" t="n">
@@ -1736,14 +1736,14 @@
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>01:54:43</t>
+          <t>00:01:21</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>22.1</v>
+        <v>0.2</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>9.42</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>0</v>
@@ -1781,11 +1781,11 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="n">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="R10" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 3:05PM CST</t>
+          <t>Jun 19 6:48PM CST</t>
         </is>
       </c>
       <c r="S10" s="1" t="n">
@@ -1838,49 +1838,49 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Luis Galindo</t>
+          <t>Jorge Tornero</t>
         </is>
       </c>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>117</t>
         </is>
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH 2009</t>
+          <t>HINO 300</t>
         </is>
       </c>
       <c r="D11" s="7" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>00:21:31</t>
+          <t>04:23:54</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>4.5</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>3.85</v>
+        <v>8.92</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:58</t>
         </is>
       </c>
       <c r="J11" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:12</t>
         </is>
       </c>
       <c r="K11" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:04</t>
         </is>
       </c>
       <c r="L11" s="1" t="inlineStr">
@@ -1901,11 +1901,11 @@
         <v>0</v>
       </c>
       <c r="Q11" s="1" t="n">
-        <v>40</v>
+        <v>85.01000000000001</v>
       </c>
       <c r="R11" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 2:54PM CST</t>
+          <t>Jun 19 12:39PM CST</t>
         </is>
       </c>
       <c r="S11" s="1" t="n">
@@ -1958,44 +1958,44 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Abraham Arana</t>
+          <t xml:space="preserve">Cristian Estrada </t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>132</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D12" s="7" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>00:14:39</t>
+          <t>04:15:37</t>
         </is>
       </c>
       <c r="F12" s="1" t="n">
-        <v>4.3</v>
+        <v>80.2</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.8100000000000001</v>
+        <v>11.42</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I12" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:01:17</t>
         </is>
       </c>
       <c r="J12" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:01:21</t>
         </is>
       </c>
       <c r="K12" s="1" t="inlineStr">
@@ -2021,11 +2021,11 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="n">
-        <v>52</v>
+        <v>87.01000000000001</v>
       </c>
       <c r="R12" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 6:15PM CST</t>
+          <t>Jun 19 1:24PM CST</t>
         </is>
       </c>
       <c r="S12" s="1" t="n">
@@ -2078,51 +2078,51 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Alexis Alvarado</t>
+          <t xml:space="preserve">Daniel Iñiguez </t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>141</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>HINO 500</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D13" s="7" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>00:18:44</t>
+          <t>03:15:32</t>
         </is>
       </c>
       <c r="F13" s="1" t="n">
-        <v>4.1</v>
+        <v>65</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>1.43</v>
+        <v>9.77</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="inlineStr">
         <is>
+          <t>00:00:52</t>
+        </is>
+      </c>
+      <c r="J13" s="1" t="inlineStr">
+        <is>
+          <t>00:00:21</t>
+        </is>
+      </c>
+      <c r="K13" s="1" t="inlineStr">
+        <is>
           <t>00:00:05</t>
         </is>
       </c>
-      <c r="J13" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="K13" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
       <c r="L13" s="1" t="inlineStr">
         <is>
           <t>00:00:00</t>
@@ -2141,11 +2141,11 @@
         <v>0</v>
       </c>
       <c r="Q13" s="1" t="n">
-        <v>58</v>
+        <v>70.01000000000001</v>
       </c>
       <c r="R13" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 2:14PM CST</t>
+          <t>Jun 19 9:22AM CST</t>
         </is>
       </c>
       <c r="S13" s="1" t="n">
@@ -2198,44 +2198,44 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Alejandro Lara</t>
+          <t xml:space="preserve">José Morales </t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>155</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>WORKEN</t>
+          <t xml:space="preserve">TOYOTA HILUX </t>
         </is>
       </c>
       <c r="D14" s="7" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>00:13:15</t>
+          <t>03:03:30</t>
         </is>
       </c>
       <c r="F14" s="1" t="n">
-        <v>4</v>
+        <v>56.5</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>2</v>
+        <v>8.51</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:48</t>
         </is>
       </c>
       <c r="J14" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="K14" s="1" t="inlineStr">
@@ -2261,11 +2261,11 @@
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>47</v>
+        <v>73.01000000000001</v>
       </c>
       <c r="R14" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 12:59PM CST</t>
+          <t>Jun 19 1:47PM CST</t>
         </is>
       </c>
       <c r="S14" s="1" t="n">
@@ -2318,44 +2318,44 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Compras </t>
+          <t>Daniel Magallanes</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>127</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>FORD RANGER 2011</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>00:14:06</t>
+          <t>03:17:57</t>
         </is>
       </c>
       <c r="F15" s="1" t="n">
-        <v>1.4</v>
+        <v>54.4</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>0.38</v>
+        <v>4.85</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:44</t>
         </is>
       </c>
       <c r="J15" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="K15" s="1" t="inlineStr">
@@ -2381,11 +2381,11 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>44</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="R15" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 6:35PM CST</t>
+          <t>Jun 19 10:50AM CST</t>
         </is>
       </c>
       <c r="S15" s="1" t="n">
@@ -2438,12 +2438,12 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Angel Cortez</t>
+          <t xml:space="preserve">David Herrera </t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>134</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
@@ -2456,21 +2456,21 @@
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>04:21:32</t>
+          <t>02:18:20</t>
         </is>
       </c>
       <c r="F16" s="1" t="n">
-        <v>108.3</v>
+        <v>42.5</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>15.77</v>
+        <v>6.49</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="inlineStr">
         <is>
-          <t>00:01:56</t>
+          <t>00:00:22</t>
         </is>
       </c>
       <c r="J16" s="1" t="inlineStr">
@@ -2501,11 +2501,11 @@
         <v>0</v>
       </c>
       <c r="Q16" s="1" t="n">
-        <v>81.01000000000001</v>
+        <v>64</v>
       </c>
       <c r="R16" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 1:45PM CST</t>
+          <t>Jun 19 4:06PM CST</t>
         </is>
       </c>
       <c r="S16" s="1" t="n">
@@ -2558,49 +2558,49 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Diego Cardenas </t>
+          <t>Fernando Ornelas</t>
         </is>
       </c>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>138</t>
         </is>
       </c>
       <c r="C17" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX 2020</t>
         </is>
       </c>
       <c r="D17" s="7" t="n">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>04:53:59</t>
+          <t>03:03:50</t>
         </is>
       </c>
       <c r="F17" s="1" t="n">
-        <v>95.09999999999999</v>
+        <v>55.7</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>15.87</v>
+        <v>8.970000000000001</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>00:02:35</t>
+          <t>00:01:12</t>
         </is>
       </c>
       <c r="J17" s="1" t="inlineStr">
         <is>
-          <t>00:01:15</t>
+          <t>00:00:28</t>
         </is>
       </c>
       <c r="K17" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="L17" s="1" t="inlineStr">
@@ -2621,11 +2621,11 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="n">
-        <v>78.01000000000001</v>
+        <v>85.01000000000001</v>
       </c>
       <c r="R17" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 11:58AM CST</t>
+          <t>Jun 19 2:27PM CST</t>
         </is>
       </c>
       <c r="S17" s="1" t="n">
@@ -2678,49 +2678,49 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daniel Iñiguez </t>
+          <t>Daniel Mercado</t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>130</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D18" s="7" t="n">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E18" s="1" t="inlineStr">
         <is>
-          <t>04:35:17</t>
+          <t>03:07:35</t>
         </is>
       </c>
       <c r="F18" s="1" t="n">
-        <v>89.8</v>
+        <v>53.2</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>12.09</v>
+        <v>8.07</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="inlineStr">
         <is>
-          <t>00:02:11</t>
+          <t>00:01:03</t>
         </is>
       </c>
       <c r="J18" s="1" t="inlineStr">
         <is>
-          <t>00:00:51</t>
+          <t>00:01:46</t>
         </is>
       </c>
       <c r="K18" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="L18" s="1" t="inlineStr">
@@ -2741,11 +2741,11 @@
         <v>0</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>70.01000000000001</v>
+        <v>74.01000000000001</v>
       </c>
       <c r="R18" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 2:33PM CST</t>
+          <t>Jun 19 11:49AM CST</t>
         </is>
       </c>
       <c r="S18" s="1" t="n">
@@ -2798,54 +2798,54 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Alberto Sesmas</t>
+          <t>Alberto Sanchez</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>154</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH</t>
+          <t>VW DELIVERY 10.6</t>
         </is>
       </c>
       <c r="D19" s="7" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>02:32:08</t>
+          <t>08:09:16</t>
         </is>
       </c>
       <c r="F19" s="1" t="n">
-        <v>52.4</v>
+        <v>344.5</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>16.44</v>
+        <v>0</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="inlineStr">
         <is>
-          <t>00:01:25</t>
+          <t>00:05:22</t>
         </is>
       </c>
       <c r="J19" s="1" t="inlineStr">
         <is>
-          <t>00:00:48</t>
+          <t>00:05:47</t>
         </is>
       </c>
       <c r="K19" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:06</t>
         </is>
       </c>
       <c r="L19" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="M19" s="1" t="n">
@@ -2861,11 +2861,11 @@
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>79.01000000000001</v>
+        <v>94.77</v>
       </c>
       <c r="R19" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 9:05AM CST</t>
+          <t>Jun 19 6:27AM CST</t>
         </is>
       </c>
       <c r="S19" s="1" t="n">
@@ -2918,49 +2918,49 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Alberto Sanchez</t>
+          <t xml:space="preserve">Diego Cardenas </t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>142</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
         <is>
-          <t>VW DELIVERY 10.6</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>00:44:39</t>
+          <t>04:26:39</t>
         </is>
       </c>
       <c r="F20" s="1" t="n">
-        <v>14.9</v>
+        <v>95.59999999999999</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>0</v>
+        <v>14.13</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="inlineStr">
         <is>
-          <t>00:00:29</t>
+          <t>00:01:30</t>
         </is>
       </c>
       <c r="J20" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:37</t>
         </is>
       </c>
       <c r="K20" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:42</t>
         </is>
       </c>
       <c r="L20" s="1" t="inlineStr">
@@ -2981,11 +2981,11 @@
         <v>0</v>
       </c>
       <c r="Q20" s="1" t="n">
-        <v>71.86</v>
+        <v>81.01000000000001</v>
       </c>
       <c r="R20" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 4:30PM CST</t>
+          <t>Jun 19 2:23PM CST</t>
         </is>
       </c>
       <c r="S20" s="1" t="n">
@@ -3038,49 +3038,49 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Miguel Guizar</t>
+          <t>Alejandro Suarez</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>146</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>Hino 300 2024</t>
+          <t>HINO 500</t>
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>02:52:45</t>
+          <t>02:01:02</t>
         </is>
       </c>
       <c r="F21" s="1" t="n">
-        <v>73.8</v>
+        <v>41.4</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>7.86</v>
+        <v>11.46</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="inlineStr">
         <is>
-          <t>00:02:34</t>
+          <t>00:01:19</t>
         </is>
       </c>
       <c r="J21" s="1" t="inlineStr">
         <is>
-          <t>00:00:52</t>
+          <t>00:00:32</t>
         </is>
       </c>
       <c r="K21" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:15</t>
         </is>
       </c>
       <c r="L21" s="1" t="inlineStr">
@@ -3101,11 +3101,11 @@
         <v>0</v>
       </c>
       <c r="Q21" s="1" t="n">
-        <v>73.01000000000001</v>
+        <v>76.01000000000001</v>
       </c>
       <c r="R21" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 5:00PM CST</t>
+          <t>Jun 19 2:46PM CST</t>
         </is>
       </c>
       <c r="S21" s="1" t="n">
@@ -3158,54 +3158,54 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">José Morales </t>
+          <t>Miguel Guizar</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>150</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">TOYOTA HILUX </t>
+          <t>Hino 300 2024</t>
         </is>
       </c>
       <c r="D22" s="7" t="n">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>02:21:22</t>
+          <t>06:16:47</t>
         </is>
       </c>
       <c r="F22" s="1" t="n">
-        <v>43.2</v>
+        <v>314</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>6.8</v>
+        <v>35.38</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="inlineStr">
         <is>
-          <t>00:00:38</t>
+          <t>00:03:01</t>
         </is>
       </c>
       <c r="J22" s="1" t="inlineStr">
         <is>
-          <t>00:00:43</t>
+          <t>00:01:44</t>
         </is>
       </c>
       <c r="K22" s="1" t="inlineStr">
         <is>
-          <t>00:00:06</t>
+          <t>00:01:01</t>
         </is>
       </c>
       <c r="L22" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="M22" s="1" t="n">
@@ -3221,11 +3221,11 @@
         <v>0</v>
       </c>
       <c r="Q22" s="1" t="n">
-        <v>71.01000000000001</v>
+        <v>102.01</v>
       </c>
       <c r="R22" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 2:14PM CST</t>
+          <t>Jun 19 4:24PM CST</t>
         </is>
       </c>
       <c r="S22" s="1" t="n">
@@ -3278,44 +3278,44 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Moises Martinez</t>
+          <t>Angel Cortez</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>133</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
-        </is>
-      </c>
-      <c r="D23" s="7" t="n">
-        <v>98</v>
+          <t>TOYOTA HILUX 2018</t>
+        </is>
+      </c>
+      <c r="D23" s="8" t="n">
+        <v>86</v>
       </c>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>02:07:01</t>
+          <t>03:38:02</t>
         </is>
       </c>
       <c r="F23" s="1" t="n">
-        <v>41.4</v>
+        <v>85.3</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>7.27</v>
+        <v>12.51</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I23" s="1" t="inlineStr">
         <is>
-          <t>00:01:14</t>
+          <t>00:00:57</t>
         </is>
       </c>
       <c r="J23" s="1" t="inlineStr">
         <is>
-          <t>00:01:04</t>
+          <t>00:00:23</t>
         </is>
       </c>
       <c r="K23" s="1" t="inlineStr">
@@ -3325,7 +3325,7 @@
       </c>
       <c r="L23" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="M23" s="1" t="n">
@@ -3341,11 +3341,11 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>77.01000000000001</v>
+        <v>82.01000000000001</v>
       </c>
       <c r="R23" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 2:13PM CST</t>
+          <t>Jun 19 12:33PM CST</t>
         </is>
       </c>
       <c r="S23" s="1" t="n">
@@ -3398,54 +3398,54 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Mario Ballinas</t>
+          <t>Jonathan Alvarez</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>131</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
-        </is>
-      </c>
-      <c r="D24" s="7" t="n">
-        <v>98</v>
+          <t>TOYOTA HILUX 2017</t>
+        </is>
+      </c>
+      <c r="D24" s="8" t="n">
+        <v>86</v>
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>02:27:01</t>
+          <t>02:31:30</t>
         </is>
       </c>
       <c r="F24" s="1" t="n">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>7.25</v>
+        <v>6.87</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I24" s="1" t="inlineStr">
         <is>
-          <t>00:00:22</t>
+          <t>00:00:15</t>
         </is>
       </c>
       <c r="J24" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="K24" s="1" t="inlineStr">
         <is>
-          <t>00:00:06</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="L24" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:09</t>
         </is>
       </c>
       <c r="M24" s="1" t="n">
@@ -3461,11 +3461,11 @@
         <v>0</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>63</v>
+        <v>75.01000000000001</v>
       </c>
       <c r="R24" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 11:38AM CST</t>
+          <t>Jun 19 1:38PM CST</t>
         </is>
       </c>
       <c r="S24" s="1" t="n">
@@ -3518,12 +3518,12 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Jonathan Alvarez</t>
+          <t>/</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>126</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr">
@@ -3531,41 +3531,41 @@
           <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
-      <c r="D25" s="7" t="n">
-        <v>98</v>
+      <c r="D25" s="8" t="n">
+        <v>85</v>
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>01:50:05</t>
+          <t>02:27:06</t>
         </is>
       </c>
       <c r="F25" s="1" t="n">
-        <v>29.3</v>
+        <v>53</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>4.73</v>
+        <v>5.01</v>
       </c>
       <c r="H25" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I25" s="1" t="inlineStr">
         <is>
-          <t>00:01:10</t>
+          <t>00:04:05</t>
         </is>
       </c>
       <c r="J25" s="1" t="inlineStr">
         <is>
-          <t>00:00:38</t>
+          <t>00:01:44</t>
         </is>
       </c>
       <c r="K25" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:27</t>
         </is>
       </c>
       <c r="L25" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:04</t>
         </is>
       </c>
       <c r="M25" s="1" t="n">
@@ -3581,11 +3581,11 @@
         <v>0</v>
       </c>
       <c r="Q25" s="1" t="n">
-        <v>67.01000000000001</v>
+        <v>86.01000000000001</v>
       </c>
       <c r="R25" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 2:29PM CST</t>
+          <t>Jun 19 10:27AM CST</t>
         </is>
       </c>
       <c r="S25" s="1" t="n">
@@ -3638,54 +3638,54 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Jorge Tornero</t>
+          <t>Hugo López</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>153</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>HINO 300</t>
-        </is>
-      </c>
-      <c r="D26" s="7" t="n">
-        <v>95</v>
+          <t>TOYOTA HILUX</t>
+        </is>
+      </c>
+      <c r="D26" s="8" t="n">
+        <v>81</v>
       </c>
       <c r="E26" s="1" t="inlineStr">
         <is>
-          <t>03:51:44</t>
+          <t>02:52:39</t>
         </is>
       </c>
       <c r="F26" s="1" t="n">
-        <v>78</v>
+        <v>52.5</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>8.15</v>
+        <v>8.76</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="1" t="inlineStr">
         <is>
-          <t>00:01:31</t>
+          <t>00:00:41</t>
         </is>
       </c>
       <c r="J26" s="1" t="inlineStr">
         <is>
-          <t>00:01:03</t>
+          <t>00:00:17</t>
         </is>
       </c>
       <c r="K26" s="1" t="inlineStr">
         <is>
-          <t>00:00:04</t>
+          <t>00:00:17</t>
         </is>
       </c>
       <c r="L26" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:15</t>
         </is>
       </c>
       <c r="M26" s="1" t="n">
@@ -3701,11 +3701,11 @@
         <v>0</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <v>76.01000000000001</v>
+        <v>74.01000000000001</v>
       </c>
       <c r="R26" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 10:22AM CST</t>
+          <t>Jun 19 2:47PM CST</t>
         </is>
       </c>
       <c r="S26" s="1" t="n">
@@ -3758,61 +3758,61 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Fernando Ornelas</t>
+          <t>Mario Ballinas</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>144</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2020</t>
-        </is>
-      </c>
-      <c r="D27" s="7" t="n">
-        <v>95</v>
+          <t>TOYOTA HILUX 2021</t>
+        </is>
+      </c>
+      <c r="D27" s="8" t="n">
+        <v>73</v>
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
-          <t>03:15:49</t>
+          <t>05:37:33</t>
         </is>
       </c>
       <c r="F27" s="1" t="n">
-        <v>44.5</v>
+        <v>289.1</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>8.289999999999999</v>
+        <v>33.83</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I27" s="1" t="inlineStr">
         <is>
-          <t>00:00:39</t>
+          <t>00:07:24</t>
         </is>
       </c>
       <c r="J27" s="1" t="inlineStr">
         <is>
+          <t>00:05:34</t>
+        </is>
+      </c>
+      <c r="K27" s="1" t="inlineStr">
+        <is>
+          <t>00:01:35</t>
+        </is>
+      </c>
+      <c r="L27" s="1" t="inlineStr">
+        <is>
           <t>00:00:28</t>
         </is>
       </c>
-      <c r="K27" s="1" t="inlineStr">
-        <is>
-          <t>00:00:28</t>
-        </is>
-      </c>
-      <c r="L27" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
       <c r="M27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O27" s="1" t="n">
         <v>0</v>
@@ -3821,11 +3821,11 @@
         <v>0</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <v>76.01000000000001</v>
+        <v>104.01</v>
       </c>
       <c r="R27" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 3:41PM CST</t>
+          <t>Jun 19 4:02PM CST</t>
         </is>
       </c>
       <c r="S27" s="1" t="n">
@@ -3878,61 +3878,61 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Daniel Magallanes</t>
+          <t>Luis Galindo</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>118</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
-        </is>
-      </c>
-      <c r="D28" s="7" t="n">
-        <v>94</v>
+          <t>KENWORTH 2009</t>
+        </is>
+      </c>
+      <c r="D28" s="8" t="n">
+        <v>71</v>
       </c>
       <c r="E28" s="1" t="inlineStr">
         <is>
-          <t>01:21:24</t>
+          <t>07:07:06</t>
         </is>
       </c>
       <c r="F28" s="1" t="n">
-        <v>22.4</v>
+        <v>365.5</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>2.12</v>
+        <v>95.56</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I28" s="1" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:06:12</t>
         </is>
       </c>
       <c r="J28" s="1" t="inlineStr">
         <is>
-          <t>00:01:02</t>
+          <t>00:12:45</t>
         </is>
       </c>
       <c r="K28" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:05:10</t>
         </is>
       </c>
       <c r="L28" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:06</t>
         </is>
       </c>
       <c r="M28" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N28" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O28" s="1" t="n">
         <v>0</v>
@@ -3941,11 +3941,11 @@
         <v>0</v>
       </c>
       <c r="Q28" s="1" t="n">
-        <v>74.01000000000001</v>
+        <v>97.01000000000001</v>
       </c>
       <c r="R28" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 11:47AM CST</t>
+          <t>Jun 19 6:06AM CST</t>
         </is>
       </c>
       <c r="S28" s="1" t="n">
@@ -3998,54 +3998,54 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Daniel Mercado</t>
+          <t>Miguel Zamora</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
-        </is>
-      </c>
-      <c r="D29" s="7" t="n">
-        <v>93</v>
+          <t>Volkswagen</t>
+        </is>
+      </c>
+      <c r="D29" s="9" t="n">
+        <v>67</v>
       </c>
       <c r="E29" s="1" t="inlineStr">
         <is>
-          <t>04:12:39</t>
+          <t>05:51:25</t>
         </is>
       </c>
       <c r="F29" s="1" t="n">
-        <v>118.8</v>
+        <v>166.5</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>14.08</v>
+        <v>0</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I29" s="1" t="inlineStr">
         <is>
-          <t>00:03:18</t>
+          <t>00:03:28</t>
         </is>
       </c>
       <c r="J29" s="1" t="inlineStr">
         <is>
-          <t>00:02:51</t>
+          <t>00:03:23</t>
         </is>
       </c>
       <c r="K29" s="1" t="inlineStr">
         <is>
-          <t>00:00:36</t>
+          <t>00:03:27</t>
         </is>
       </c>
       <c r="L29" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:27</t>
         </is>
       </c>
       <c r="M29" s="1" t="n">
@@ -4061,11 +4061,11 @@
         <v>0</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>84.01000000000001</v>
+        <v>94.34</v>
       </c>
       <c r="R29" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 2:02PM CST</t>
+          <t>Jun 19 2:46PM CST</t>
         </is>
       </c>
       <c r="S29" s="1" t="n">
@@ -4131,16 +4131,16 @@
           <t>Volkswagen</t>
         </is>
       </c>
-      <c r="D30" s="7" t="n">
-        <v>91</v>
+      <c r="D30" s="9" t="n">
+        <v>63</v>
       </c>
       <c r="E30" s="1" t="inlineStr">
         <is>
-          <t>10:09:15</t>
+          <t>06:44:23</t>
         </is>
       </c>
       <c r="F30" s="1" t="n">
-        <v>407.2</v>
+        <v>355.3</v>
       </c>
       <c r="G30" s="1" t="n">
         <v>0</v>
@@ -4150,22 +4150,22 @@
       </c>
       <c r="I30" s="1" t="inlineStr">
         <is>
-          <t>00:06:13</t>
+          <t>00:04:45</t>
         </is>
       </c>
       <c r="J30" s="1" t="inlineStr">
         <is>
-          <t>00:04:28</t>
+          <t>00:03:33</t>
         </is>
       </c>
       <c r="K30" s="1" t="inlineStr">
         <is>
-          <t>00:01:54</t>
+          <t>00:01:00</t>
         </is>
       </c>
       <c r="L30" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:01:14</t>
         </is>
       </c>
       <c r="M30" s="1" t="n">
@@ -4181,11 +4181,11 @@
         <v>0</v>
       </c>
       <c r="Q30" s="1" t="n">
-        <v>97.64</v>
+        <v>99.81999999999999</v>
       </c>
       <c r="R30" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 7:06AM CST</t>
+          <t>Jun 19 7:15PM CST</t>
         </is>
       </c>
       <c r="S30" s="1" t="n">
@@ -4251,41 +4251,41 @@
           <t>HINO 300</t>
         </is>
       </c>
-      <c r="D31" s="8" t="n">
-        <v>79</v>
+      <c r="D31" s="9" t="n">
+        <v>60</v>
       </c>
       <c r="E31" s="1" t="inlineStr">
         <is>
-          <t>08:35:08</t>
+          <t>04:57:16</t>
         </is>
       </c>
       <c r="F31" s="1" t="n">
-        <v>359.9</v>
+        <v>266.5</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>47.57</v>
+        <v>28.36</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I31" s="1" t="inlineStr">
         <is>
-          <t>00:12:25</t>
+          <t>00:03:45</t>
         </is>
       </c>
       <c r="J31" s="1" t="inlineStr">
         <is>
-          <t>00:08:34</t>
+          <t>00:07:33</t>
         </is>
       </c>
       <c r="K31" s="1" t="inlineStr">
         <is>
-          <t>00:01:18</t>
+          <t>00:05:55</t>
         </is>
       </c>
       <c r="L31" s="1" t="inlineStr">
         <is>
-          <t>00:00:38</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M31" s="1" t="n">
@@ -4295,17 +4295,17 @@
         <v>1</v>
       </c>
       <c r="O31" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P31" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q31" s="1" t="n">
-        <v>91.01000000000001</v>
+        <v>93.01000000000001</v>
       </c>
       <c r="R31" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 6:02AM CST</t>
+          <t>Jun 19 1:31PM CST</t>
         </is>
       </c>
       <c r="S31" s="1" t="n">
@@ -4358,54 +4358,54 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Francisco Marquez</t>
+          <t>Martin Quezada</t>
         </is>
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>122</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr">
         <is>
-          <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
-        </is>
-      </c>
-      <c r="D32" s="8" t="n">
-        <v>79</v>
+          <t>INTERNACIONAL</t>
+        </is>
+      </c>
+      <c r="D32" s="9" t="n">
+        <v>25</v>
       </c>
       <c r="E32" s="1" t="inlineStr">
         <is>
-          <t>06:07:50</t>
+          <t>00:41:37</t>
         </is>
       </c>
       <c r="F32" s="1" t="n">
-        <v>323.1</v>
+        <v>11.4</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>85.5</v>
+        <v>6.24</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I32" s="1" t="inlineStr">
         <is>
-          <t>00:09:37</t>
+          <t>00:00:31</t>
         </is>
       </c>
       <c r="J32" s="1" t="inlineStr">
         <is>
-          <t>00:02:25</t>
+          <t>00:00:47</t>
         </is>
       </c>
       <c r="K32" s="1" t="inlineStr">
         <is>
-          <t>00:01:18</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="L32" s="1" t="inlineStr">
         <is>
-          <t>00:00:26</t>
+          <t>00:00:15</t>
         </is>
       </c>
       <c r="M32" s="1" t="n">
@@ -4421,11 +4421,11 @@
         <v>0</v>
       </c>
       <c r="Q32" s="1" t="n">
-        <v>99.01000000000001</v>
+        <v>74.01000000000001</v>
       </c>
       <c r="R32" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 11:22AM CST</t>
+          <t>Jun 19 1:18PM CST</t>
         </is>
       </c>
       <c r="S32" s="1" t="n">
@@ -4478,61 +4478,61 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Alejandro Suarez</t>
+          <t>Abraham Arana</t>
         </is>
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr">
         <is>
-          <t>HINO 500</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D33" s="9" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E33" s="1" t="inlineStr">
         <is>
-          <t>05:22:06</t>
+          <t>03:13:57</t>
         </is>
       </c>
       <c r="F33" s="1" t="n">
-        <v>331</v>
+        <v>52</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>74.56999999999999</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H33" s="1" t="n">
         <v>2</v>
       </c>
       <c r="I33" s="1" t="inlineStr">
         <is>
-          <t>00:04:02</t>
+          <t>00:01:09</t>
         </is>
       </c>
       <c r="J33" s="1" t="inlineStr">
         <is>
-          <t>00:07:58</t>
+          <t>00:00:26</t>
         </is>
       </c>
       <c r="K33" s="1" t="inlineStr">
         <is>
-          <t>00:04:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L33" s="1" t="inlineStr">
         <is>
-          <t>00:01:03</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="M33" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N33" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33" s="1" t="n">
         <v>0</v>
@@ -4541,11 +4541,11 @@
         <v>0</v>
       </c>
       <c r="Q33" s="1" t="n">
-        <v>107.01</v>
+        <v>75.01000000000001</v>
       </c>
       <c r="R33" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 12:41PM CST</t>
+          <t>Jun 19 1:21PM CST</t>
         </is>
       </c>
       <c r="S33" s="1" t="n">
@@ -4558,7 +4558,7 @@
         <v>0</v>
       </c>
       <c r="V33" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W33" s="1" t="n">
         <v>0</v>
@@ -4589,7 +4589,7 @@
         <v>0</v>
       </c>
       <c r="AE33" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AF33" s="1" t="n">
         <v>0</v>
@@ -4598,54 +4598,54 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Adrian Caro</t>
+          <t>David Serrano</t>
         </is>
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>125</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D34" s="9" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="E34" s="1" t="inlineStr">
         <is>
-          <t>03:13:45</t>
+          <t>01:45:02</t>
         </is>
       </c>
       <c r="F34" s="1" t="n">
-        <v>67.90000000000001</v>
+        <v>33.6</v>
       </c>
       <c r="G34" s="1" t="n">
-        <v>0</v>
+        <v>3.34</v>
       </c>
       <c r="H34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I34" s="1" t="inlineStr">
         <is>
-          <t>00:01:48</t>
+          <t>00:00:27</t>
         </is>
       </c>
       <c r="J34" s="1" t="inlineStr">
         <is>
-          <t>00:00:36</t>
+          <t>00:01:04</t>
         </is>
       </c>
       <c r="K34" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:44</t>
         </is>
       </c>
       <c r="L34" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:15</t>
         </is>
       </c>
       <c r="M34" s="1" t="n">
@@ -4661,24 +4661,24 @@
         <v>0</v>
       </c>
       <c r="Q34" s="1" t="n">
-        <v>85.77</v>
+        <v>92.01000000000001</v>
       </c>
       <c r="R34" s="1" t="inlineStr">
         <is>
-          <t>Jun 18 4:35PM CST</t>
+          <t>Jun 19 12:02PM CST</t>
         </is>
       </c>
       <c r="S34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T34" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="V34" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W34" s="1" t="n">
         <v>0</v>
@@ -4718,617 +4718,827 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Martin Quezada</t>
+          <t>Alberto Jimenez</t>
         </is>
       </c>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>103</t>
         </is>
       </c>
       <c r="C35" s="1" t="inlineStr">
         <is>
-          <t>INTERNACIONAL</t>
-        </is>
-      </c>
-      <c r="D35" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" s="1" t="inlineStr">
-        <is>
-          <t>07:23:03</t>
-        </is>
-      </c>
-      <c r="F35" s="1" t="n">
-        <v>469.4</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>132.51</v>
-      </c>
-      <c r="H35" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I35" s="1" t="inlineStr">
-        <is>
-          <t>00:02:04</t>
-        </is>
-      </c>
-      <c r="J35" s="1" t="inlineStr">
-        <is>
-          <t>00:05:45</t>
-        </is>
-      </c>
-      <c r="K35" s="1" t="inlineStr">
-        <is>
-          <t>00:00:28</t>
-        </is>
-      </c>
-      <c r="L35" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="M35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="O35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="1" t="n">
-        <v>101.01</v>
-      </c>
-      <c r="R35" s="1" t="inlineStr">
-        <is>
-          <t>Jun 18 6:05AM CST</t>
-        </is>
-      </c>
-      <c r="S35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y35" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z35" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD35" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AE35" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF35" s="1" t="n">
-        <v>0</v>
+          <t>VAN HYUNDAI</t>
+        </is>
+      </c>
+      <c r="D35" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF35" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Luis Ibarra</t>
+          <t>Alberto Compras</t>
         </is>
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>115</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
-        </is>
-      </c>
-      <c r="D36" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="1" t="inlineStr">
-        <is>
-          <t>04:52:13</t>
-        </is>
-      </c>
-      <c r="F36" s="1" t="n">
-        <v>102.1</v>
-      </c>
-      <c r="G36" s="1" t="n">
-        <v>15.3</v>
-      </c>
-      <c r="H36" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I36" s="1" t="inlineStr">
-        <is>
-          <t>00:00:33</t>
-        </is>
-      </c>
-      <c r="J36" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="K36" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="L36" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="M36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="1" t="n">
-        <v>80.01000000000001</v>
-      </c>
-      <c r="R36" s="1" t="inlineStr">
-        <is>
-          <t>Jun 18 2:09PM CST</t>
-        </is>
-      </c>
-      <c r="S36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z36" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD36" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE36" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF36" s="1" t="n">
-        <v>0</v>
+          <t>NISSAN 1993</t>
+        </is>
+      </c>
+      <c r="D36" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF36" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>David Serrano</t>
+          <t>Adrian Caro</t>
         </is>
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>116</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
-        </is>
-      </c>
-      <c r="D37" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" s="1" t="inlineStr">
-        <is>
-          <t>01:59:26</t>
-        </is>
-      </c>
-      <c r="F37" s="1" t="n">
-        <v>41.5</v>
-      </c>
-      <c r="G37" s="1" t="n">
-        <v>3.72</v>
-      </c>
-      <c r="H37" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I37" s="1" t="inlineStr">
-        <is>
-          <t>00:01:34</t>
-        </is>
-      </c>
-      <c r="J37" s="1" t="inlineStr">
-        <is>
-          <t>00:01:28</t>
-        </is>
-      </c>
-      <c r="K37" s="1" t="inlineStr">
-        <is>
-          <t>00:00:11</t>
-        </is>
-      </c>
-      <c r="L37" s="1" t="inlineStr">
-        <is>
-          <t>00:00:10</t>
-        </is>
-      </c>
-      <c r="M37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="1" t="n">
-        <v>88.01000000000001</v>
-      </c>
-      <c r="R37" s="1" t="inlineStr">
-        <is>
-          <t>Jun 18 8:53AM CST</t>
-        </is>
-      </c>
-      <c r="S37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T37" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="U37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y37" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z37" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF37" s="1" t="n">
-        <v>0</v>
+          <t>VAN HYUNDAI</t>
+        </is>
+      </c>
+      <c r="D37" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>Daniel Rocha</t>
         </is>
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>136</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
-        </is>
-      </c>
-      <c r="D38" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" s="1" t="inlineStr">
-        <is>
-          <t>02:26:38</t>
-        </is>
-      </c>
-      <c r="F38" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="G38" s="1" t="n">
-        <v>4.87</v>
-      </c>
-      <c r="H38" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I38" s="1" t="inlineStr">
-        <is>
-          <t>00:01:11</t>
-        </is>
-      </c>
-      <c r="J38" s="1" t="inlineStr">
-        <is>
-          <t>00:00:55</t>
-        </is>
-      </c>
-      <c r="K38" s="1" t="inlineStr">
-        <is>
-          <t>00:00:10</t>
-        </is>
-      </c>
-      <c r="L38" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="M38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="1" t="n">
-        <v>74.01000000000001</v>
-      </c>
-      <c r="R38" s="1" t="inlineStr">
-        <is>
-          <t>Jun 18 9:32AM CST</t>
-        </is>
-      </c>
-      <c r="S38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T38" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="U38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y38" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z38" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF38" s="1" t="n">
-        <v>0</v>
+          <t>TOYOTA HILUX 2020</t>
+        </is>
+      </c>
+      <c r="D38" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF38" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Miguel Zamora</t>
+          <t>Francisco Marquez</t>
         </is>
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>135</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
-        </is>
-      </c>
-      <c r="D39" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="1" t="inlineStr">
-        <is>
-          <t>01:18:07</t>
-        </is>
-      </c>
-      <c r="F39" s="1" t="n">
-        <v>33.5</v>
-      </c>
-      <c r="G39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" s="1" t="inlineStr">
-        <is>
-          <t>00:01:30</t>
-        </is>
-      </c>
-      <c r="J39" s="1" t="inlineStr">
-        <is>
-          <t>00:04:24</t>
-        </is>
-      </c>
-      <c r="K39" s="1" t="inlineStr">
-        <is>
-          <t>00:02:29</t>
-        </is>
-      </c>
-      <c r="L39" s="1" t="inlineStr">
-        <is>
-          <t>00:00:22</t>
-        </is>
-      </c>
-      <c r="M39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="1" t="n">
-        <v>83.39</v>
-      </c>
-      <c r="R39" s="1" t="inlineStr">
-        <is>
-          <t>Jun 18 1:01PM CST</t>
-        </is>
-      </c>
-      <c r="S39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="U39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y39" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z39" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE39" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF39" s="1" t="n">
-        <v>0</v>
+          <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
+        </is>
+      </c>
+      <c r="D39" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF39" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Alberto Jimenez</t>
+          <t>Alexis Alvarado</t>
         </is>
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>145</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
+          <t>HINO 500</t>
         </is>
       </c>
       <c r="D40" s="10" t="inlineStr">
@@ -5480,17 +5690,17 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Alberto Compras</t>
+          <t>Moises Martinez</t>
         </is>
       </c>
       <c r="B41" s="1" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>149</t>
         </is>
       </c>
       <c r="C41" s="1" t="inlineStr">
         <is>
-          <t>NISSAN 1993</t>
+          <t>TOYOTA HILUX 2024</t>
         </is>
       </c>
       <c r="D41" s="10" t="inlineStr">

</xml_diff>

<commit_message>
Actualización automática: 2025-07-17 10:37
</commit_message>
<xml_diff>
--- a/seguridad/Informe_Diario_Unidades.xlsx
+++ b/seguridad/Informe_Diario_Unidades.xlsx
@@ -776,26 +776,26 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>03:58:42</t>
+          <t>05:40:14</t>
         </is>
       </c>
       <c r="F2" s="1" t="n">
-        <v>67.3</v>
+        <v>121.7</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>10.95</v>
+        <v>17.69</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>00:00:28</t>
+          <t>00:00:47</t>
         </is>
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:12</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="R2" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 11:49AM CST</t>
+          <t>Jul 16 1:42PM CST</t>
         </is>
       </c>
       <c r="S2" s="1" t="n">
@@ -878,17 +878,17 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Luis Ibarra</t>
+          <t xml:space="preserve">CRISTIAN ESTRADA </t>
         </is>
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>155</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
+          <t xml:space="preserve">TOYOTA HILUX </t>
         </is>
       </c>
       <c r="D3" s="7" t="n">
@@ -896,26 +896,26 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>04:03:34</t>
+          <t>03:10:51</t>
         </is>
       </c>
       <c r="F3" s="1" t="n">
-        <v>66.3</v>
+        <v>54.9</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>10.69</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:42</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="K3" s="1" t="inlineStr">
@@ -941,11 +941,11 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1" t="n">
-        <v>60</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="R3" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 10:01AM CST</t>
+          <t>Jul 16 3:58PM CST</t>
         </is>
       </c>
       <c r="S3" s="1" t="n">
@@ -998,17 +998,17 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Alejandro Suarez</t>
+          <t>CARLOS JIMENEZ</t>
         </is>
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>146</t>
+          <t>140</t>
         </is>
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>HINO 500</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D4" s="7" t="n">
@@ -1016,26 +1016,26 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>02:32:32</t>
+          <t>03:19:24</t>
         </is>
       </c>
       <c r="F4" s="1" t="n">
-        <v>48.2</v>
+        <v>47.4</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>12.1</v>
+        <v>8.42</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I4" s="1" t="inlineStr">
         <is>
-          <t>00:00:20</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="J4" s="1" t="inlineStr">
         <is>
-          <t>00:00:23</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="K4" s="1" t="inlineStr">
@@ -1061,11 +1061,11 @@
         <v>0</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <v>66.01000000000001</v>
+        <v>60</v>
       </c>
       <c r="R4" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 9:21AM CST</t>
+          <t>Jul 16 3:22PM CST</t>
         </is>
       </c>
       <c r="S4" s="1" t="n">
@@ -1118,17 +1118,17 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Gerardo Aguillón</t>
+          <t>Adrian Caro</t>
         </is>
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>116</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">TOYOTA HILUX </t>
+          <t>VAN HYUNDAI</t>
         </is>
       </c>
       <c r="D5" s="7" t="n">
@@ -1136,26 +1136,26 @@
       </c>
       <c r="E5" s="1" t="inlineStr">
         <is>
-          <t>02:52:00</t>
+          <t>02:46:25</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>34.5</v>
+        <v>46.4</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>6.26</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:23</t>
         </is>
       </c>
       <c r="J5" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="K5" s="1" t="inlineStr">
@@ -1181,11 +1181,11 @@
         <v>0</v>
       </c>
       <c r="Q5" s="1" t="n">
-        <v>54</v>
+        <v>74.04000000000001</v>
       </c>
       <c r="R5" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 2:56PM CST</t>
+          <t>Jul 16 5:06PM CST</t>
         </is>
       </c>
       <c r="S5" s="1" t="n">
@@ -1238,17 +1238,17 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Hugo López</t>
+          <t>Marcos Barbosa</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>153</t>
+          <t>147</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX</t>
+          <t>TOYOTA HILUX 2023</t>
         </is>
       </c>
       <c r="D6" s="7" t="n">
@@ -1256,26 +1256,26 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>02:23:57</t>
+          <t>02:34:12</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>33.1</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>6.64</v>
+        <v>5.89</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr">
@@ -1301,11 +1301,11 @@
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="n">
-        <v>57</v>
+        <v>71.01000000000001</v>
       </c>
       <c r="R6" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 12:45PM CST</t>
+          <t>Jul 16 1:40PM CST</t>
         </is>
       </c>
       <c r="S6" s="1" t="n">
@@ -1358,17 +1358,17 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Christian Aguilar</t>
+          <t>Gerardo Aguillón</t>
         </is>
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>143</t>
+          <t>156</t>
         </is>
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t xml:space="preserve">TOYOTA HILUX </t>
         </is>
       </c>
       <c r="D7" s="7" t="n">
@@ -1376,21 +1376,21 @@
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>02:38:31</t>
+          <t>02:44:16</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>32.8</v>
+        <v>30.7</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>5.94</v>
+        <v>4.84</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
@@ -1421,11 +1421,11 @@
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="R7" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 1:58PM CST</t>
+          <t>Jul 16 8:06AM CST</t>
         </is>
       </c>
       <c r="S7" s="1" t="n">
@@ -1478,17 +1478,17 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Marcos Barbosa</t>
+          <t>Miguel Zamora</t>
         </is>
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>147</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2023</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="D8" s="7" t="n">
@@ -1496,26 +1496,26 @@
       </c>
       <c r="E8" s="1" t="inlineStr">
         <is>
-          <t>02:27:34</t>
+          <t>01:56:51</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>30</v>
+        <v>28.6</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>5.24</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="1" t="inlineStr">
         <is>
-          <t>00:00:17</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J8" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K8" s="1" t="inlineStr">
@@ -1541,11 +1541,11 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <v>53</v>
+        <v>59.13</v>
       </c>
       <c r="R8" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 2:04PM CST</t>
+          <t>Jul 16 10:07AM CST</t>
         </is>
       </c>
       <c r="S8" s="1" t="n">
@@ -1598,17 +1598,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Daniel Magallanes</t>
+          <t>Christian Aguilar</t>
         </is>
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>143</t>
         </is>
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D9" s="7" t="n">
@@ -1616,26 +1616,26 @@
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>02:09:55</t>
+          <t>02:23:55</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>28.9</v>
+        <v>28.1</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>2.79</v>
+        <v>5.38</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:21</t>
         </is>
       </c>
       <c r="J9" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="K9" s="1" t="inlineStr">
@@ -1661,11 +1661,11 @@
         <v>0</v>
       </c>
       <c r="Q9" s="1" t="n">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="R9" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 6:21PM CST</t>
+          <t>Jul 16 3:02PM CST</t>
         </is>
       </c>
       <c r="S9" s="1" t="n">
@@ -1718,17 +1718,17 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Miguel Zamora</t>
+          <t>Francisco Marquez</t>
         </is>
       </c>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>135</t>
         </is>
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
         </is>
       </c>
       <c r="D10" s="7" t="n">
@@ -1736,21 +1736,21 @@
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>01:48:25</t>
+          <t>00:58:47</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>24.5</v>
+        <v>25.7</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="J10" s="1" t="inlineStr">
@@ -1781,11 +1781,11 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="n">
-        <v>58.36</v>
+        <v>70.01000000000001</v>
       </c>
       <c r="R10" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 3:41PM CST</t>
+          <t>Jul 16 11:54AM CST</t>
         </is>
       </c>
       <c r="S10" s="1" t="n">
@@ -1856,21 +1856,21 @@
       </c>
       <c r="E11" s="1" t="inlineStr">
         <is>
-          <t>01:36:58</t>
+          <t>01:49:24</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>18.3</v>
+        <v>17.5</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>8.81</v>
+        <v>9.380000000000001</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="J11" s="1" t="inlineStr">
@@ -1901,11 +1901,11 @@
         <v>0</v>
       </c>
       <c r="Q11" s="1" t="n">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="R11" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 3:11PM CST</t>
+          <t>Jul 16 3:30PM CST</t>
         </is>
       </c>
       <c r="S11" s="1" t="n">
@@ -1958,17 +1958,17 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Diego Cardenas </t>
+          <t>Fernando Garcia</t>
         </is>
       </c>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>151</t>
         </is>
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="D12" s="7" t="n">
@@ -1976,14 +1976,14 @@
       </c>
       <c r="E12" s="1" t="inlineStr">
         <is>
-          <t>00:07:13</t>
+          <t>01:01:25</t>
         </is>
       </c>
       <c r="F12" s="1" t="n">
-        <v>2.2</v>
+        <v>14.1</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>1.56</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>0</v>
@@ -2021,11 +2021,11 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="n">
-        <v>40</v>
+        <v>53.01</v>
       </c>
       <c r="R12" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 4:56PM CST</t>
+          <t>Jul 16 5:34PM CST</t>
         </is>
       </c>
       <c r="S12" s="1" t="n">
@@ -2078,17 +2078,17 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Fernando Garcia</t>
+          <t>Daniel Magallanes</t>
         </is>
       </c>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>127</t>
         </is>
       </c>
       <c r="C13" s="1" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D13" s="7" t="n">
@@ -2096,14 +2096,14 @@
       </c>
       <c r="E13" s="1" t="inlineStr">
         <is>
-          <t>00:08:16</t>
+          <t>01:00:25</t>
         </is>
       </c>
       <c r="F13" s="1" t="n">
-        <v>0.8</v>
+        <v>12.8</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0</v>
+        <v>1.56</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>0</v>
@@ -2141,11 +2141,11 @@
         <v>0</v>
       </c>
       <c r="Q13" s="1" t="n">
-        <v>26.74</v>
+        <v>52</v>
       </c>
       <c r="R13" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 5:07PM CST</t>
+          <t>Jul 16 6:40PM CST</t>
         </is>
       </c>
       <c r="S13" s="1" t="n">
@@ -2198,17 +2198,17 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Luis Galindo</t>
+          <t xml:space="preserve">Diego Cardenas </t>
         </is>
       </c>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>142</t>
         </is>
       </c>
       <c r="C14" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH 2009</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D14" s="7" t="n">
@@ -2216,14 +2216,14 @@
       </c>
       <c r="E14" s="1" t="inlineStr">
         <is>
-          <t>00:02:21</t>
+          <t>00:34:52</t>
         </is>
       </c>
       <c r="F14" s="1" t="n">
-        <v>0.3</v>
+        <v>9.1</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.9</v>
+        <v>1.71</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>0</v>
@@ -2261,11 +2261,11 @@
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="R14" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 7:12AM CST</t>
+          <t>Jul 16 9:07AM CST</t>
         </is>
       </c>
       <c r="S14" s="1" t="n">
@@ -2318,44 +2318,44 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Angel Cortez</t>
+          <t>Alejandro Lara</t>
         </is>
       </c>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>110</t>
         </is>
       </c>
       <c r="C15" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2018</t>
+          <t>WORKEN</t>
         </is>
       </c>
       <c r="D15" s="7" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="inlineStr">
         <is>
-          <t>03:21:26</t>
+          <t>00:02:38</t>
         </is>
       </c>
       <c r="F15" s="1" t="n">
-        <v>89.3</v>
+        <v>0.7</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>13.43</v>
+        <v>1</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="inlineStr">
         <is>
-          <t>00:00:37</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="J15" s="1" t="inlineStr">
         <is>
-          <t>00:00:43</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="K15" s="1" t="inlineStr">
@@ -2381,11 +2381,11 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <v>85.01000000000001</v>
+        <v>42.78</v>
       </c>
       <c r="R15" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 10:08AM CST</t>
+          <t>Jul 16 11:10AM CST</t>
         </is>
       </c>
       <c r="S15" s="1" t="n">
@@ -2438,17 +2438,17 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>JOSE MORALES</t>
+          <t>Luis Ibarra</t>
         </is>
       </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>148</t>
         </is>
       </c>
       <c r="C16" s="1" t="inlineStr">
         <is>
-          <t>Hino 300 2024</t>
+          <t>TOYOTA HILUX 2024</t>
         </is>
       </c>
       <c r="D16" s="7" t="n">
@@ -2456,31 +2456,31 @@
       </c>
       <c r="E16" s="1" t="inlineStr">
         <is>
-          <t>03:51:52</t>
+          <t>05:16:03</t>
         </is>
       </c>
       <c r="F16" s="1" t="n">
-        <v>83.5</v>
+        <v>106.9</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>8.880000000000001</v>
+        <v>16.53</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="inlineStr">
         <is>
-          <t>00:01:44</t>
+          <t>00:00:06</t>
         </is>
       </c>
       <c r="J16" s="1" t="inlineStr">
         <is>
-          <t>00:00:47</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="K16" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="L16" s="1" t="inlineStr">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="R16" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 1:30PM CST</t>
+          <t>Jul 16 2:04PM CST</t>
         </is>
       </c>
       <c r="S16" s="1" t="n">
@@ -2576,26 +2576,26 @@
       </c>
       <c r="E17" s="1" t="inlineStr">
         <is>
-          <t>03:07:47</t>
+          <t>03:28:15</t>
         </is>
       </c>
       <c r="F17" s="1" t="n">
-        <v>60.6</v>
+        <v>55.1</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>9.57</v>
+        <v>9.82</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="1" t="inlineStr">
         <is>
-          <t>00:00:55</t>
+          <t>00:00:36</t>
         </is>
       </c>
       <c r="J17" s="1" t="inlineStr">
         <is>
-          <t>00:00:26</t>
+          <t>00:00:31</t>
         </is>
       </c>
       <c r="K17" s="1" t="inlineStr">
@@ -2621,11 +2621,11 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="n">
-        <v>74.01000000000001</v>
+        <v>58</v>
       </c>
       <c r="R17" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 2:02PM CST</t>
+          <t>Jul 16 2:53PM CST</t>
         </is>
       </c>
       <c r="S17" s="1" t="n">
@@ -2678,17 +2678,17 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Armando Muñoz</t>
+          <t>ANTONIO GODOY</t>
         </is>
       </c>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>103</t>
         </is>
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>HINO 300</t>
+          <t>VAN HYUNDAI</t>
         </is>
       </c>
       <c r="D18" s="7" t="n">
@@ -2696,26 +2696,26 @@
       </c>
       <c r="E18" s="1" t="inlineStr">
         <is>
-          <t>02:51:06</t>
+          <t>02:15:44</t>
         </is>
       </c>
       <c r="F18" s="1" t="n">
-        <v>59.5</v>
+        <v>50.2</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>6.36</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="inlineStr">
         <is>
-          <t>00:00:46</t>
+          <t>00:01:13</t>
         </is>
       </c>
       <c r="J18" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:00:15</t>
         </is>
       </c>
       <c r="K18" s="1" t="inlineStr">
@@ -2741,11 +2741,11 @@
         <v>0</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <v>67.01000000000001</v>
+        <v>75.43000000000001</v>
       </c>
       <c r="R18" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 4:18PM CST</t>
+          <t>Jul 16 3:17PM CST</t>
         </is>
       </c>
       <c r="S18" s="1" t="n">
@@ -2798,17 +2798,17 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Adrian Caro</t>
+          <t>Hugo López</t>
         </is>
       </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>153</t>
         </is>
       </c>
       <c r="C19" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
+          <t>TOYOTA HILUX</t>
         </is>
       </c>
       <c r="D19" s="7" t="n">
@@ -2816,26 +2816,26 @@
       </c>
       <c r="E19" s="1" t="inlineStr">
         <is>
-          <t>03:35:17</t>
+          <t>02:29:00</t>
         </is>
       </c>
       <c r="F19" s="1" t="n">
-        <v>59.2</v>
+        <v>33.5</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>0</v>
+        <v>6.48</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I19" s="1" t="inlineStr">
         <is>
-          <t>00:01:16</t>
+          <t>00:00:20</t>
         </is>
       </c>
       <c r="J19" s="1" t="inlineStr">
         <is>
-          <t>00:00:28</t>
+          <t>00:00:27</t>
         </is>
       </c>
       <c r="K19" s="1" t="inlineStr">
@@ -2861,11 +2861,11 @@
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <v>67.59999999999999</v>
+        <v>61</v>
       </c>
       <c r="R19" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 3:54PM CST</t>
+          <t>Jul 16 2:03PM CST</t>
         </is>
       </c>
       <c r="S19" s="1" t="n">
@@ -2918,12 +2918,12 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>CARLOS JIMENEZ</t>
+          <t xml:space="preserve">Daniel Iñiguez </t>
         </is>
       </c>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>141</t>
         </is>
       </c>
       <c r="C20" s="1" t="inlineStr">
@@ -2932,35 +2932,35 @@
         </is>
       </c>
       <c r="D20" s="7" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" s="1" t="inlineStr">
         <is>
-          <t>02:59:32</t>
+          <t>03:36:45</t>
         </is>
       </c>
       <c r="F20" s="1" t="n">
-        <v>49.7</v>
+        <v>73.5</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>7.9</v>
+        <v>8.82</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I20" s="1" t="inlineStr">
         <is>
-          <t>00:00:50</t>
+          <t>00:00:54</t>
         </is>
       </c>
       <c r="J20" s="1" t="inlineStr">
         <is>
-          <t>00:00:26</t>
+          <t>00:00:49</t>
         </is>
       </c>
       <c r="K20" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:09</t>
         </is>
       </c>
       <c r="L20" s="1" t="inlineStr">
@@ -2981,11 +2981,11 @@
         <v>0</v>
       </c>
       <c r="Q20" s="1" t="n">
-        <v>56</v>
+        <v>75.01000000000001</v>
       </c>
       <c r="R20" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 8:50AM CST</t>
+          <t>Jul 16 1:00PM CST</t>
         </is>
       </c>
       <c r="S20" s="1" t="n">
@@ -3038,44 +3038,44 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Daniel Rocha</t>
+          <t>JOSE MORALES</t>
         </is>
       </c>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>150</t>
         </is>
       </c>
       <c r="C21" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2020</t>
+          <t>Hino 300 2024</t>
         </is>
       </c>
       <c r="D21" s="7" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E21" s="1" t="inlineStr">
         <is>
-          <t>01:36:30</t>
+          <t>03:24:28</t>
         </is>
       </c>
       <c r="F21" s="1" t="n">
-        <v>22.8</v>
+        <v>57.5</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>4.8</v>
+        <v>5.05</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:01:13</t>
         </is>
       </c>
       <c r="J21" s="1" t="inlineStr">
         <is>
-          <t>00:00:16</t>
+          <t>00:01:56</t>
         </is>
       </c>
       <c r="K21" s="1" t="inlineStr">
@@ -3101,11 +3101,11 @@
         <v>0</v>
       </c>
       <c r="Q21" s="1" t="n">
-        <v>66.01000000000001</v>
+        <v>87.01000000000001</v>
       </c>
       <c r="R21" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 2:30PM CST</t>
+          <t>Jul 16 3:41PM CST</t>
         </is>
       </c>
       <c r="S21" s="1" t="n">
@@ -3158,17 +3158,17 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Mario Ballinas</t>
+          <t>Daniel Rocha</t>
         </is>
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>144</t>
+          <t>136</t>
         </is>
       </c>
       <c r="C22" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX 2020</t>
         </is>
       </c>
       <c r="D22" s="7" t="n">
@@ -3176,26 +3176,26 @@
       </c>
       <c r="E22" s="1" t="inlineStr">
         <is>
-          <t>02:27:45</t>
+          <t>01:59:46</t>
         </is>
       </c>
       <c r="F22" s="1" t="n">
-        <v>38.3</v>
+        <v>41.2</v>
       </c>
       <c r="G22" s="1" t="n">
-        <v>6.64</v>
+        <v>6.66</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="inlineStr">
         <is>
-          <t>00:00:27</t>
+          <t>00:00:39</t>
         </is>
       </c>
       <c r="J22" s="1" t="inlineStr">
         <is>
-          <t>00:00:11</t>
+          <t>00:00:21</t>
         </is>
       </c>
       <c r="K22" s="1" t="inlineStr">
@@ -3221,11 +3221,11 @@
         <v>0</v>
       </c>
       <c r="Q22" s="1" t="n">
-        <v>70.01000000000001</v>
+        <v>71.01000000000001</v>
       </c>
       <c r="R22" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 2:47PM CST</t>
+          <t>Jul 16 10:49AM CST</t>
         </is>
       </c>
       <c r="S22" s="1" t="n">
@@ -3278,17 +3278,17 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Fernando Ornelas</t>
+          <t>Mario Ballinas</t>
         </is>
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>138</t>
+          <t>144</t>
         </is>
       </c>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2020</t>
+          <t>TOYOTA HILUX 2021</t>
         </is>
       </c>
       <c r="D23" s="7" t="n">
@@ -3296,31 +3296,31 @@
       </c>
       <c r="E23" s="1" t="inlineStr">
         <is>
-          <t>02:04:21</t>
+          <t>02:27:16</t>
         </is>
       </c>
       <c r="F23" s="1" t="n">
-        <v>27.6</v>
+        <v>37.8</v>
       </c>
       <c r="G23" s="1" t="n">
-        <v>5.64</v>
+        <v>6.8</v>
       </c>
       <c r="H23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I23" s="1" t="inlineStr">
         <is>
-          <t>00:00:32</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="J23" s="1" t="inlineStr">
         <is>
-          <t>00:00:33</t>
+          <t>00:00:10</t>
         </is>
       </c>
       <c r="K23" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="L23" s="1" t="inlineStr">
@@ -3341,11 +3341,11 @@
         <v>0</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <v>64</v>
+        <v>68.01000000000001</v>
       </c>
       <c r="R23" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 2:47PM CST</t>
+          <t>Jul 16 11:24AM CST</t>
         </is>
       </c>
       <c r="S23" s="1" t="n">
@@ -3398,17 +3398,17 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Jorge Tornero</t>
+          <t>LEONARDO GONZALEZ</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>132</t>
         </is>
       </c>
       <c r="C24" s="1" t="inlineStr">
         <is>
-          <t>HINO 300</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D24" s="7" t="n">
@@ -3416,31 +3416,31 @@
       </c>
       <c r="E24" s="1" t="inlineStr">
         <is>
-          <t>04:16:15</t>
+          <t>05:28:26</t>
         </is>
       </c>
       <c r="F24" s="1" t="n">
-        <v>86.09999999999999</v>
+        <v>116.3</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>8.15</v>
+        <v>18.76</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I24" s="1" t="inlineStr">
         <is>
-          <t>00:04:24</t>
+          <t>00:01:38</t>
         </is>
       </c>
       <c r="J24" s="1" t="inlineStr">
         <is>
-          <t>00:01:35</t>
+          <t>00:01:32</t>
         </is>
       </c>
       <c r="K24" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:21</t>
         </is>
       </c>
       <c r="L24" s="1" t="inlineStr">
@@ -3449,7 +3449,7 @@
         </is>
       </c>
       <c r="M24" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24" s="1" t="n">
         <v>0</v>
@@ -3461,11 +3461,11 @@
         <v>0</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <v>71.01000000000001</v>
+        <v>83.01000000000001</v>
       </c>
       <c r="R24" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 2:47PM CST</t>
+          <t>Jul 16 4:49PM CST</t>
         </is>
       </c>
       <c r="S24" s="1" t="n">
@@ -3518,12 +3518,12 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>LEONARDO GONZALEZ</t>
+          <t>Daniel Mercado</t>
         </is>
       </c>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>130</t>
         </is>
       </c>
       <c r="C25" s="1" t="inlineStr">
@@ -3532,35 +3532,35 @@
         </is>
       </c>
       <c r="D25" s="7" t="n">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E25" s="1" t="inlineStr">
         <is>
-          <t>01:45:58</t>
+          <t>05:10:42</t>
         </is>
       </c>
       <c r="F25" s="1" t="n">
-        <v>37.8</v>
+        <v>147.5</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>6.67</v>
+        <v>18.82</v>
       </c>
       <c r="H25" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I25" s="1" t="inlineStr">
         <is>
-          <t>00:00:54</t>
+          <t>00:05:24</t>
         </is>
       </c>
       <c r="J25" s="1" t="inlineStr">
         <is>
-          <t>00:00:34</t>
+          <t>00:02:36</t>
         </is>
       </c>
       <c r="K25" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:21</t>
         </is>
       </c>
       <c r="L25" s="1" t="inlineStr">
@@ -3581,11 +3581,11 @@
         <v>0</v>
       </c>
       <c r="Q25" s="1" t="n">
-        <v>64</v>
+        <v>92.01000000000001</v>
       </c>
       <c r="R25" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 10:14AM CST</t>
+          <t>Jul 16 11:51AM CST</t>
         </is>
       </c>
       <c r="S25" s="1" t="n">
@@ -3638,49 +3638,49 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>ANTONIO GODOY</t>
+          <t>FELIPE</t>
         </is>
       </c>
       <c r="B26" s="1" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>126</t>
         </is>
       </c>
       <c r="C26" s="1" t="inlineStr">
         <is>
-          <t>VAN HYUNDAI</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D26" s="7" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E26" s="1" t="inlineStr">
         <is>
-          <t>02:10:20</t>
+          <t>02:40:11</t>
         </is>
       </c>
       <c r="F26" s="1" t="n">
-        <v>40.3</v>
+        <v>44.3</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I26" s="1" t="inlineStr">
         <is>
-          <t>00:02:03</t>
+          <t>00:01:27</t>
         </is>
       </c>
       <c r="J26" s="1" t="inlineStr">
         <is>
-          <t>00:01:08</t>
+          <t>00:01:56</t>
         </is>
       </c>
       <c r="K26" s="1" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:15</t>
         </is>
       </c>
       <c r="L26" s="1" t="inlineStr">
@@ -3692,7 +3692,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O26" s="1" t="n">
         <v>0</v>
@@ -3701,11 +3701,11 @@
         <v>0</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <v>81.8</v>
+        <v>70.01000000000001</v>
       </c>
       <c r="R26" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 3:08PM CST</t>
+          <t>Jul 16 11:05AM CST</t>
         </is>
       </c>
       <c r="S26" s="1" t="n">
@@ -3758,54 +3758,54 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Daniel Mercado</t>
+          <t>Jorge Tornero</t>
         </is>
       </c>
       <c r="B27" s="1" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>117</t>
         </is>
       </c>
       <c r="C27" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>HINO 300</t>
         </is>
       </c>
       <c r="D27" s="7" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E27" s="1" t="inlineStr">
         <is>
-          <t>03:04:30</t>
+          <t>05:15:29</t>
         </is>
       </c>
       <c r="F27" s="1" t="n">
-        <v>64</v>
+        <v>97.3</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>9.51</v>
+        <v>10.88</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I27" s="1" t="inlineStr">
         <is>
-          <t>00:00:56</t>
+          <t>00:04:16</t>
         </is>
       </c>
       <c r="J27" s="1" t="inlineStr">
         <is>
-          <t>00:00:53</t>
+          <t>00:01:12</t>
         </is>
       </c>
       <c r="K27" s="1" t="inlineStr">
         <is>
-          <t>00:00:21</t>
+          <t>00:00:15</t>
         </is>
       </c>
       <c r="L27" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="M27" s="1" t="n">
@@ -3821,11 +3821,11 @@
         <v>0</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <v>83.01000000000001</v>
+        <v>75.01000000000001</v>
       </c>
       <c r="R27" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 12:52PM CST</t>
+          <t>Jul 16 10:45AM CST</t>
         </is>
       </c>
       <c r="S27" s="1" t="n">
@@ -3878,39 +3878,39 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>David Serrano</t>
+          <t>Moises Martinez</t>
         </is>
       </c>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>149</t>
         </is>
       </c>
       <c r="C28" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>TOYOTA HILUX 2024</t>
         </is>
       </c>
       <c r="D28" s="7" t="n">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E28" s="1" t="inlineStr">
         <is>
-          <t>02:36:19</t>
+          <t>02:42:12</t>
         </is>
       </c>
       <c r="F28" s="1" t="n">
-        <v>39.5</v>
+        <v>52.4</v>
       </c>
       <c r="G28" s="1" t="n">
-        <v>4.19</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H28" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I28" s="1" t="inlineStr">
         <is>
-          <t>00:00:56</t>
+          <t>00:00:33</t>
         </is>
       </c>
       <c r="J28" s="1" t="inlineStr">
@@ -3920,7 +3920,7 @@
       </c>
       <c r="K28" s="1" t="inlineStr">
         <is>
-          <t>00:00:18</t>
+          <t>00:00:44</t>
         </is>
       </c>
       <c r="L28" s="1" t="inlineStr">
@@ -3941,11 +3941,11 @@
         <v>0</v>
       </c>
       <c r="Q28" s="1" t="n">
-        <v>80.01000000000001</v>
+        <v>88.01000000000001</v>
       </c>
       <c r="R28" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 10:30AM CST</t>
+          <t>Jul 16 1:54PM CST</t>
         </is>
       </c>
       <c r="S28" s="1" t="n">
@@ -3998,44 +3998,44 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Moises Martinez</t>
+          <t>MIGUEL GUIZAR</t>
         </is>
       </c>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>154</t>
         </is>
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2024</t>
-        </is>
-      </c>
-      <c r="D29" s="7" t="n">
-        <v>94</v>
+          <t>VW DELIVERY 10.6</t>
+        </is>
+      </c>
+      <c r="D29" s="8" t="n">
+        <v>87</v>
       </c>
       <c r="E29" s="1" t="inlineStr">
         <is>
-          <t>02:24:44</t>
+          <t>09:07:12</t>
         </is>
       </c>
       <c r="F29" s="1" t="n">
-        <v>44.8</v>
+        <v>397.5</v>
       </c>
       <c r="G29" s="1" t="n">
-        <v>8.82</v>
+        <v>0</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I29" s="1" t="inlineStr">
         <is>
-          <t>00:01:31</t>
+          <t>00:04:27</t>
         </is>
       </c>
       <c r="J29" s="1" t="inlineStr">
         <is>
-          <t>00:00:50</t>
+          <t>00:04:43</t>
         </is>
       </c>
       <c r="K29" s="1" t="inlineStr">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="L29" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:33</t>
         </is>
       </c>
       <c r="M29" s="1" t="n">
@@ -4061,11 +4061,11 @@
         <v>0</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <v>87.01000000000001</v>
+        <v>104</v>
       </c>
       <c r="R29" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 3:39PM CST</t>
+          <t>Jul 16 8:02AM CST</t>
         </is>
       </c>
       <c r="S29" s="1" t="n">
@@ -4118,54 +4118,54 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">CRISTIAN ESTRADA </t>
+          <t xml:space="preserve">Compras </t>
         </is>
       </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>120</t>
         </is>
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">TOYOTA HILUX </t>
-        </is>
-      </c>
-      <c r="D30" s="7" t="n">
-        <v>93</v>
+          <t>FORD RANGER 2011</t>
+        </is>
+      </c>
+      <c r="D30" s="8" t="n">
+        <v>87</v>
       </c>
       <c r="E30" s="1" t="inlineStr">
         <is>
-          <t>03:06:31</t>
+          <t>04:32:52</t>
         </is>
       </c>
       <c r="F30" s="1" t="n">
-        <v>53</v>
+        <v>102.5</v>
       </c>
       <c r="G30" s="1" t="n">
-        <v>9.15</v>
+        <v>17.54</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I30" s="1" t="inlineStr">
         <is>
-          <t>00:00:56</t>
+          <t>00:01:30</t>
         </is>
       </c>
       <c r="J30" s="1" t="inlineStr">
         <is>
-          <t>00:00:51</t>
+          <t>00:01:26</t>
         </is>
       </c>
       <c r="K30" s="1" t="inlineStr">
         <is>
-          <t>00:00:39</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="L30" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:16</t>
         </is>
       </c>
       <c r="M30" s="1" t="n">
@@ -4181,11 +4181,11 @@
         <v>0</v>
       </c>
       <c r="Q30" s="1" t="n">
-        <v>74.01000000000001</v>
+        <v>93.01000000000001</v>
       </c>
       <c r="R30" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 3:52PM CST</t>
+          <t>Jul 16 2:55PM CST</t>
         </is>
       </c>
       <c r="S30" s="1" t="n">
@@ -4238,61 +4238,61 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Alberto Sesmas</t>
+          <t>Luis Galindo</t>
         </is>
       </c>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>118</t>
         </is>
       </c>
       <c r="C31" s="1" t="inlineStr">
         <is>
-          <t>KENWORTH</t>
-        </is>
-      </c>
-      <c r="D31" s="7" t="n">
-        <v>92</v>
+          <t>KENWORTH 2009</t>
+        </is>
+      </c>
+      <c r="D31" s="8" t="n">
+        <v>85</v>
       </c>
       <c r="E31" s="1" t="inlineStr">
         <is>
-          <t>08:05:38</t>
+          <t>09:27:07</t>
         </is>
       </c>
       <c r="F31" s="1" t="n">
-        <v>380.7</v>
+        <v>567.4</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>101.7</v>
+        <v>124.24</v>
       </c>
       <c r="H31" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I31" s="1" t="inlineStr">
         <is>
-          <t>00:02:54</t>
+          <t>00:03:59</t>
         </is>
       </c>
       <c r="J31" s="1" t="inlineStr">
         <is>
-          <t>00:01:54</t>
+          <t>00:09:41</t>
         </is>
       </c>
       <c r="K31" s="1" t="inlineStr">
         <is>
-          <t>00:00:52</t>
+          <t>00:01:17</t>
         </is>
       </c>
       <c r="L31" s="1" t="inlineStr">
         <is>
-          <t>00:00:10</t>
+          <t>00:00:28</t>
         </is>
       </c>
       <c r="M31" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O31" s="1" t="n">
         <v>0</v>
@@ -4301,11 +4301,11 @@
         <v>0</v>
       </c>
       <c r="Q31" s="1" t="n">
-        <v>109.01</v>
+        <v>97.01000000000001</v>
       </c>
       <c r="R31" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 2:25AM CST</t>
+          <t>Jul 16 5:57AM CST</t>
         </is>
       </c>
       <c r="S31" s="1" t="n">
@@ -4358,74 +4358,74 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>MIGUEL GUIZAR</t>
+          <t>Armando Muñoz</t>
         </is>
       </c>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>102</t>
         </is>
       </c>
       <c r="C32" s="1" t="inlineStr">
         <is>
-          <t>VW DELIVERY 10.6</t>
+          <t>HINO 300</t>
         </is>
       </c>
       <c r="D32" s="8" t="n">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E32" s="1" t="inlineStr">
         <is>
-          <t>05:30:57</t>
+          <t>09:53:20</t>
         </is>
       </c>
       <c r="F32" s="1" t="n">
-        <v>286.7</v>
+        <v>509.1</v>
       </c>
       <c r="G32" s="1" t="n">
-        <v>0</v>
+        <v>66.12</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I32" s="1" t="inlineStr">
         <is>
-          <t>00:17:17</t>
+          <t>00:10:29</t>
         </is>
       </c>
       <c r="J32" s="1" t="inlineStr">
         <is>
-          <t>00:18:33</t>
+          <t>00:13:30</t>
         </is>
       </c>
       <c r="K32" s="1" t="inlineStr">
         <is>
-          <t>00:01:11</t>
+          <t>00:04:05</t>
         </is>
       </c>
       <c r="L32" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:33</t>
         </is>
       </c>
       <c r="M32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N32" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="O32" s="1" t="n">
-        <v>0</v>
-      </c>
       <c r="P32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q32" s="1" t="n">
-        <v>117.46</v>
+        <v>90.01000000000001</v>
       </c>
       <c r="R32" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 12:14PM CST</t>
+          <t>Jul 16 1:56PM CST</t>
         </is>
       </c>
       <c r="S32" s="1" t="n">
@@ -4478,17 +4478,17 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Francisco Marquez</t>
+          <t>Fernando Ornelas</t>
         </is>
       </c>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>138</t>
         </is>
       </c>
       <c r="C33" s="1" t="inlineStr">
         <is>
-          <t>FREIGHTLINER NUEVA M2 106 52K 6X4</t>
+          <t>TOYOTA HILUX 2020</t>
         </is>
       </c>
       <c r="D33" s="8" t="n">
@@ -4496,43 +4496,43 @@
       </c>
       <c r="E33" s="1" t="inlineStr">
         <is>
-          <t>11:46:54</t>
+          <t>02:14:29</t>
         </is>
       </c>
       <c r="F33" s="1" t="n">
-        <v>660.5</v>
+        <v>47.5</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>182.49</v>
+        <v>7.77</v>
       </c>
       <c r="H33" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I33" s="1" t="inlineStr">
         <is>
-          <t>00:13:52</t>
+          <t>00:00:09</t>
         </is>
       </c>
       <c r="J33" s="1" t="inlineStr">
         <is>
-          <t>00:11:36</t>
+          <t>00:00:29</t>
         </is>
       </c>
       <c r="K33" s="1" t="inlineStr">
         <is>
-          <t>00:04:20</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="L33" s="1" t="inlineStr">
         <is>
-          <t>00:00:57</t>
+          <t>00:00:22</t>
         </is>
       </c>
       <c r="M33" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O33" s="1" t="n">
         <v>0</v>
@@ -4541,11 +4541,11 @@
         <v>0</v>
       </c>
       <c r="Q33" s="1" t="n">
-        <v>100.01</v>
+        <v>85.01000000000001</v>
       </c>
       <c r="R33" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 4:53PM CST</t>
+          <t>Jul 16 1:38PM CST</t>
         </is>
       </c>
       <c r="S33" s="1" t="n">
@@ -4598,54 +4598,54 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Martin Quezada</t>
+          <t>Alberto Sesmas</t>
         </is>
       </c>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>122</t>
+          <t>124</t>
         </is>
       </c>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>INTERNACIONAL</t>
+          <t>KENWORTH</t>
         </is>
       </c>
       <c r="D34" s="9" t="n">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E34" s="1" t="inlineStr">
         <is>
-          <t>00:18:52</t>
+          <t>06:01:02</t>
         </is>
       </c>
       <c r="F34" s="1" t="n">
-        <v>7.1</v>
+        <v>334.3</v>
       </c>
       <c r="G34" s="1" t="n">
-        <v>3.84</v>
+        <v>85.7</v>
       </c>
       <c r="H34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I34" s="1" t="inlineStr">
         <is>
-          <t>00:00:33</t>
+          <t>00:04:57</t>
         </is>
       </c>
       <c r="J34" s="1" t="inlineStr">
         <is>
-          <t>00:00:23</t>
+          <t>00:04:06</t>
         </is>
       </c>
       <c r="K34" s="1" t="inlineStr">
         <is>
-          <t>00:00:26</t>
+          <t>00:01:07</t>
         </is>
       </c>
       <c r="L34" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:55</t>
         </is>
       </c>
       <c r="M34" s="1" t="n">
@@ -4661,11 +4661,11 @@
         <v>0</v>
       </c>
       <c r="Q34" s="1" t="n">
-        <v>66.01000000000001</v>
+        <v>113.01</v>
       </c>
       <c r="R34" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 8:54AM CST</t>
+          <t>Jul 16 2:29PM CST</t>
         </is>
       </c>
       <c r="S34" s="1" t="n">
@@ -4732,60 +4732,60 @@
         </is>
       </c>
       <c r="D35" s="9" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E35" s="1" t="inlineStr">
         <is>
-          <t>07:55:54</t>
+          <t>05:54:53</t>
         </is>
       </c>
       <c r="F35" s="1" t="n">
-        <v>363.6</v>
+        <v>327.8</v>
       </c>
       <c r="G35" s="1" t="n">
-        <v>80.09999999999999</v>
+        <v>73.20999999999999</v>
       </c>
       <c r="H35" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I35" s="1" t="inlineStr">
         <is>
-          <t>00:10:33</t>
+          <t>00:08:09</t>
         </is>
       </c>
       <c r="J35" s="1" t="inlineStr">
         <is>
-          <t>00:07:05</t>
+          <t>00:08:20</t>
         </is>
       </c>
       <c r="K35" s="1" t="inlineStr">
         <is>
-          <t>00:06:39</t>
+          <t>00:06:20</t>
         </is>
       </c>
       <c r="L35" s="1" t="inlineStr">
         <is>
-          <t>00:00:58</t>
+          <t>00:02:17</t>
         </is>
       </c>
       <c r="M35" s="1" t="n">
         <v>0</v>
       </c>
       <c r="N35" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O35" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P35" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q35" s="1" t="n">
-        <v>104.01</v>
+        <v>102.01</v>
       </c>
       <c r="R35" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 2:27AM CST</t>
+          <t>Jul 16 12:11PM CST</t>
         </is>
       </c>
       <c r="S35" s="1" t="n">
@@ -4838,54 +4838,54 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daniel Iñiguez </t>
+          <t>David Serrano</t>
         </is>
       </c>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>125</t>
         </is>
       </c>
       <c r="C36" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2021</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D36" s="9" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E36" s="1" t="inlineStr">
         <is>
-          <t>03:45:53</t>
+          <t>01:25:11</t>
         </is>
       </c>
       <c r="F36" s="1" t="n">
-        <v>70.90000000000001</v>
+        <v>33.4</v>
       </c>
       <c r="G36" s="1" t="n">
-        <v>9.15</v>
+        <v>3.29</v>
       </c>
       <c r="H36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I36" s="1" t="inlineStr">
         <is>
-          <t>00:02:36</t>
+          <t>00:01:49</t>
         </is>
       </c>
       <c r="J36" s="1" t="inlineStr">
         <is>
-          <t>00:01:15</t>
+          <t>00:02:00</t>
         </is>
       </c>
       <c r="K36" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:39</t>
         </is>
       </c>
       <c r="L36" s="1" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:09</t>
         </is>
       </c>
       <c r="M36" s="1" t="n">
@@ -4901,24 +4901,24 @@
         <v>0</v>
       </c>
       <c r="Q36" s="1" t="n">
-        <v>77.01000000000001</v>
+        <v>92.01000000000001</v>
       </c>
       <c r="R36" s="1" t="inlineStr">
         <is>
-          <t>Jul 15 10:29AM CST</t>
+          <t>Jul 16 12:33PM CST</t>
         </is>
       </c>
       <c r="S36" s="1" t="n">
         <v>0</v>
       </c>
       <c r="T36" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U36" s="1" t="n">
         <v>0</v>
       </c>
       <c r="V36" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W36" s="1" t="n">
         <v>0</v>
@@ -4958,137 +4958,179 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>FELIPE</t>
+          <t>Martin Quezada</t>
         </is>
       </c>
       <c r="B37" s="1" t="inlineStr">
         <is>
-          <t>126</t>
+          <t>122</t>
         </is>
       </c>
       <c r="C37" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
-        </is>
-      </c>
-      <c r="D37" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" s="1" t="inlineStr">
-        <is>
-          <t>03:08:15</t>
-        </is>
-      </c>
-      <c r="F37" s="1" t="n">
-        <v>60.4</v>
-      </c>
-      <c r="G37" s="1" t="n">
-        <v>5.93</v>
-      </c>
-      <c r="H37" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="I37" s="1" t="inlineStr">
-        <is>
-          <t>00:01:15</t>
-        </is>
-      </c>
-      <c r="J37" s="1" t="inlineStr">
-        <is>
-          <t>00:00:36</t>
-        </is>
-      </c>
-      <c r="K37" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="L37" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="M37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="P37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="1" t="n">
-        <v>76.01000000000001</v>
-      </c>
-      <c r="R37" s="1" t="inlineStr">
-        <is>
-          <t>Jul 15 12:32PM CST</t>
-        </is>
-      </c>
-      <c r="S37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="T37" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="U37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="V37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="W37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="X37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y37" s="1" t="inlineStr">
-        <is>
-          <t>Sin ruta.</t>
-        </is>
-      </c>
-      <c r="Z37" s="1" t="inlineStr">
-        <is>
-          <t>00:00:00</t>
-        </is>
-      </c>
-      <c r="AA37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE37" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF37" s="1" t="n">
-        <v>0</v>
+          <t>INTERNACIONAL</t>
+        </is>
+      </c>
+      <c r="D37" s="10" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="E37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="F37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="G37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="H37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="I37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="J37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="K37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="L37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="M37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="N37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="O37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="P37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Q37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="R37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="S37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="T37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="U37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="V37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="W37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="X37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Y37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="Z37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AA37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AB37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AC37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AD37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AE37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
+      </c>
+      <c r="AF37" s="11" t="inlineStr">
+        <is>
+          <t>Sin ruta</t>
+        </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Alejandro Lara</t>
+          <t>Jonathan Alvarez</t>
         </is>
       </c>
       <c r="B38" s="1" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>131</t>
         </is>
       </c>
       <c r="C38" s="1" t="inlineStr">
         <is>
-          <t>WORKEN</t>
+          <t>TOYOTA HILUX 2017</t>
         </is>
       </c>
       <c r="D38" s="10" t="inlineStr">
@@ -5240,17 +5282,17 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Compras </t>
+          <t>Angel Cortez</t>
         </is>
       </c>
       <c r="B39" s="1" t="inlineStr">
         <is>
-          <t>120</t>
+          <t>133</t>
         </is>
       </c>
       <c r="C39" s="1" t="inlineStr">
         <is>
-          <t>FORD RANGER 2011</t>
+          <t>TOYOTA HILUX 2018</t>
         </is>
       </c>
       <c r="D39" s="10" t="inlineStr">
@@ -5402,17 +5444,17 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Jonathan Alvarez</t>
+          <t>Alejandro Suarez</t>
         </is>
       </c>
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>146</t>
         </is>
       </c>
       <c r="C40" s="1" t="inlineStr">
         <is>
-          <t>TOYOTA HILUX 2017</t>
+          <t>HINO 500</t>
         </is>
       </c>
       <c r="D40" s="10" t="inlineStr">

</xml_diff>